<commit_message>
add more tweets and remove retweets of new tweets
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="1636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2820" uniqueCount="2012">
   <si>
     <t>instance_id</t>
   </si>
@@ -4938,19 +4938,1147 @@
     <t>"RT @MaheshNegombo: @Erandeeplus ඔන්න 600 වෙනි ෆලෝවර් 😃😃"</t>
   </si>
   <si>
-    <t>947</t>
-  </si>
-  <si>
-    <t>1037463307714617345</t>
-  </si>
-  <si>
-    <t>Wed Sep 05 22:11:42 +0000 2018</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>1075942865950425088</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 02:35:43 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Dilan_Perera45 කොපි කරලා සර්ච් කරලා බලන්න ඔයාට සැක නම් ඕකෙ ඔරිජිනල් කාගෙද කියලා හුම්😒"</t>
+  </si>
+  <si>
+    <t>1075937583576829957</t>
+  </si>
+  <si>
+    <t>2713529238</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 02:14:44 +0000 2018</t>
+  </si>
+  <si>
+    <t>"එඩේරා පසුපස ගව රැල එන්නා සේ අපි පසු පස අපේ ගව රැල එනවලු...අයියො ....🤣🤣🤣 https://t.co/DD39YRdrWR"</t>
+  </si>
+  <si>
+    <t>1075933584626569216</t>
+  </si>
+  <si>
+    <t>324432673</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 01:58:51 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@milindarj රංගේ ඉන්නවා... කොහොමත් මෙෙත්‍රීගේ සෙල්ලම් තව උපරිම උනොත් දවස් 352යි... 😂"</t>
+  </si>
+  <si>
+    <t>1075921815174832128</t>
+  </si>
+  <si>
+    <t>147184014</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 01:12:05 +0000 2018</t>
+  </si>
+  <si>
+    <t>"බේරු­වල හොරො­යින් තොගයේ සැක­ක­රුවෝ රිමාන්ඩ් https://t.co/Yan4JyZIGG"</t>
+  </si>
+  <si>
+    <t>1075917438301003776</t>
+  </si>
+  <si>
+    <t>980446497685852160</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 00:54:41 +0000 2018</t>
+  </si>
+  <si>
+    <t>"තිලා උඹ එදා මේ කෙල්ලට මතුරපු නාරං කැවුමක් කැව්ව නේද? ඇත්ත කියාපන්.. මට සැක හිතුන ළඟටම වෙලා ඉඳගෙන හිටපු විදිහට 🤨🤨 https://t.co/cdlhoDv11C"</t>
+  </si>
+  <si>
+    <t>1075891717428178944</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 23:12:29 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@RakzzMaduOnline @Chamalka_N @Soulchild_Rishi ෆේක් එකක් කියලා හිතලා බ්ලොක් කරනවා තව ටිකෙන්😂"</t>
+  </si>
+  <si>
+    <t>1075843006811365376</t>
+  </si>
+  <si>
+    <t>1060024229167489024</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 19:58:55 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@ChanakaDinushan @SajithP අනේ පල හුත්තො තොපේ මහ එකාගෙ දවසක වියඳම කීයද ඒ දවස් වල"</t>
+  </si>
+  <si>
+    <t>1075802379847557120</t>
+  </si>
+  <si>
+    <t>905674137133133824</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 17:17:29 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@DJSlash9 @moogater @RathuMakaraFM_ එන්න එන්න දැන් පරක්කු නෑ... මුළ ටික හෙට https://t.co/p7vdVphhDN එකෙන් අහමු ඊට පස්සේ ආයම 🙊"</t>
+  </si>
+  <si>
+    <t>1075795210624557057</t>
+  </si>
+  <si>
+    <t>343755137</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 16:49:00 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@maalupaan හා මම ලංකාවට ආපු දවසක ඔයාගේ මාළූ පාන් හදලා දෙන්න"</t>
+  </si>
+  <si>
+    <t>1075793783051042816</t>
+  </si>
+  <si>
+    <t>3238982816</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 16:43:19 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@nwty_ck @dudeum_Nethu අපිටත් එහෙම කරයිද දන් නෑ දවසක 😥😥😥"</t>
+  </si>
+  <si>
+    <t>1075784895820050432</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 16:08:00 +0000 2018</t>
+  </si>
+  <si>
+    <t>"හිතලා ට්වීට් දානවට වඩා ඩුබ් ගහන එක නම් 😍✋🤝"</t>
+  </si>
+  <si>
+    <t>1075776273211768833</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 15:33:45 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@MatiBole බෑනෙ මැටිබෝලෙ කරන්න...ගමේ කෙල්ලො ගැන හිතලා නොයා ඉන්නවා 😂✌🏽  අර නාඩගමේ රජාට ඇන්ද සීන් එක වෙන්නෙ නැත්තන් 🤭"</t>
+  </si>
+  <si>
+    <t>1075759595908300800</t>
+  </si>
+  <si>
+    <t>973814985234272256</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 14:27:28 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Madurangakalpa1 ගහමු..පතා එකේ... දවසක..😁"</t>
+  </si>
+  <si>
+    <t>1075750684065116160</t>
+  </si>
+  <si>
+    <t>1302348002</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:52:04 +0000 2018</t>
+  </si>
+  <si>
+    <t>"නංගි තරහ වෙලා කියහල්ලකො... ඕක කෙල්ලට ආරංචි උනොත් කෙලින්ම නෑන පොඩ්ඩගෙ පැත්ත අරන් මාව බලයෙන් පහ කරනව කියහල්ලකො....😌"</t>
+  </si>
+  <si>
+    <t>1075748464477249537</t>
+  </si>
+  <si>
+    <t>2315810478</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:43:15 +0000 2018</t>
+  </si>
+  <si>
+    <t>"එක දවසක අපි නුපුරුදු සුවඳක හිත හෙමිහිට බැඳුනා අප හමුවුණු හිනැහුණු මතකය  සසර පුරුදු හැඟුණා  🖤🖤🖤 — feeling loved"</t>
+  </si>
+  <si>
+    <t>1075744897368449024</t>
+  </si>
+  <si>
+    <t>1319729186</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:29:04 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@nsadisha 😂😂😂😂 ආපු දවසක පෙනන"</t>
+  </si>
+  <si>
+    <t>1075743213376364546</t>
+  </si>
+  <si>
+    <t>1075417369273458690</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:22:23 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@techn0ish 😂😂😂 මේකට මොනාට් උනොත් මං ආයෙ ටුයිටර් නෑහ් 😂🤘"</t>
+  </si>
+  <si>
+    <t>1075743194183135232</t>
+  </si>
+  <si>
+    <t>199129412</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:22:18 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@MatiBole උදම්මිට පාරෙන් එන දවසක අනිවා එනවා ඔන්න"</t>
+  </si>
+  <si>
+    <t>1075737752006647808</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 13:00:40 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@PeirisDarshana මම හොයලා හිතලා නෑ. ඇහෙන යමක් විතරයි."</t>
+  </si>
+  <si>
+    <t>1075692140599148547</t>
+  </si>
+  <si>
+    <t>1685742714</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 09:59:26 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@MatiBole ම්ම්ම්ම් බැරිවෙලාවත් සැන්ටා උනොත් මුලින්ම හොයලා දෙන්නේ ඔයාට එහෙනම්.. ☺️"</t>
+  </si>
+  <si>
+    <t>1075670371821645824</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 08:32:56 +0000 2018</t>
+  </si>
+  <si>
+    <t>"විද්‍යාත්මක ව හිතලා කාන්තා කටයුතු හා වියලි කලාප සංවර්ධන අමාත්‍යාංශය හැදුවා. දැන් කාන්තාවන් ගේ වියලි කලාප සංවර්ධනය වෙයි මේම මේම."</t>
+  </si>
+  <si>
+    <t>1075666053907312640</t>
+  </si>
+  <si>
+    <t>345649350</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 08:15:46 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@PoDiyaa වටයක් දෙකක් දාලා බැරිම උනොත් හිස් අතින් ෆිටෝන් එකට ගිහින් ආයේ වරෙන් 😂"</t>
+  </si>
+  <si>
+    <t>972847580517298176</t>
+  </si>
+  <si>
+    <t>1075653126542114816</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 07:24:24 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අනේ නිකන් ඉන්නව සංජු අක්කෙ 😂 ඔයාහෙ 6යිද ලිස්ට් එක 🙊🙊 ආයෙ හදන් නෑමයි මේකට මොනාහරි උනොත් 😂 https://t.co/7eoD8BRUYz"</t>
+  </si>
+  <si>
+    <t>1075650598580543489</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 07:14:21 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@AchiniHansima එහෙම උනොත් නම් ලොකු දෙයක් 😭♥️"</t>
+  </si>
+  <si>
+    <t>1075631388001353728</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 05:58:01 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@chathuranga513 ඔව් ඉතින් දෙකක් හදලත් මෙහෙම උනානෙ. මේකටත් එහෙම උනොත් ආයෙ හද න්නද ? බෑනෙ"</t>
+  </si>
+  <si>
+    <t>1075620470269956096</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 05:14:38 +0000 2018</t>
+  </si>
+  <si>
+    <t>"සමහරු කතා කරන්නේ නිකන් ජනාධිපතිපති හිතලා කට්ටියව පත් කරනවා වගේනේ. 😂😂😂  පව් අර අහිංසකයා. 😁😂"</t>
+  </si>
+  <si>
+    <t>1075614985584205824</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:52:51 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ හා බායි එහෙනම් 😂 මොනාහරි උනොත් බායි කියන්න වෙන්නෙත් නෑනෙ 😂😂😂😂"</t>
+  </si>
+  <si>
+    <t>1075612975178772480</t>
+  </si>
+  <si>
+    <t>730199737333207041</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:44:51 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@wishawanath හහා 😂😂😂 එහෙමවත් සෙට් උනොත් තමා අපිට"</t>
+  </si>
+  <si>
+    <t>1075612716176293888</t>
+  </si>
+  <si>
+    <t>880606053754208256</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:43:50 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක - https://t.co/8bZoOfHdHU"</t>
+  </si>
+  <si>
+    <t>1075612714746007552</t>
+  </si>
+  <si>
+    <t>2921561887</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:43:49 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක - https://t.co/RkGbK2kU8K"</t>
+  </si>
+  <si>
+    <t>1075608706002280448</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:27:54 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ නෑ නෑ නෑ 😂😂😂 පරණ එක හදාගත්තොත් ඉන්නව. මේකටත් ඒකම උනොත් එන්නෙ නෑ නෑ නෑ නෑ නෑ"</t>
+  </si>
+  <si>
+    <t>1075607615688761345</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:23:34 +0000 2018</t>
+  </si>
+  <si>
+    <t>"මම මේක නැති උනොත් ආයෙ ටුයිටර් එන්නෙ නෑ 😂 https://t.co/yx0XHIdIGl"</t>
+  </si>
+  <si>
+    <t>1075607167225409538</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:21:47 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Nadeez__ හා එහෙනම් 😏 ආයෙ ඉතින් මේකත් නැති උනොත් නම් හදන්නෙ නෑමයි එකක් 😂 පරණ එක හරි ගියොත් නම් 😍😍😍😍😍😍😍😍😍😍"</t>
+  </si>
+  <si>
+    <t>1075603323397361664</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:06:30 +0000 2018</t>
+  </si>
+  <si>
+    <t>"මේකටත් මොනාහරි උනොත් ආයෙ ටුයිටර් එන්නෙ නෑ 😂👋"</t>
+  </si>
+  <si>
+    <t>1075603008963043328</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 04:05:15 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Sansajran @dead_mans_creed 😂😂😂 මාත් දැම්මා එහෙම හිතලා"</t>
+  </si>
+  <si>
+    <t>1075588326277685254</t>
+  </si>
+  <si>
+    <t>2399526168</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 03:06:55 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක https://t.co/pYURblAJDo https://t.co/pYURblAJDo"</t>
+  </si>
+  <si>
+    <t>1075588291469238272</t>
+  </si>
+  <si>
+    <t>288156548</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 03:06:46 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අර්ජුන් ඇලෝසියස් හදිසියේ අසනීප වෙයි - ඩෙංගුදැයි සැක https://t.co/LTcyrbML7T https://t.co/LTcyrbML7T"</t>
+  </si>
+  <si>
+    <t>1075586235991773189</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 02:58:36 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Lovely_Paba @tharu__ @akhilasg @Nadeez__ පබා අපි ආයෙම දවසක කතා කරමු."</t>
+  </si>
+  <si>
+    <t>1075561569692602368</t>
+  </si>
+  <si>
+    <t>965533805179174912</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 01:20:35 +0000 2018</t>
+  </si>
+  <si>
+    <t>"සත්තයි දවසක ඔබ හඩනවා මම හඩන තරමටම...."</t>
+  </si>
+  <si>
+    <t>1075470854379704320</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 19:20:07 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අපි ආයේ ඒ ගැන දවසක කතා කරමු. https://t.co/Fe45fEqV12"</t>
+  </si>
+  <si>
+    <t>1075440629037989888</t>
+  </si>
+  <si>
+    <t>432130044</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 17:20:01 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando @tikirimaarie වැඩිම උනොත් ඇවිත් "haha" emoji එකක් දාල යාවි 😂😂"</t>
+  </si>
+  <si>
+    <t>1075435199666614273</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 16:58:26 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@sheshandj ඔයා තමා වගකියන්න ඕනෙ ඔහොම කියල මට මොනාහරි උනොත් 😏😭"</t>
+  </si>
+  <si>
+    <t>1075429878860734465</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 16:37:18 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Rasthiyaduwa ✋😂 දවසක හාද"</t>
+  </si>
+  <si>
+    <t>1075419885986029568</t>
+  </si>
+  <si>
+    <t>1056620438477045763</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 15:57:35 +0000 2018</t>
+  </si>
+  <si>
+    <t>"නුඹ නැතුව හිත හැදෙන් නෑ ළඟට ඇවිදින් අඬන් නෑ ලැබෙන දවසක ලැබෙනවා නම් සිතින් කිසිදින හැලෙන් නෑ.. #සිතුවිලි"</t>
+  </si>
+  <si>
+    <t>1075418248890511362</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 15:51:05 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@MatiBole එන්නේම නැති උනොත්."</t>
+  </si>
+  <si>
+    <t>1075417589327659008</t>
+  </si>
+  <si>
+    <t>192037491</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 15:48:28 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@AyeshaShehani බොහෝම ස්තූතියි අයේසෝ! ඉක්මනට දවසක හම්බෙමු? තිසූගෙන් කේක් ගන්නත් තියේ."</t>
+  </si>
+  <si>
+    <t>1075409043022180354</t>
+  </si>
+  <si>
+    <t>2993019091</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 15:14:30 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@DraXTwitt උඹ දැන් වැඩ කරන තනේ නැති උනොත් එහා තනට පැනපං. ගොඩං වෙලාවට ඔව්වා එක වගේ 😂😂🤣"</t>
+  </si>
+  <si>
+    <t>1075403386067927040</t>
+  </si>
+  <si>
+    <t>995273332843950080</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:52:01 +0000 2018</t>
+  </si>
+  <si>
+    <t>"🍃.......... අපි ආයෙත් හමු නොවුනා නම් ඉස්සර දවසක මියගිය සෙනෙහස  යලි ඉපදී මා හද හඬවන්නට අපි ආයෙත් හමු නොවුනා නම්...🍂  #සදාකාලිකනොවූලෝකේ"</t>
+  </si>
+  <si>
+    <t>1075403200348463104</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:51:17 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando @piumi_silva ආයේ ඒවා ගැන හිතලා හිත මෙව්වා කර ගන්න එපා."</t>
+  </si>
+  <si>
+    <t>1075398782509084673</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:33:44 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@_Thamarasa_ එල එල.. නැත්තන් අපෙ අම්මලගෙ ගමේ එන දවසක මම එනවා ඔහේ..😂😂😂"</t>
+  </si>
+  <si>
+    <t>178606641</t>
+  </si>
+  <si>
+    <t>1075390738396012545</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:01:46 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Annnuza අාහ් එහෙමද.. එල.. පස්සෙ දවසක සෙට් වෙමු එහෙනම්..."</t>
+  </si>
+  <si>
+    <t>1075362193548337152</t>
+  </si>
+  <si>
+    <t>885726737073451009</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 12:08:20 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@_ouTliER__ අගමැති උනොත් මට රස්සාවක් දෙන්න අක්කේ"</t>
+  </si>
+  <si>
+    <t>1075357957892833281</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 11:51:31 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@maalupaan බැරිම උනොත් වරෙන් මෙහෙ. ගහල කීයක් හරි හොයන් ජීවත් වෙමු. මම කීවේ ෆොටෝ ගහල."</t>
+  </si>
+  <si>
+    <t>1075335857983315968</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 10:23:41 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@FriendsGammadda ඒ makeup කරන දේවල් නෙමෙ.අනික මං makeup කරන්න දන්නේ නෑ 😂 වැඩිම උනොත් lipstick සහ eye liner පාවිච්චි කරයි 😂"</t>
+  </si>
+  <si>
+    <t>1075333797292326913</t>
+  </si>
+  <si>
+    <t>965080511205949440</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 10:15:30 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Jude_H_Fernando හම්මේ ඉතින් 😂👊... මේ මාසෙ ෆුල් බිසී නසියරේ.. හම්බවෙමුකො දවසක 🖤"</t>
+  </si>
+  <si>
+    <t>212847371</t>
+  </si>
+  <si>
+    <t>1075926385410146305</t>
+  </si>
+  <si>
+    <t>2496331741</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 01:30:14 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ඉරාකය, ඇෆ්ගනිස්ථානය, පකිස්ථානය, සිරියාව, ලිබියාව සහ තවත් රටවල් වල ලමයි ජනතාව මරනව live බලව් හිටපු ඔබාමා නියම පාලකයෙක්ලු..  Check out @childrenshealth’s Tweet: https://t.co/OfiBKLXBGT"</t>
+  </si>
+  <si>
+    <t>1075915567251353600</t>
+  </si>
+  <si>
+    <t>1854407280</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 00:47:15 +0000 2018</t>
+  </si>
+  <si>
+    <t>"සිංගප්පූරුව දියුණු කරපු මිනිහා වැඩ පටං ගත්තේ මෙන්න මෙහෙමයි.. ඒයා ලඟ තිබුනේ කාරණා තුනයි.. උවමනාව, කැපවීම සහ හැකියාව..   රටවල් දියුණු කරන්න දේශපාලන experience අනිවාර්ය නෑ.. #lka #GR2020 https://t.co/v9U3oyNbPs"</t>
+  </si>
+  <si>
+    <t>1075814109046726656</t>
+  </si>
+  <si>
+    <t>1011390594</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 18:04:05 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ඉරාකය, ඇෆ්ගනිස්ථානය, පකිස්ථානය, සිරියාව, ලිබියාව සහ තවත් රටවල් වල ලමයි ජනතාව මරනව live බලව් හිටපු ඔබාමා නියම පාලකයෙක්ලු..  ළමයි මැරුවට මොකද නත්තලට ළමයින්ට බඩු බෙදුවනේ...🎅🎅🎅 මේව රඟපෑම් එහෙම නෙමෙයි හොඳෙ.. https://t.co/0CEV50nwAm"</t>
+  </si>
+  <si>
+    <t>1075730060022210562</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 12:30:07 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@notNaughtyE දන්නේ නෑ මෙයා. සුද්දා ගල විද්ද නිසා තමයි අපි යාන්තම් කොළඹ හරි යන්නේ. නුවර අපිට එහෙම මහලොකු දැනුමක් නැහැ. ඒකයි ඇත්ත. අනිත් රටවල් වලත් එහෙමද කියන්න එහේ යන්න තියා ඉන්ටර්නෙට් එකේ සර්ච් කරලා ඒ දේවල් බලන්නවත් අපිට ඉංග්‍රීසි දන්නේ නෑ 😢"</t>
+  </si>
+  <si>
+    <t>1075701507163635714</t>
+  </si>
+  <si>
+    <t>156612704</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 10:36:39 +0000 2018</t>
+  </si>
+  <si>
+    <t>"&amp;lt;3 මගේ ආදරේ තවමත් ඒ වගේ සොදුරු කතාවක් වගේ නුබේ හීනයේ දැවටී එදා වගේ ඉන්න ආසයි තවමත් හිතේ  දවසක නුබ හා මේ ගී පද ගැලපු  තනුවක් වාගේ නුබ මට මියුරු  එන මග සරසා නුබ යනවිට තනිවූ  දවසක් ඒවිද ආයෙත් නුබ මට හිමි වූ.. &amp;lt;3 https://t.co/7OPJnK4RSs"</t>
+  </si>
+  <si>
+    <t>1075657268056576000</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 07:40:52 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Nimal15700736 @cleanpoltics @NimaliWijesuri3 @ApiWenuwen @JMLPBandara @GayaniGunaseke2 @nnalani1231 @ranjanieguruge @CBSL @RW_UNP @HarshadeSilvaMP @EranWick @MangalaLK @MaithripalaS @Senaratne77 @Neetwit @PresRajapaksa @ParliamentLK @randheeraM @nilanp @astroanu @hithuwakkari89 @galpathatlr @KalyanaMithraya @medaperadiga @AsIFxOubyozDmOY @ra5tha @Sudumameduvada @WasthiOfficial @DooWeere @udanaekanayake @Dilanka_ss @hesha_UNP01 @PiyumiShashi @Media_NR @tmfallen @Ru_Weerasuriya @vishiru @LUshimarie @paranawithana @JosephMorgan @amalab @mihywun @Aqua097 @hima_flake @LankanJokes @Yawathashi @ManoGanesan @PodujanaParty මේ ගිවිසුම හරහා අපේ රටේ සේවා ටික සිංගප්පූරුවට පමණක් නොවෙයි පාවලා දීලා තිබෙන්නේ. ඉන්දියාව, චීනය, මැලේසියාව කියන රටවල් හමුවේ පාවලා දීලා තිබෙනවා. 1815 අපේ රට සුද්දාට විතරයි යටත් වුණේ. නමුත් ලෝකයේ සියලු රටවල් හමුවේ අපිව පාවා දීලා ඉවරයි මේ https://t.co/imfO4FngUd https://t.co/F4qhD3dpJK"</t>
+  </si>
+  <si>
+    <t>1075621099487027201</t>
+  </si>
+  <si>
+    <t>2503150696</t>
+  </si>
+  <si>
+    <t>Thu Dec 20 05:17:08 +0000 2018</t>
+  </si>
+  <si>
+    <t>"වැරදි දැක්කත් ඒවා ප්‍රසිද්ධ කරලා තමන්ගෙ ආගම ගැන තියන වටිනාකම,බක්තිය අන්ආගමිකයන් ඉස්සරා නැති කර ගන්නෙ නෑ.අපිට හිතන්න සෑහෙන්න දේවල් තියෙනවා රැඩිකල් විදිහට හිතලා ටෑටු එකක් සාධාරණීකරනය කරන්න කලින්."</t>
+  </si>
+  <si>
+    <t>1075479209114505217</t>
+  </si>
+  <si>
+    <t>2290874334</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 19:53:19 +0000 2018</t>
+  </si>
+  <si>
+    <t>"එන්න දවසක. ඇවිත් මගෙ හදවතත් මෙගා පික්සල් බිලියන විසිහතරදාකට කඩල සූම් කරල බලන්න ඒ හැම කොන්ටම් අංශුවකම ආදරේ තියේවි ඔයාගෙ නමින් ලියවිලා හැමදාටම .... ❤️  යෝ..යෝ... #බොබී"</t>
+  </si>
+  <si>
+    <t>1075453827577303040</t>
+  </si>
+  <si>
+    <t>169831468</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 18:12:28 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ඔයාටත් ඉන්නවද?  පාරෙ යද්දි අඳුරන අය ඉස්සරහට එද්දි අත අතාරින   ඔයා එයාගෙ යාලුවෙක් විතරයි කියලා හැමෝටම කියලා තියන   හැම තිස්සෙම නිදහසට කාරණා කිය කිය කාර්‍යබහුල බව අඟවන, ඒත් online ඉන්න  හැම දේටම බොරුවට සැක කරන, හේතු හදාගෙන තරහ වෙන   .............කෙනෙක්??? 😔😔"</t>
+  </si>
+  <si>
+    <t>1075452856977678336</t>
+  </si>
+  <si>
+    <t>836512553622593536</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 18:08:36 +0000 2018</t>
+  </si>
+  <si>
+    <t>"මේම පැටලැවිල්ලක් උනොත් තමා අපිට කෝල් එන්නේ.. නැත්තම් කොල් කරන්නේ අර dialog එකෙන් බූට් සින්දු call a tune දාගන්න කියන කෝල් එක තමා..😂😂 https://t.co/8ctmWnrSGc"</t>
+  </si>
+  <si>
+    <t>1075442890300518400</t>
+  </si>
+  <si>
+    <t>181142874</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 17:29:00 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අතීතයට ගිහින් දේවල් වෙනස් කරනවා කියන මිත්‍යාව මිත්‍යාවක් ලෙසටම හැමදාම තියෙනවනම් හොඳයි. අනාගතයක් කියලා දෙයක් නැත්තටම නැති වෙන්න පුලුවන් එහෙම උනොත්."</t>
+  </si>
+  <si>
+    <t>1075404513094262784</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:56:30 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ගෙදරින් පිට, බෝඩිං වල ඉන්නකොට ගෙදර වෙන කිසිම අවුලක් තාත්තා මට කියන්නෙ නෑ. වෙන අයට කියන්න දෙන්නෙත් නෑ. අම්මා මොකක් හරි කියන්න යනකොට පැනලා ඒක නවත්තනවා.  ඒ මම ඒවා හිතට අරන් ඔළුවට වදයක් කරගනී කියලා හිතලා ලු.  තාත්තලාගෙ ආදරේ හරි වෙනස්. ගැඹුරුයි. සමහරවිට තේරුම්ගන්නත් අමාරුයි. 😌❤️"</t>
+  </si>
+  <si>
+    <t>1075398073344389120</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:30:55 +0000 2018</t>
+  </si>
+  <si>
+    <t>"මට ජිවිතේ කවදාකවත් නුවර යන්න හේතුවක් ඕනි වුණේ නෑ.. දළදා මාලිගාව ඉස්සරහින් වැව දිගේ යද්දී , මාලිගාවෙන් එන සුවද , ඒ මගුල්බෙර වාදනය නිසා හිතට පුදුම සැහැල්ලුවක් දැනෙන්නේ.. මේ අවුරුදු ගානටම සෙරෙප්පු දෙක හිතලා ගලවනවා නෙවෙයි ... කකුල් වලින් සෙරෙප්පු දෙක ගැලවෙනවා ශ්‍රී දන්ත ධාතුව 👇"</t>
+  </si>
+  <si>
+    <t>1075397181173977088</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 14:27:22 +0000 2018</t>
+  </si>
+  <si>
+    <t>"‌සමහර එවුන් මේකට එන්නෙම කෙනෙක් කරන වැඩේ නතර කරලා මොකක් හරි පොර ටෝක් එකක් දීලා යන්න. උන් කරන්නෙත් නෑ, කරන එවුන්ට කරන්න දෙන්නෙත් නෑ. ඕකුන් තමයි කවදාහරි බැන්ද දවසක පලමු රාත්‍රීයේ යාලුවන්ට කෝල් කර කර " ඒ මචන් මොකෝ බං මං දැන් කරන්න ඕන, නිදාගත්තට කමක් නැද්ද " කිය කිය ඇඩ්වයිස් ගන්නේ. 😅"</t>
+  </si>
+  <si>
+    <t>1075385644476760064</t>
+  </si>
+  <si>
+    <t>494966093</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 13:41:31 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ජනපතිගේ බලතල අඩුකරන...20සේ මාරයා  !  වර්ධරාජා පෙරැමල් ඊළාම් රාජ්‍යයක් ප්‍රකාශයට පත්කල විට ප්‍රේමදාස ජනපති වහාම පලාත් සභාව විසරැවා හැරිමෙන් උතුරේ ඊළම් රාජ්‍යය එදා වැළකුනා  අද 20න් ජනපතිගේ බලතල කප්පාදුවක් සිදු උනොත් රට ජාතියට සිදුවන බරපතල වරද යලි හදනු බෑ පිහිට වූ ඊළම යලි ගනුත් බෑ🤔"</t>
+  </si>
+  <si>
+    <t>1075380583541293056</t>
+  </si>
+  <si>
+    <t>1840541953</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 13:21:25 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ අපාරාදෙ කියන්නෙ බැ මෙකෙ ඉන්න මිනිසුන් කවද හරි දවසක් ඔය  administer role එකක්.කරොත් තමන්ගේ service ගන්න පුද්ගලයෙක් අසාධාරණයක් උනොත් පිලිසරණ ක් නැ මොලෙ පරිණත වෙලා.නැ එකතාමා  අවුල"</t>
+  </si>
+  <si>
+    <t>1075363607679025152</t>
+  </si>
+  <si>
+    <t>809347326</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 12:13:58 +0000 2018</t>
+  </si>
+  <si>
+    <t>"දුම්රියේ යන කට්ටියගෙන් මෙච්චර කල් කිසි උදව්වක් ඉල්ලලා නෑ මං...අද පොඩි උදව්වක් ඉල්ලන්න කල්පනා කරා...  https://t.co/AQkH2cpR8y Train ඇප් එකට Vote කරලා උදව්වක් කරන්න...හැමදාම පරක්කු වෙන කෝච්චිය ගැන Update ගන්නවා වගේම සේවය ලබාගත්... https://t.co/8NiYoxy4sY"</t>
+  </si>
+  <si>
+    <t>1075325247627309056</t>
+  </si>
+  <si>
+    <t>36591833</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 09:41:32 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@ranukad යකෝ කවුරු හරි මුල්වෙලා එහෙම දෙයක් කරන නිසයි එන්න බැරි වුනත් මුන්ටික ආතල් එකක් ගන්නවා නේද කියලා හිතලා හරි සතුටුවෙන්නේ..! අහක ඉන්න වේස නරි එක එක ඒවා කිව්වා කියලා, උඹලා කරන වැඩ නවත්තන්න හිතනවා නං, මට කියන්න තියෙන්නේ අනේ මංදා කියලා තමා රනුක.! 😑"</t>
+  </si>
+  <si>
+    <t>1075967834671374336</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 04:14:56 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Sanju_Live දිගටම නොනවත්වා මෙහෙම උනොත් අපිට සිද්ද වෙනව ක්‍රියාමාර්ගයක් ගන්න.. ගහනව අපිත් ඔක්කොම ඩුප්ලිකේට්.."</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>1075287281508831233</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 07:10:40 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@SHAN_EVO_ දවසක එන්නම් බීලා යන්න 🍻"</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>1075276452445151232</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 06:27:38 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@PinkySandaruwni අපි හිතලා ඒක කරලා දෙමු... අකැමැති වෙන්න දෙයක් නෑ.. අපි දෙන්නට කැමතියිනේ 😏"</t>
+  </si>
+  <si>
+    <t>1075271169970921473</t>
+  </si>
+  <si>
+    <t>875015304639676417</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 06:06:39 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@SHAN_EVO_ @CHIRU_Vibes කෝමත් දවසක මීට් වෙමුකෝ 😊"</t>
+  </si>
+  <si>
+    <t>1075270084820590592</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 06:02:20 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@nadeerap6 තවම.නෑ ඉස්සරහට නැති උනොත් කියන්නම්කො"</t>
+  </si>
+  <si>
+    <t>1075268863833432064</t>
+  </si>
+  <si>
+    <t>1014093357318934529</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 05:57:29 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@RShashiya @PinkySandaruwni සස් පෙන් අනේ ඇන්ටිගේ යාලුවෙක් උනොත් කියල කියන්නෙ 😂"</t>
+  </si>
+  <si>
+    <t>1075268593770586112</t>
+  </si>
+  <si>
+    <t>2425930645</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 05:56:24 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@PinkySandaruwni @RakzzMaduOnline මොන පෙන් උනොත්.. ???"</t>
+  </si>
+  <si>
+    <t>1075266730887446529</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 05:49:00 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අහල පහල ගෙදරකින් #රතුමකරාFM එකේ ඔටෝ ප්ලේ යන සිංදු වගේ සෙට් එකක් ඇහෙනවා.. 🤔 සැක සහිතයි.."</t>
+  </si>
+  <si>
+    <t>1075265885835689984</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 05:45:39 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@da_sukiya @imhiran99 ඔය රිප්ලයි එක මකාං යකෝ. බඩු බනිස්වෙයි. ඉංගිරිසියෙන් ප්‍රොනව්න්ස් උනාට අකුරු සිංහල උනොත් කේස්"</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>1075205669094129665</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 01:46:22 +0000 2018</t>
+  </si>
+  <si>
+    <t>"මාගේ දෑස දෙස බලනු! මෙතැන් පටන් ඔබ ඇසිපිය ගහන්නෙ හිතින් හිතලා."</t>
+  </si>
+  <si>
+    <t>1075205618623893504</t>
+  </si>
+  <si>
+    <t>877432405014888449</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 01:46:10 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අපෙ ගෙවල් පැත්ත අරාබිය වගෙ උනාට මෙ ලගදි දවසක රුවැති යුවැතියක් පැමිනියා  අම්මො අම්මො"</t>
+  </si>
+  <si>
+    <t>1075193453183676416</t>
+  </si>
+  <si>
+    <t>1685141124</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 00:57:50 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ජිම් යන එකට් එපා වෙලා තියෙන්නෙ කිලෝ දෙකක් වැඩි උනොත් ඊලග සතියෙ කිලෝ තුනක් අඩු වෙනවා😑"</t>
+  </si>
+  <si>
+    <t>1075166071823499265</t>
+  </si>
+  <si>
+    <t>2995187646</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 23:09:01 +0000 2018</t>
+  </si>
+  <si>
+    <t>"අපිට සෙට් උනොත් සෙට් වෙන්නෙ කැරිම නඩුවක්😂නැත්තන් කැරිම බඩුවක්😂🤘 — feeling ���"</t>
+  </si>
+  <si>
+    <t>1075131327010074624</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 20:50:57 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ලෝගන් කෝ සුඛියා කෝ අරූ කෝ මු කෝ කියලා අහන උන් තමා කවදාහරි බැන්ඳ දවසක ගෑණි කෝ කියලා හොයන්නේ 🙄"</t>
+  </si>
+  <si>
+    <t>1075129774782083073</t>
+  </si>
+  <si>
+    <t>166556379</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 20:44:47 +0000 2018</t>
+  </si>
+  <si>
+    <t>"හොයලා හොයලා කොල්ලෙක් හොයා ගන්නම බැරි උනොත් මම හම්සව බදිනවා"</t>
+  </si>
+  <si>
+    <t>1075129710147969025</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 20:44:32 +0000 2018</t>
+  </si>
+  <si>
+    <t>1075121878270861312</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 20:13:25 +0000 2018</t>
+  </si>
+  <si>
+    <t>"දත් දොස්තර කෝ?? මගෙ වෙඩිමට පරක්කු වෙනවා."</t>
+  </si>
+  <si>
+    <t>1075119614969864192</t>
+  </si>
+  <si>
+    <t>137992580</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 20:04:25 +0000 2018</t>
+  </si>
+  <si>
+    <t>"බීලා මාට්ටු උනොත් වල් අලි ගහනවා යකෝ. 😂"</t>
+  </si>
+  <si>
+    <t>1075114065222098944</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 19:42:22 +0000 2018</t>
+  </si>
+  <si>
+    <t>"උඹල මෙහෙම සබ් ගහනවා කියලා දන්නවනම් මම දවසක් පරක්කු⁣ වෙලා ඉපදෙනවා..  - මීට චෙත්‍යා"</t>
+  </si>
+  <si>
+    <t>1075967724428222464</t>
+  </si>
+  <si>
+    <t>Fri Dec 21 04:14:30 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@maalupaan මම සැක කලා.   ඒ දරුවා මුල සිටම මං ගැන අමනාපෙන් හිටියේ. ඉතින් මමත් ඒ වගේ අය පැත්තකට කරලා නොසොයා හිටියේ. ඒකයි එක පාර මතක නැති උනේ.  හැබැයි එයාගේ බුදු ෆිට් ලිස්ට් එකේ ඔයත් හිටියද? කීයටවත් වෙන්න බෑ"</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>1075295092347469824</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 07:41:42 +0000 2018</t>
+  </si>
+  <si>
+    <t>"හිතෙන විකාර ට්වීට් කරලා හැමදාම දැම්මා. ඒකෙ චුට්ටං හරි ආර්ට් එකක් දැකලා  #ජොබ්එකගාවගමු කියලා හිතලා @moogater අක්කා ලියන්න උදව්කරා. ඇයි අනිත් අයටත් ඒ වගේ හොඳ විදිහට අනිත් අයට උදව්කරන්න බැරි?"</t>
+  </si>
+  <si>
+    <t>1075230792844861441</t>
+  </si>
+  <si>
+    <t>981202311908179968</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 03:26:12 +0000 2018</t>
+  </si>
+  <si>
+    <t>"එයා කිවුවා කැටයක් අරගෙන හැමදාම ඒකට රුපියක් දහය ගානේ හරි.. ඊට වැඩියෙන් හරි දාන්න කියලා. හොද දෙයක් වෙනුවෙන් කිවුවා.දවසක ආයෙත් මගේ ලගට එනවා කිවුවා හේතුවත් අරගෙනම. මොකක්ද ඒ මාරම පස්නයක් ඒක..... 🧐🧐🧐🧐🧐🧐🧐🧐 #දැවෙනප්‍රශ්න"</t>
+  </si>
+  <si>
+    <t>1075219187994222592</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 02:40:05 +0000 2018</t>
+  </si>
+  <si>
+    <t>"නෑ නෑ මම දැන් දැක්කේ තව ලෝගන් අයියා කෙනෙක් ඉන්නවනේ..... හිත හදාගනින් බං.... උබේ නම කියලත් දවසක කවුරුහරි ටුයිට් කරාවි 😔😔 #තනියමකියවයි https://t.co/cNKdVPxWLz"</t>
+  </si>
+  <si>
+    <t>1075206313230155776</t>
+  </si>
+  <si>
+    <t>3001832971</t>
+  </si>
+  <si>
+    <t>Wed Dec 19 01:48:56 +0000 2018</t>
+  </si>
+  <si>
+    <t>"Naththal Awa - Latha Walpola and Eranga Lanka  නත්තල් ආවා ආවා ආවා ජේසු බිලිඳු ආවා  උඳුවප් මාසේ සීතල දවසක මැදියම් රෑ යාමේ  බෙත්ලෙහෙමේ පුංචි ගවලෙනේ ජේසු උපත වූයේ  සාමයේ අරුණලු දසත පැතිර ගියේ  නත්තලේ අපි... https://t.co/cOu1xPZhFm"</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>1075115578552008704</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 19:48:23 +0000 2018</t>
+  </si>
+  <si>
+    <t>"ලෝගා දාපු එක ඩුප්ලිකේට් ගහන්නත් හිතලා ආයේ අතෑරියා. සයිබර් බුලින් කරලා රස්සාව නැති කරගන්න බෑ. ලෝගව රිපෝර්ට් කලා හේට් ස්පීච් කියලා. වෙලාවට ඌ රිපෝර්ට් කරන විදිහ කලින් කියලා තිබුනේ 😂"</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>1075115398851248128</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 19:47:40 +0000 2018</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>1075109556919853056</t>
+  </si>
+  <si>
+    <t>911573887</t>
+  </si>
+  <si>
+    <t>Tue Dec 18 19:24:27 +0000 2018</t>
+  </si>
+  <si>
+    <t>"එතකොට බැරිවෙලාවත් ඒකාබද්ධෙන් ආන්ඩුව පිහිටවලා තිබිලා ඒකට unp එකෙන් කවුරු හරි පැන්නොත් ඇමතිකම් දෙනවා.  හැබැයි,   Unp එකෙන් ආන්ඩු පිහිටවලා ඒකට ඒකාබද්දේ හෝ නිදහස් පක්ශේ කවුරු හරි unp එක එක්කලා එක්කහු උනොත් එතකොට ඇමතිකම් නෑ.  මෛත්‍රිපාලගෙත් තියෙන්නේ ටෞකණ තියරි බොල..! 🤭🤔"</t>
   </si>
 </sst>
 </file>
@@ -5325,10 +6453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F371"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5356,7 +6484,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -12741,26 +13869,2006 @@
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A371" s="7" t="s">
-        <v>1631</v>
+        <v>52</v>
       </c>
       <c r="B371" s="7" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C371" s="7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D371" s="7" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E371" s="7" t="s">
+        <v>1898</v>
+      </c>
+      <c r="F371" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A372" s="7" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B372" s="7" t="s">
         <v>1632</v>
       </c>
-      <c r="C371" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="D371" s="7" t="s">
+      <c r="C372" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D372" s="7" t="s">
         <v>1633</v>
       </c>
-      <c r="E371" s="7" t="s">
+      <c r="E372" s="7" t="s">
+        <v>1634</v>
+      </c>
+      <c r="F372" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A373" s="7" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B373" s="7" t="s">
         <v>1635</v>
       </c>
-      <c r="F371" s="7" t="s">
+      <c r="C373" s="7" t="s">
+        <v>1636</v>
+      </c>
+      <c r="D373" s="7" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E373" s="7" t="s">
+        <v>1638</v>
+      </c>
+      <c r="F373" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A374" s="7" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B374" s="7" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C374" s="7" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D374" s="7" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E374" s="7" t="s">
+        <v>1642</v>
+      </c>
+      <c r="F374" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A375" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B375" s="7" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C375" s="7" t="s">
+        <v>1644</v>
+      </c>
+      <c r="D375" s="7" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E375" s="7" t="s">
+        <v>1646</v>
+      </c>
+      <c r="F375" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A376" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B376" s="7" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C376" s="7" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D376" s="7" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E376" s="7" t="s">
+        <v>1650</v>
+      </c>
+      <c r="F376" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A377" s="7" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B377" s="7" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C377" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D377" s="7" t="s">
+        <v>1652</v>
+      </c>
+      <c r="E377" s="7" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F377" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A378" s="7" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B378" s="7" t="s">
+        <v>1654</v>
+      </c>
+      <c r="C378" s="7" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D378" s="7" t="s">
+        <v>1656</v>
+      </c>
+      <c r="E378" s="7" t="s">
+        <v>1657</v>
+      </c>
+      <c r="F378" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A379" s="7" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B379" s="7" t="s">
+        <v>1658</v>
+      </c>
+      <c r="C379" s="7" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D379" s="7" t="s">
+        <v>1660</v>
+      </c>
+      <c r="E379" s="7" t="s">
+        <v>1661</v>
+      </c>
+      <c r="F379" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A380" s="7" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B380" s="7" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C380" s="7" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D380" s="7" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E380" s="7" t="s">
+        <v>1665</v>
+      </c>
+      <c r="F380" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A381" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B381" s="7" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C381" s="7" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D381" s="7" t="s">
+        <v>1668</v>
+      </c>
+      <c r="E381" s="7" t="s">
+        <v>1669</v>
+      </c>
+      <c r="F381" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A382" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B382" s="7" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C382" s="7" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D382" s="7" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E382" s="7" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F382" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A383" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B383" s="7" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C383" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D383" s="7" t="s">
+        <v>1674</v>
+      </c>
+      <c r="E383" s="7" t="s">
+        <v>1675</v>
+      </c>
+      <c r="F383" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A384" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B384" s="7" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C384" s="7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D384" s="7" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E384" s="7" t="s">
+        <v>1679</v>
+      </c>
+      <c r="F384" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A385" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B385" s="7" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C385" s="7" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D385" s="7" t="s">
+        <v>1682</v>
+      </c>
+      <c r="E385" s="7" t="s">
+        <v>1683</v>
+      </c>
+      <c r="F385" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A386" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B386" s="7" t="s">
+        <v>1684</v>
+      </c>
+      <c r="C386" s="7" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D386" s="7" t="s">
+        <v>1686</v>
+      </c>
+      <c r="E386" s="7" t="s">
+        <v>1687</v>
+      </c>
+      <c r="F386" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A387" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B387" s="7" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C387" s="7" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D387" s="7" t="s">
+        <v>1690</v>
+      </c>
+      <c r="E387" s="7" t="s">
+        <v>1691</v>
+      </c>
+      <c r="F387" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A388" s="7" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B388" s="7" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C388" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D388" s="7" t="s">
+        <v>1694</v>
+      </c>
+      <c r="E388" s="7" t="s">
+        <v>1695</v>
+      </c>
+      <c r="F388" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A389" s="7" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B389" s="7" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C389" s="7" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D389" s="7" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E389" s="7" t="s">
+        <v>1699</v>
+      </c>
+      <c r="F389" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A390" s="7" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B390" s="7" t="s">
+        <v>1700</v>
+      </c>
+      <c r="C390" s="7" t="s">
+        <v>829</v>
+      </c>
+      <c r="D390" s="7" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E390" s="7" t="s">
+        <v>1702</v>
+      </c>
+      <c r="F390" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A391" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B391" s="7" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C391" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D391" s="7" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E391" s="7" t="s">
+        <v>1706</v>
+      </c>
+      <c r="F391" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A392" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B392" s="7" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C392" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D392" s="7" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E392" s="7" t="s">
+        <v>1709</v>
+      </c>
+      <c r="F392" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A393" s="7" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B393" s="7" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C393" s="7" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D393" s="7" t="s">
+        <v>1712</v>
+      </c>
+      <c r="E393" s="7" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F393" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A394" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B394" s="7" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C394" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D394" s="7" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E394" s="7" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F394" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A395" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B395" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C395" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D395" s="7" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E395" s="7" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F395" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A396" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B396" s="7" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C396" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D396" s="7" t="s">
+        <v>1722</v>
+      </c>
+      <c r="E396" s="7" t="s">
+        <v>1723</v>
+      </c>
+      <c r="F396" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A397" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B397" s="7" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C397" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="D397" s="7" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E397" s="7" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F397" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A398" s="7" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B398" s="7" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C398" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D398" s="7" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E398" s="7" t="s">
+        <v>1729</v>
+      </c>
+      <c r="F398" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A399" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B399" s="7" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C399" s="7" t="s">
+        <v>1731</v>
+      </c>
+      <c r="D399" s="7" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E399" s="7" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F399" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A400" s="7" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B400" s="7" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C400" s="7" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D400" s="7" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E400" s="7" t="s">
+        <v>1737</v>
+      </c>
+      <c r="F400" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A401" s="7" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B401" s="7" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C401" s="7" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D401" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E401" s="7" t="s">
+        <v>1741</v>
+      </c>
+      <c r="F401" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A402" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B402" s="7" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C402" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D402" s="7" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E402" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F402" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A403" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B403" s="7" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C403" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D403" s="7" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E403" s="7" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F403" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A404" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B404" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C404" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D404" s="7" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E404" s="7" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F404" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A405" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B405" s="7" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C405" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D405" s="7" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E405" s="7" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F405" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A406" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B406" s="7" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C406" s="7" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D406" s="7" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E406" s="7" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F406" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A407" s="7" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B407" s="7" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C407" s="7" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D407" s="7" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E407" s="7" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F407" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A408" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B408" s="7" t="s">
+        <v>1761</v>
+      </c>
+      <c r="C408" s="7" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D408" s="7" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E408" s="7" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F408" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A409" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B409" s="7" t="s">
+        <v>1765</v>
+      </c>
+      <c r="C409" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D409" s="7" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E409" s="7" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F409" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A410" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B410" s="7" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C410" s="7" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D410" s="7" t="s">
+        <v>1770</v>
+      </c>
+      <c r="E410" s="7" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F410" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A411" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B411" s="7" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C411" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D411" s="7" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E411" s="7" t="s">
+        <v>1774</v>
+      </c>
+      <c r="F411" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A412" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B412" s="7" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C412" s="7" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D412" s="7" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E412" s="7" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F412" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A413" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B413" s="7" t="s">
+        <v>1779</v>
+      </c>
+      <c r="C413" s="7" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D413" s="7" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E413" s="7" t="s">
+        <v>1781</v>
+      </c>
+      <c r="F413" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A414" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B414" s="7" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C414" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="D414" s="7" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E414" s="7" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F414" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A415" s="7" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B415" s="7" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C415" s="7" t="s">
+        <v>1786</v>
+      </c>
+      <c r="D415" s="7" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E415" s="7" t="s">
+        <v>1788</v>
+      </c>
+      <c r="F415" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A416" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B416" s="7" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C416" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D416" s="7" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E416" s="7" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F416" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A417" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B417" s="7" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C417" s="7" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D417" s="7" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E417" s="7" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F417" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A418" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B418" s="7" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C418" s="7" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D418" s="7" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E418" s="7" t="s">
+        <v>1799</v>
+      </c>
+      <c r="F418" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A419" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B419" s="7" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C419" s="7" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D419" s="7" t="s">
+        <v>1802</v>
+      </c>
+      <c r="E419" s="7" t="s">
+        <v>1803</v>
+      </c>
+      <c r="F419" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A420" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B420" s="7" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C420" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D420" s="7" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E420" s="7" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F420" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A421" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B421" s="7" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C421" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D421" s="7" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E421" s="7" t="s">
+        <v>1809</v>
+      </c>
+      <c r="F421" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A422" s="7" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B422" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="C422" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D422" s="7" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E422" s="7" t="s">
+        <v>1813</v>
+      </c>
+      <c r="F422" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A423" s="7" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B423" s="7" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C423" s="7" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D423" s="7" t="s">
+        <v>1816</v>
+      </c>
+      <c r="E423" s="7" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F423" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A424" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B424" s="7" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C424" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D424" s="7" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E424" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="F424" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A425" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B425" s="7" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C425" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D425" s="7" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E425" s="7" t="s">
+        <v>1823</v>
+      </c>
+      <c r="F425" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A426" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B426" s="7" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C426" s="7" t="s">
+        <v>1825</v>
+      </c>
+      <c r="D426" s="7" t="s">
+        <v>1826</v>
+      </c>
+      <c r="E426" s="7" t="s">
+        <v>1827</v>
+      </c>
+      <c r="F426" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A427" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B427" s="7" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C427" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D427" s="7" t="s">
+        <v>1918</v>
+      </c>
+      <c r="E427" s="7" t="s">
+        <v>1919</v>
+      </c>
+      <c r="F427" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A428" s="7" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B428" s="7" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C428" s="7" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D428" s="7" t="s">
+        <v>1922</v>
+      </c>
+      <c r="E428" s="7" t="s">
+        <v>1923</v>
+      </c>
+      <c r="F428" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A429" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B429" s="7" t="s">
+        <v>1924</v>
+      </c>
+      <c r="C429" s="7" t="s">
+        <v>1925</v>
+      </c>
+      <c r="D429" s="7" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E429" s="7" t="s">
+        <v>1927</v>
+      </c>
+      <c r="F429" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A430" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B430" s="7" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C430" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="D430" s="7" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E430" s="7" t="s">
+        <v>1930</v>
+      </c>
+      <c r="F430" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A431" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B431" s="7" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C431" s="7" t="s">
+        <v>1932</v>
+      </c>
+      <c r="D431" s="7" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E431" s="7" t="s">
+        <v>1934</v>
+      </c>
+      <c r="F431" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A432" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B432" s="7" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C432" s="7" t="s">
+        <v>1936</v>
+      </c>
+      <c r="D432" s="7" t="s">
+        <v>1937</v>
+      </c>
+      <c r="E432" s="7" t="s">
+        <v>1938</v>
+      </c>
+      <c r="F432" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A433" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B433" s="7" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C433" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D433" s="7" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E433" s="7" t="s">
+        <v>1941</v>
+      </c>
+      <c r="F433" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A434" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B434" s="7" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C434" s="7" t="s">
+        <v>1936</v>
+      </c>
+      <c r="D434" s="7" t="s">
+        <v>1943</v>
+      </c>
+      <c r="E434" s="7" t="s">
+        <v>1944</v>
+      </c>
+      <c r="F434" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A435" s="7" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B435" s="7" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C435" s="7" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D435" s="7" t="s">
+        <v>1947</v>
+      </c>
+      <c r="E435" s="7" t="s">
+        <v>1948</v>
+      </c>
+      <c r="F435" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A436" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B436" s="7" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C436" s="7" t="s">
+        <v>1950</v>
+      </c>
+      <c r="D436" s="7" t="s">
+        <v>1951</v>
+      </c>
+      <c r="E436" s="7" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F436" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A437" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B437" s="7" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C437" s="7" t="s">
+        <v>1954</v>
+      </c>
+      <c r="D437" s="7" t="s">
+        <v>1955</v>
+      </c>
+      <c r="E437" s="7" t="s">
+        <v>1956</v>
+      </c>
+      <c r="F437" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A438" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B438" s="7" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C438" s="7" t="s">
+        <v>1958</v>
+      </c>
+      <c r="D438" s="7" t="s">
+        <v>1959</v>
+      </c>
+      <c r="E438" s="4" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F438" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A439" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B439" s="7" t="s">
+        <v>1961</v>
+      </c>
+      <c r="C439" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="D439" s="7" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E439" s="7" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F439" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A440" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B440" s="7" t="s">
+        <v>1964</v>
+      </c>
+      <c r="C440" s="7" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D440" s="7" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E440" s="4" t="s">
+        <v>1967</v>
+      </c>
+      <c r="F440" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A441" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B441" s="7" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C441" s="7" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D441" s="7" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E441" s="4" t="s">
+        <v>1967</v>
+      </c>
+      <c r="F441" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A442" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B442" s="7" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C442" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="D442" s="7" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E442" s="7" t="s">
+        <v>1972</v>
+      </c>
+      <c r="F442" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A443" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B443" s="7" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C443" s="7" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D443" s="7" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E443" s="7" t="s">
+        <v>1976</v>
+      </c>
+      <c r="F443" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A444" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B444" s="7" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C444" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D444" s="7" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E444" s="7" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F444" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A445" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B445" s="7" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C445" s="7" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D445" s="7" t="s">
+        <v>1981</v>
+      </c>
+      <c r="E445" s="7" t="s">
+        <v>1982</v>
+      </c>
+      <c r="F445" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A446" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B446" s="7" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C446" s="7" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D446" s="7" t="s">
+        <v>1831</v>
+      </c>
+      <c r="E446" s="7" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F446" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A447" s="7" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B447" s="7" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C447" s="7" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D447" s="7" t="s">
+        <v>1835</v>
+      </c>
+      <c r="E447" s="7" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F447" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A448" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B448" s="7" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C448" s="7" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D448" s="7" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E448" s="7" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F448" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A449" s="7" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B449" s="7" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C449" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="D449" s="7" t="s">
+        <v>1842</v>
+      </c>
+      <c r="E449" s="7" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F449" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A450" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B450" s="7" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C450" s="7" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D450" s="7" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E450" s="7" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F450" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A451" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B451" s="7" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C451" s="7" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D451" s="7" t="s">
+        <v>1849</v>
+      </c>
+      <c r="E451" s="7" t="s">
+        <v>1850</v>
+      </c>
+      <c r="F451" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A452" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B452" s="7" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C452" s="7" t="s">
+        <v>1852</v>
+      </c>
+      <c r="D452" s="7" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E452" s="7" t="s">
+        <v>1854</v>
+      </c>
+      <c r="F452" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A453" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B453" s="7" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C453" s="7" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D453" s="7" t="s">
+        <v>1857</v>
+      </c>
+      <c r="E453" s="7" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F453" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A454" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B454" s="7" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C454" s="7" t="s">
+        <v>1860</v>
+      </c>
+      <c r="D454" s="7" t="s">
+        <v>1861</v>
+      </c>
+      <c r="E454" s="7" t="s">
+        <v>1862</v>
+      </c>
+      <c r="F454" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A455" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B455" s="7" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C455" s="7" t="s">
+        <v>1864</v>
+      </c>
+      <c r="D455" s="7" t="s">
+        <v>1865</v>
+      </c>
+      <c r="E455" s="7" t="s">
+        <v>1866</v>
+      </c>
+      <c r="F455" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A456" s="7" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B456" s="7" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C456" s="7" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D456" s="7" t="s">
+        <v>1869</v>
+      </c>
+      <c r="E456" s="7" t="s">
+        <v>1870</v>
+      </c>
+      <c r="F456" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A457" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="B457" s="7" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C457" s="7" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D457" s="7" t="s">
+        <v>1872</v>
+      </c>
+      <c r="E457" s="7" t="s">
+        <v>1873</v>
+      </c>
+      <c r="F457" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A458" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B458" s="7" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C458" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D458" s="7" t="s">
+        <v>1875</v>
+      </c>
+      <c r="E458" s="7" t="s">
+        <v>1876</v>
+      </c>
+      <c r="F458" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A459" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B459" s="7" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C459" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="D459" s="7" t="s">
+        <v>1878</v>
+      </c>
+      <c r="E459" s="7" t="s">
+        <v>1879</v>
+      </c>
+      <c r="F459" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A460" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B460" s="7" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C460" s="7" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D460" s="7" t="s">
+        <v>1882</v>
+      </c>
+      <c r="E460" s="4" t="s">
+        <v>1883</v>
+      </c>
+      <c r="F460" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A461" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B461" s="7" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C461" s="7" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D461" s="7" t="s">
+        <v>1886</v>
+      </c>
+      <c r="E461" s="7" t="s">
+        <v>1887</v>
+      </c>
+      <c r="F461" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A462" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B462" s="7" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C462" s="7" t="s">
+        <v>1889</v>
+      </c>
+      <c r="D462" s="7" t="s">
+        <v>1890</v>
+      </c>
+      <c r="E462" s="7" t="s">
+        <v>1891</v>
+      </c>
+      <c r="F462" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A463" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B463" s="7" t="s">
+        <v>1892</v>
+      </c>
+      <c r="C463" s="7" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D463" s="7" t="s">
+        <v>1894</v>
+      </c>
+      <c r="E463" s="4" t="s">
+        <v>1895</v>
+      </c>
+      <c r="F463" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A464" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B464" s="7" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C464" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="D464" s="7" t="s">
+        <v>1987</v>
+      </c>
+      <c r="E464" s="7" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F464" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A465" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B465" s="7" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C465" s="7" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D465" s="7" t="s">
+        <v>1991</v>
+      </c>
+      <c r="E465" s="7" t="s">
+        <v>1992</v>
+      </c>
+      <c r="F465" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A466" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B466" s="7" t="s">
+        <v>1993</v>
+      </c>
+      <c r="C466" s="7" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D466" s="7" t="s">
+        <v>1994</v>
+      </c>
+      <c r="E466" s="4" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F466" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A467" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B467" s="7" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C467" s="7" t="s">
+        <v>1997</v>
+      </c>
+      <c r="D467" s="7" t="s">
+        <v>1998</v>
+      </c>
+      <c r="E467" s="7" t="s">
+        <v>1999</v>
+      </c>
+      <c r="F467" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A468" s="7" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B468" s="7" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C468" s="7" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D468" s="7" t="s">
+        <v>2002</v>
+      </c>
+      <c r="E468" s="4" t="s">
+        <v>2003</v>
+      </c>
+      <c r="F468" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A469" s="7" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B469" s="7" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C469" s="7" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D469" s="7" t="s">
+        <v>2006</v>
+      </c>
+      <c r="E469" s="4" t="s">
+        <v>2003</v>
+      </c>
+      <c r="F469" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A470" s="7" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B470" s="7" t="s">
+        <v>2008</v>
+      </c>
+      <c r="C470" s="7" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D470" s="7" t="s">
+        <v>2010</v>
+      </c>
+      <c r="E470" s="7" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F470" s="7" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Neutral,Racist,Sexism"</formula1>
     </dataValidation>
@@ -12768,7 +15876,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211" numberStoredAsText="1"/>
+    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211 A371:E470" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more 100 tweets to final-data-set excel file
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2820" uniqueCount="2012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3408" uniqueCount="2376">
   <si>
     <t>instance_id</t>
   </si>
@@ -6079,6 +6079,1098 @@
   </si>
   <si>
     <t>"එතකොට බැරිවෙලාවත් ඒකාබද්ධෙන් ආන්ඩුව පිහිටවලා තිබිලා ඒකට unp එකෙන් කවුරු හරි පැන්නොත් ඇමතිකම් දෙනවා.  හැබැයි,   Unp එකෙන් ආන්ඩු පිහිටවලා ඒකට ඒකාබද්දේ හෝ නිදහස් පක්ශේ කවුරු හරි unp එක එක්කලා එක්කහු උනොත් එතකොට ඇමතිකම් නෑ.  මෛත්‍රිපාලගෙත් තියෙන්නේ ටෞකණ තියරි බොල..! 🤭🤔"</t>
+  </si>
+  <si>
+    <t>1085457780142616577</t>
+  </si>
+  <si>
+    <t>750011074762551300</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 08:44:36 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@sanathk53122963 ගල් ගොඩ උඩ ඉන්න ඇච්චා 😂👋"</t>
+  </si>
+  <si>
+    <t>1085444873833062401</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 07:53:19 +0000 2019</t>
+  </si>
+  <si>
+    <t>"*සාරංශය....* ***'අායුෂ කෙටියි'***  වැඩිය  'උඩ පනින' 'කෑැැ....ගහන' 'දගලන' කාට කාටත්.....ඔන්න කිව්වා🧐🤔🧐 https://t.co/FISpuezJCI"</t>
+  </si>
+  <si>
+    <t>1085443762094891008</t>
+  </si>
+  <si>
+    <t>810810947099127809</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 07:48:54 +0000 2019</t>
+  </si>
+  <si>
+    <t>"පාරෙ යන මිනිස්සු මං දිහා බල බල යනව..මොකක් හරි අවුලක්වත්ද මගෙ..😲😧"</t>
+  </si>
+  <si>
+    <t>1085434776696217600</t>
+  </si>
+  <si>
+    <t>872998596936962050</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 07:13:11 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ayajnaz උඩ යන්න එපා😏"</t>
+  </si>
+  <si>
+    <t>1085429523779338240</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 06:52:19 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NandiyaLive අපි හිටපු විදිහේ මොකක් මතක් වෙන්නද බං !! එදත් පිස්සු කෙලිය අදත් එහෙම තමා 😉උබ දැන් ඉන්න විදිහ හොදයි !!"</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>1085395714476306432</t>
+  </si>
+  <si>
+    <t>860871066532663298</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 04:37:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sansajran ඒ කියන්නෙ ඕන කෙනෙක් සදුන් ගැන දන්නව😂"</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>1085389700729315330</t>
+  </si>
+  <si>
+    <t>3066340099</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 04:14:04 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@KawdaBoy @piumi_silva @itzJambole මම ඉතිං උඩ abroad ඉන්නේ 😂"</t>
+  </si>
+  <si>
+    <t>1085356807113957376</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 02:03:22 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඔය මොකක් හරි එකක් දාල...2009 කියල කියන්න.😁🙏 https://t.co/Gee0mzDjo6"</t>
+  </si>
+  <si>
+    <t>1085275097060003842</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 20:38:41 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@FriendsGammadda අනේ එතකොට නම් උඩ බිම ඉන්න බැහැ රශ්නය නිසා.තව ජර්සී දැම්මොත් හොදට තියේ...😂😂"</t>
+  </si>
+  <si>
+    <t>1085231476252147712</t>
+  </si>
+  <si>
+    <t>2590801622</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 17:45:21 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඕනෑවට වඩා උඩ තැබීමෙන් වලකින්න. බිමට බහින්නට බැරිවිය හැක."</t>
+  </si>
+  <si>
+    <t>1085218604054794241</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 16:54:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@BasnayakageGopi මොකක් 🤔🤔😂"</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>1085210515960487936</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 16:22:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ItzmeNeepi මේසෙ උඩ තියන පෝන් එක දැක්ක 😒😒😒😒"</t>
+  </si>
+  <si>
+    <t>1085202126597283841</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 15:48:43 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඇච්චා කලේ ඉඳලම ගල් උඩ තමා 😂👋😂👋 https://t.co/7wlqNZ4orQ"</t>
+  </si>
+  <si>
+    <t>1085193901902721027</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 15:16:02 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@pasiya14 දන්නව😂😂"</t>
+  </si>
+  <si>
+    <t>1085193097997209600</t>
+  </si>
+  <si>
+    <t>477723520</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 15:12:51 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@maalupaan එයාට මොකක් දැම්මත් ලයික්ස් රිප්ලයිස්. ඉරිසියයිත් එක්ක. 😩"</t>
+  </si>
+  <si>
+    <t>1085186338444333057</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 14:45:59 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@amalskr ඔව්.නැත්නම් ඔවුන් උඩ යනවා තවත්."</t>
+  </si>
+  <si>
+    <t>1085185530885623809</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 14:42:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Chami08416797 බංගි උඩ බලන් බුරනවා 😁 ඒක ඊට වඩා වදේ එතකොට"</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>1085182988978073606</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 14:32:40 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@EnThunga @Annnuza PS නං Wine උඩ වැඩ අවුලක් නැතුව"</t>
+  </si>
+  <si>
+    <t>1085164127784382464</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 13:17:44 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Nalinda_lk මොකක්"</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>1085163216823635968</t>
+  </si>
+  <si>
+    <t>125697659</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 13:14:06 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@lishwebber @moogater සිරාවටම බං! උඩ යනවනං කොහොම උඩින් යන්න ඕනේ කෙනෙක්ද නේ 💪🏽😉😊"</t>
+  </si>
+  <si>
+    <t>1085129393255530497</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 10:59:42 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@SathsaraPahan ඇයි සැක නම් මොකක් කරන්නද"</t>
+  </si>
+  <si>
+    <t>1085126265273704448</t>
+  </si>
+  <si>
+    <t>826381208728723458</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 10:47:16 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ගිය ආත්මෙ පුරුද්දට එක උඩ එක ගල් තියලා ලෙවල් බටෙන් ලෙවල් කළා නම් හරි ...😂🔫 https://t.co/7pNWWLuzkj"</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1085125052260003840</t>
+  </si>
+  <si>
+    <t>3201142667</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 10:42:27 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මිනිසා හඳට ගියාලූ මිනිසා පුදුම උනාලූ බිම බැලුවාලූ උඩ බැලුවාලූ මිනිසා හඳට ගියාලූ  #sajje #lka"</t>
+  </si>
+  <si>
+    <t>1085114105529159680</t>
+  </si>
+  <si>
+    <t>462219172</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 09:58:57 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@BeardedBrosLK දන්නව මෙයා කෙල්ලෙක්ට කෙල්ලෙක් බෝල් කරන්ඩෝනෙ ඒත් ඉතින් පැපී බෝල් කරන්නෙ අමිත් මාලින්ගගෙ ආවේසෙන් කියල ඔයල දැනගෙන ඉන්න ඕනෙ 🤦"</t>
+  </si>
+  <si>
+    <t>1085099827892051968</t>
+  </si>
+  <si>
+    <t>28772428</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 09:02:13 +0000 2019</t>
+  </si>
+  <si>
+    <t>"🤣😂😂 අපේ එවුන් නම් මොකක් හරි රෙද්දක් අල්ලගෙන මැරෙයි 🤣🤣🤣🔫 https://t.co/R2OFcnOzFl"</t>
+  </si>
+  <si>
+    <t>1085094043778863106</t>
+  </si>
+  <si>
+    <t>937851182864678913</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 08:39:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NishadiAnuttara අපි දන්නව😏"</t>
+  </si>
+  <si>
+    <t>1085080906237267969</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:47:02 +0000 2019</t>
+  </si>
+  <si>
+    <t>"P.s උඩින් දාපු පොලිතින් එක ඉරිලා ගිහින් ඒ හින්දා අල්පෙනිති උඩ මලකඩ කාලා. හදපු දවස් වල තිබ්බ ගතිය නැතුව ගිහින්."</t>
+  </si>
+  <si>
+    <t>1085079650596982784</t>
+  </si>
+  <si>
+    <t>1064609664309043202</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:42:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@SHAN_EVO_ @pasiya14 මේ ඉවෝට කවුරු හරි වතුර ටිකක් ඉහින්න පීස්. මෙයා නැති උනොත් ලස්සන මියුසික් අහලත් ඉවරයි. (ඔව් ඔව් උඩ යවන්න කිව්වෙ 🙊)"</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>1085077063294377984</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:31:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"උඩ ඉන්නෙ 😂👋 https://t.co/EkdITpAF7K"</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>1085073434026041345</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:17:21 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@TeamSesLk අහ් අයියේ ක්‍රිකට් කියන්නේ කෙල්ලො ගොඩක් දාගෙන ඇඳ උඩ කරන එකක් නෙවෙයි 😂😂"</t>
+  </si>
+  <si>
+    <t>1085071543963504640</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:09:50 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මෙයාලා මේ කියන්නෙ ක්‍රිකට් ගහන එක ගැනද.... කෙල්ලො 7 නම් ම්ම්ම්ම්.. ඒත් අන්තිමට අර කොල්ලට මොකක් වෙයිද 😂😂🏃🔪 #TCLSLමඩ https://t.co/PS9tLRnuZt"</t>
+  </si>
+  <si>
+    <t>1085065552333164544</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 06:46:01 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@KawdaBoy @piumi_silva @akhilasg @BeardedBrosLK @EkaThamaiMeka ම්ම්ම්ම් ටොස් එක 😂😂 ලෝගා නේද කාසිය උඩ දාන්නේ"</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>1085048422036496384</t>
+  </si>
+  <si>
+    <t>3238809572</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 05:37:57 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Wind_Desika බංගි මොකක් කියලද බැන්නෙ ඔයාට?🤭"</t>
+  </si>
+  <si>
+    <t>1085039082172862465</t>
+  </si>
+  <si>
+    <t>1057807789</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 05:00:50 +0000 2019</t>
+  </si>
+  <si>
+    <t>"I liked a @YouTube video https://t.co/IT1XsY2GCo දඹුල්ලෙන් උඩ ගිය වායු බැලුනයක්"</t>
+  </si>
+  <si>
+    <t>1085039025155534849</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 05:00:37 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@punchi_kella මොකක්?🤨"</t>
+  </si>
+  <si>
+    <t>1085034498172035072</t>
+  </si>
+  <si>
+    <t>488202570</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 04:42:37 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Indrajithlk ඔයා Match එක එන්නේ නෑ මොකක් උනත් 🤪🤪🤪"</t>
+  </si>
+  <si>
+    <t>1085022236866572289</t>
+  </si>
+  <si>
+    <t>1046100586121158656</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:53:54 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@_nxveen @LakisuruS දන්නව මචං. කියල වැඩක් නැතිනිසා කටවහන් ඉන්න ව ඉතින්..."</t>
+  </si>
+  <si>
+    <t>1085019640382644224</t>
+  </si>
+  <si>
+    <t>864255662</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:43:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@KawdaBoy හම්මො.. 😂😂😂😂😂  ඒකත් කමක් නෑ කියමු. කාසි වෙනුවට පැපීව උඩ දාන්න ඔට්ටු නෑ.. 🤭"</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>1085018709096185856</t>
+  </si>
+  <si>
+    <t>976734101595140098</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:39:53 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Wind_Desika හුම්ම්ම් උං උඩයන්න උඩ යන්න අපිටයි අමාරු."</t>
+  </si>
+  <si>
+    <t>1085014749253750784</t>
+  </si>
+  <si>
+    <t>36644221</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:24:09 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Wind_Desika ඔහොම තමයි උඩ තට්ටුව කුලියට දුන්නම"</t>
+  </si>
+  <si>
+    <t>1085011471862501376</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:11:08 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@maalupaan පැපී දැන් #මාතර_අහස_උඩ"</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>1085005198383243264</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 02:46:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ranukad රිදිච්ච උන් ටීම් එකේ නම නැතුවම උඩ පනිනවා බං. බලපං. 🙊🙊🙊"</t>
+  </si>
+  <si>
+    <t>1085004363649744898</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 02:42:53 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@MaheshNegombo මොකක් ගැනද බං කියවන්නේ??"</t>
+  </si>
+  <si>
+    <t>1084968968153120768</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 00:22:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@dkparamee මොකක්?"</t>
+  </si>
+  <si>
+    <t>1084964280808566784</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 00:03:36 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@dudeum_Nethu උඩ පොඩි සිපයියෙක් පෝම් වෙලා ගනන් ගන්න එපා"</t>
+  </si>
+  <si>
+    <t>1084925492715798528</t>
+  </si>
+  <si>
+    <t>62795461</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 21:29:29 +0000 2019</t>
+  </si>
+  <si>
+    <t>"I liked a @YouTube video https://t.co/8dE2HGRA1Y දඹුල්ලෙන් උඩ ගිය වායු බැලුනයක්"</t>
+  </si>
+  <si>
+    <t>1084880992832241664</t>
+  </si>
+  <si>
+    <t>1072765984468021248</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 18:32:39 +0000 2019</t>
+  </si>
+  <si>
+    <t>"TL එකේ උඩ පහල යද්දි බුටක් කාපු කෙල්ලක් ගේ අදෝනාවක් වරදින්නේ නැ 😃"</t>
+  </si>
+  <si>
+    <t>1084867411998760961</t>
+  </si>
+  <si>
+    <t>1007970722021425153</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 17:38:41 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Amashani_Herath මොකක් කිව්වා 😠😠 ඩැෆ්නිට පස්සෙ මගෙ crush එක මෙයා 😂"</t>
+  </si>
+  <si>
+    <t>1084859011764113411</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 17:05:18 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@piumi_silva උඩ එකාද"</t>
+  </si>
+  <si>
+    <t>1084833679623376896</t>
+  </si>
+  <si>
+    <t>2380919498</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 15:24:39 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@iamgayash @IamNalinda @bumrahge @NileeGamage හ්ම්ම් අන්න එයා ගං වතුර වෙලාවේ උඩ තට්ට්ටුවේ ඉන්නේ නැතුව ඔයාලාගේ ආපු කෙනා 🤣🤣🤣"</t>
+  </si>
+  <si>
+    <t>1084830038200143874</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 15:10:10 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sudumameduvada මොකක්"</t>
+  </si>
+  <si>
+    <t>1084828818571849729</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 15:05:20 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@zamudesh මං උඩ😂😂🔫"</t>
+  </si>
+  <si>
+    <t>1084826278962872321</t>
+  </si>
+  <si>
+    <t>1920039648</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 14:55:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NandiyaLive උබේ මොකක් දිගේ😂"</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>1084821677219864577</t>
+  </si>
+  <si>
+    <t>1035880539155095552</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 14:36:57 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NishadiAnuttara මොකක් ද මොකක් ද අැත්තට හෙට😁😁😁"</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>1084816896862519296</t>
+  </si>
+  <si>
+    <t>3523674194</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 14:17:57 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@itsme_sii මොකක් කියලද කිව්වෙ 😂"</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>1084814434105622528</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 14:08:10 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@SLpathumaa අපි ඒමයි මල්ලි. යවනකොට යවනවා හොයාගන්න බැරි වෙන්ඩම උඩ."</t>
+  </si>
+  <si>
+    <t>1084812551525990406</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 14:00:41 +0000 2019</t>
+  </si>
+  <si>
+    <t>"#ආතල්මල්ලි මොකක් පදනම් කරගෙනද මෙ🤔"</t>
+  </si>
+  <si>
+    <t>1084789058260221953</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 12:27:20 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Disapamok හම්සයි ඔයයි තමා උඩ යැව්වෙ"</t>
+  </si>
+  <si>
+    <t>1084786240359063552</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 12:16:08 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@noodles1191 මිදි තිත්ත උඩ පැනල ඉවර උනාමනෙ"</t>
+  </si>
+  <si>
+    <t>1084780359961755649</t>
+  </si>
+  <si>
+    <t>201395218</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 11:52:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@tharu__ @EnThunga @imal_dasanayake මෙතන මොකක් නමුත් ලොකු දෙයක් සිද්ධ වෙලා තියෙනෝ"</t>
+  </si>
+  <si>
+    <t>1084774235640258560</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 11:28:26 +0000 2019</t>
+  </si>
+  <si>
+    <t>"නෑ නෑ මම බෝනික්කියෙක් නෙවෙයි🙊🙊😂  - උඩ යැවීමට ලක් වූ පසු ට්වීට් කරන ලද්දකි-😂😂😂"</t>
+  </si>
+  <si>
+    <t>1084768640648531968</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 11:06:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@IshanSameera8 @NishadiAnuttara මොකක්"</t>
+  </si>
+  <si>
+    <t>1084767811791028230</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 11:02:54 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@hashikalpana @anuwa01 එතකොට සුකියා ඇවිත් ආයෙ උඩ යවනවනෙ"</t>
+  </si>
+  <si>
+    <t>1084758506258030594</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 10:25:56 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@She_is_Nu @nam3chang3d ඒ උනාට අන්න කෙල්ලොන්ට බනිනව කොල්ලො පස්සෙන් ආවට උඩ යන්න එපාලු ඉල්ලුම වැඩි බාල බඩු වලටලු🤦🏼‍♀️🤦🏼‍♀️😂"</t>
+  </si>
+  <si>
+    <t>1084754679127453697</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 10:10:43 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@maalupaan හ්ම්ම්ම් දැක්කා එක දැන් ඩිලිට් නේ.. අඩේ ඔකා එක්ක හුරතල් වෙන්න තරම් මට මොකක් හරි මානසික අවුලක් තියෙනවා වගේ පේනවා ද🤔🤔"</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>1084743230573371392</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 09:25:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Nimsidk මොකක් 😂"</t>
+  </si>
+  <si>
+    <t>1084737530426155008</t>
+  </si>
+  <si>
+    <t>713738846416973824</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 09:02:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ItzmeNeepi මං දන්නව මමත් එක්කෙනෙක් කියල අක්කෙ🤗"</t>
+  </si>
+  <si>
+    <t>1084734839142592512</t>
+  </si>
+  <si>
+    <t>1742620412</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 08:51:53 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ලබ්බට කෝටු ගහපු පඩරැලක් හරි ලස්සනට පේන ගොං හුත්තලා ඉන්නකන්  ලංකාවෙ ඉන්න ඕන ගොං බඩුවක් මේකප් ටිකක් උලාගෙන උඩ යයි...🤢  #නොදකිං #ආතල්මල්ලි"</t>
+  </si>
+  <si>
+    <t>1084726753770131457</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 08:19:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඊයේ මේ පැත්තට එන්න බැරි වුනා. මොකක් හරි ක්‍රිකට් සීන් එකක් වුනාද ? අපේ එවුන් ටුවර් එකක් වත් දිනලද ? මොකක්ද අර ඉමේජ් සීන් එක ? 🤔"</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>1084721976399155200</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 08:00:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@nam3chang3d @DeV_DaZ මොකක් 😭 නෑ අරක හොඳයි 😏"</t>
+  </si>
+  <si>
+    <t>1084721043627884544</t>
+  </si>
+  <si>
+    <t>2991695292</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:57:04 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ @Amashani_Herath උඩ යන්න? කවකටු පෙට්ටි උඩගියේ මොන ලෝකෙද? මොන කාලෙද? 😂😂😂"</t>
+  </si>
+  <si>
+    <t>1084720224962674688</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:53:49 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ @nam3chang3d අම්මෝහ් 😂 බිම වැටුණත් උඩ යන් නෑමයි අයියෙ 😌😂😂😂😂😂😂"</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>1084720074391379968</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:53:13 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Amashani_Herath @nam3chang3d පුටුවට තියලා බැදගන්න අමා.නැත්තන් උඩ ගියොත් මාර අව්ල 😂"</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>1084717190035558401</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:41:45 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Rasthiyaduwa අඩෝ උඩ කොනේ ඉන්නවා දැක්කේ දැන් 😂"</t>
+  </si>
+  <si>
+    <t>1084715693352730624</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:35:48 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අඩෝ අයියේ ඊයේ රත්නපුරේ ත්‍රීවිල් එකක චූටික්කි කියලා ගහලා තිබ්බා.( පහත් ටුවීටයට අදාලව - මන් දැන් උඩ) https://t.co/CQVqrDuruC"</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>1084714017904459776</t>
+  </si>
+  <si>
+    <t>2689996932</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:29:09 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Lasaa_V ඕය ලිස්ට් එකෙන් දෙන්නෙක්ව නම් දන්නව උන් මරු චරිත..."</t>
+  </si>
+  <si>
+    <t>1084712503937040385</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:23:08 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මොකක් හරි පොස්ට් එකක් හදලා හෙනගහනන?  කියලා සෙයා කරාම ඇත්තටම  හෙනවදිනවද?"</t>
+  </si>
+  <si>
+    <t>1084711253161857024</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:18:10 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ExcuzeMiReturn @GloryMinion ෆීල් කරා මොකක්? 🌚"</t>
+  </si>
+  <si>
+    <t>1084705947170336768</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 06:57:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මොකක් හරි හේතුවක් හින්ඳා.. අමුඩේ අමතක වෙලා තිබීයන්  https://t.co/uQ4wyu2nPO"</t>
+  </si>
+  <si>
+    <t>1084695516808544256</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 06:15:38 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ගෙදර වහල උඩ රිලව් දඟලනවා අම්මා: පුතේ රිලව් ඇවිත් මම: දැන් මම මොකද්ද කරන්න ඕන අම්මා: පොඩ්ඩක් ඉස්සරහට ගිහින් බලන්නකො මම: ඇයි හායි කියන්නද"</t>
+  </si>
+  <si>
+    <t>1085475796276445184</t>
+  </si>
+  <si>
+    <t>4216937062</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 09:56:11 +0000 2019</t>
+  </si>
+  <si>
+    <t>"සමහර එවුන් ට්‍රැවල් කිය කියා බොරුවට දඟල දඟල යන්නේ මොකක් හරි වඩිග පටුනක් නටලා ඇඳන් යන එකයි කන්න අරන් යන එකයි එතනම කරන එකක් කරලා දාලා එන්න තමා..  අනේ හු* උන්ගේ ට්‍රැවල් 😎🖕 https://t.co/fbRF2ycA4B"</t>
+  </si>
+  <si>
+    <t>1085434623331463168</t>
+  </si>
+  <si>
+    <t>100980318</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 07:12:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@kazZtr_ @DJSlash9 ඔයිල් නැත.. ඔය එකී මෙකී සියල්ලම පරීක්ෂා කර බැලුව බං. කොරන්නම දෙයක් නැති තැන තමා පටවන් අවෙ.. ඒකයි මට හිතුනෙ එන්ජිමට කෙලවිලාම ඇති කියල. අනික ඔය කියන වෙලාවෙ මම අධික වේගයෙන් රිය ධවනය කලා.. සමහර විට එන්ජිමට  නවතින්න ඕනෙ උනත් නවතින්න නැතිව ඇති.. තියන සබ්බ සකලමනාවම ඇඹරිලා හිටිනකම්ම."</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>1085372366690181122</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 03:05:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@nthathsaranii කෙල්ල බැදලා ටික කාලෙකින් මැරෙනවා මොකක් හරි වෙලා. කොල්ලගෙ අම්මයි තාත්තයි කොල්ලට ආයෙ බදින්න කියනවනෙ?නොකියා ඉන්නෑනෙ.මං මෙ වෙන කතාවක් ගත්තෙ.මොනා උනත් තමන්ගෙ අම්මයි තාත්තයි තරම් අපිට ආදරෙ කවුරුවත් නෑනෙ."</t>
+  </si>
+  <si>
+    <t>1085251327972728833</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 19:04:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@iamharshana1 @iamgayash එක්කෙනෙකුට බැයිද තුන් හතර දෙනෙක්ව තියා ගන්න. පල්ලෙහා ගෙදර අක්කයි තව නම්කි කෙනෙකුයි වෙන්ඩ කෙනයි.  මං උඩ දෙන්නට බලාපොරොත්තු දීලත් නැත්තේ අනවශ්‍යය සම්බන්ධකම් පවත්වන්නෙත් නැත්තේ තුන්වැනියා නිසා. හැබැයි එහෙම පුළුවන්නම් ගයාශ් අයියවත් ගෙට දාගන්නවා 😍😍😍😍"</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>1085235644266352642</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 18:01:54 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@tharu__ මම දවසක් ඉන්දියන් එකෙක් එක්ක වලියක් දා ගත්තා. අන්තිමට ඌ කිව්වා මොකක් හරි එකකට Wrong English කියලා. මම කිව්වා මගේ තාත්තා සුද්දෙක් නෙවෙයි උඹේ වගේ කියලා 😃😃"</t>
+  </si>
+  <si>
+    <t>1085230908339187712</t>
+  </si>
+  <si>
+    <t>965954850092535811</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 17:43:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කම්මැලි වෙයන් පොලවේ ඉදන් අහසට පාවෙන්න  උබලා උඩ නිසා තිස්තුන්කෝටියක්ම දැන් පොලවේ ඉස්සර රොටිය 5යි දැන් 25යි ඉස්කෝලේ කැන්ටිමේ ඇමතුම ඉස්සුවම 13යි ඉස්සර දැන් එන ඒවා නොමිලේ තාක්ෂනය දියුණුයි බඩට වෙන ආක්‍රමණ තියුණුයි අපි කන්න මැරෙන්නේ අකාලේ මැරෙන්න අපි යන්න හදන්නෙම අපායේ ඇරෙන්න …"</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>1085189686740410368</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 14:59:17 +0000 2019</t>
+  </si>
+  <si>
+    <t>"බැදීමේ නම මොකක් වුනත් වැරැද්දක් වෙන්න යද්දි ඕක ඔයාට ගැළපෙන් නෑ හරියන් නෑ ඕක කරන්න කලින් හිතන්න කියලා මට කියන්නේ බොහොම සුළුතරයක්..😊  එහෙම කෙනෙක් කියන දෙයක් මම හදවතින්ම අහනවා💛  මොකද බහුතරය කැමති වරදිනවට  බලන් ඉන්නේ තව කෙනෙක්ට ඇගිල්ල දික් කරන්න, ලැජ්ජා කරන්න  ඒ තමා මනුස්ස ගතිය"</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>1085130828273709056</t>
+  </si>
+  <si>
+    <t>983394040790925312</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 11:05:24 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අපේ රට දැන් එන්න එන්නම දුප්පත් වෙනව.දුගි ජනතාව සල්ලි කාරයගේ වහලුන් කරගන මේ රටේ පාලකයො මොනවද කරන්නෙ නිකන් උඩ බලාගෙන ඉන්නව.මැති අැමති වරැන්ට තමන්ගෙ පැත්ත දිනුවට පස්සෙ ජනතාවට හෙන ගැහුවත් කමන්නැ කියල වැඩ කරන්නෙ.දුසිත පාලකයන්ට එරෙහිව ජනතාව පෙල ගැහුනු දවසට පාලකයන්ට වස බොන්න වෙන්නෙ එදාට"</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>1085083613367029760</t>
+  </si>
+  <si>
+    <t>924978151</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:57:47 +0000 2019</t>
+  </si>
+  <si>
+    <t>"වක්කඩ ලඟ දිය වැටෙන තාලයට තිත්ත පැටව් උඩ පැන නැටුවා වැස්ස වහින්නට ඉස්සර අහසේ වලාකුලෙන් විදුලිය කෙටුවා කිව්වට වස් නැත නිල් නිල් පාටින් කටරොළු මල් වැට වට කෙරුවා තුන් දවසක් අමනාපෙන් සිටි කලු නෝක්කාඩු... https://t.co/HvHxp2bxE5"</t>
+  </si>
+  <si>
+    <t>1085047387284885506</t>
+  </si>
+  <si>
+    <t>955051442183684096</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 05:33:50 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ෆේස්බුක්වලට වෙලාතියෙන්නෙ මේක තමයි. මිනිස්සුන්ව සයිකලොජිකලි ඉන්ෆ්ලුවන්ස් කරල අල්ලගන්න පුලුවන් කියල තේරුනු ගමන් ඒව එක්ස්ප්ලොයිට් කරන එක්ස්පර්ට්ල ටිකක් හැදුන. උන් දන්නව මිනිස්සුන්ගෙ ක්ලික් වෙන තැන්.   අන්තිමේ ජෙනුයින් මොකක්ද, ඉන්ෆ්ලුවන්ස් කරන්නෙ මොකක්ද කියල හිතාගන්න බැරි තැනටම ආව. https://t.co/SB3Jy6MzUA"</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>1085022538604851200</t>
+  </si>
+  <si>
+    <t>877338855413694464</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:55:06 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කොස් ගහේ උඩ අත්තෙ  පොඩි කුරුලු කූඩුවක්  කිචි බිචිය ඇහෙනවා  නිරතුරුව ජනේලෙන්  අම්මා එයි පොඩි පැටියො  අඬන්නට එපා දැන්  අද  කෑම දෙන්න නැහැ  මාත් බඩගින්නෙදැන් https://t.co/b2kc0kyzII"</t>
+  </si>
+  <si>
+    <t>1085015983452958720</t>
+  </si>
+  <si>
+    <t>931662782264696838</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:29:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>"රට බෙදෙන්නත් පුලුවන්.. ආණ්ඩුවේ තීරක බලවේගය අපි.. අපි ඒක පෙන්නන්නෙ නෑ.. පෙන්න ගත්තොත් ඒක ප්‍රශ්නයක්.. ඒක ආණ්ඩුවත් දන්නව.. - ඒබ්‍රහම් සුමන් - https://t.co/0XHlhPLryx"</t>
+  </si>
+  <si>
+    <t>1085001464202911744</t>
+  </si>
+  <si>
+    <t>344148748</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 02:31:22 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අස්ලි ඩෙරික්ගේ ඔළුවෙන් කෙස් ගලවගන්නේ මොකක් කරන්නද?  අද රාත්‍රී 9:25 ට හිරු TV බලන්න | තාමත් ආදරේ නැත්නම් පසුගිය කොටස් සියල්ලම හිරු Tube ඔස්සේ නරඹන්න - https://t.co/Vo0ZPC2lnr Like US - @Hiru TV Follow US - https://t.co/FuhHOGzhog  #ahasmaliga... https://t.co/KFpVM4GHFe"</t>
+  </si>
+  <si>
+    <t>1085000979903324160</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 02:29:26 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ගිනි පොලියා හැම ඇත්තක්ම කිවුවම කැලුම්ට මොකක් වෙයිද ?  අද රාත්‍රී 8:30 ට හිරු TV බලන්න | අහස් මාලිගා පසුගිය කොටස් සියල්ලම නරඹන්න - https://t.co/wo9oMHV9w5 Like US - Hiru TV - Sri Lanka's Number One Television Channel Follow... https://t.co/JvhJvsj62Y"</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>1084880822941962246</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 18:31:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>""රහත් හිමිවරුන්", Charitha Rakshitha Attalage ගෙ අලුත්ම වැඩේ 😍  ලංකාවෙ නහයෙන් අඬපු අඳෝනා, සංගීතමය  ද නොවුණු කලාවක් ද නොවුණු මොකක් දෝ එකේ අවසානය සනිටුහන් කරපු සංගීත අධ්‍යක්ෂකවරුන්ගෙන්  කෙනෙක් තම යි Charitha Rakshitha Attalage .... https://t.co/KFu1fAGGYc"</t>
+  </si>
+  <si>
+    <t>1084852886922653696</t>
+  </si>
+  <si>
+    <t>2911831267</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 16:40:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කුඹ ගසක් උඩ නැවතිලා සිනා තලමින් සඳේ ඇයි සරදම්.. බලන් කැඩපත සොඳුරියේ පාට වත්සුනු දෙකොපුලෙන් පිසදා..  පෙරුම් පුරමින් හමුවෙලා උනුන් රහසින් බැන්ද ආදර පෙම් බලන් කැඩපත සොඳුරියේ කුමන අරුමද නර කෙසක් පැහිලා.. https://t.co/sDsKvgzdaB"</t>
+  </si>
+  <si>
+    <t>1084809484235563008</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 13:48:30 +0000 2019</t>
+  </si>
+  <si>
+    <t>"#TCLSL වල පැපීගේ ටීම් එකයි පාරමීගේ ටීම් එකයි මැච් එකක් වැටිලා, පාරමී කාසිය උඩ දාලා නෝනද පොල්ලද කියලා පැපීගෙන් ඇහුවොත් පැපී මොකක් ඉල්ලයිද? #Loගොන්Answers #RathumakaraFM"</t>
+  </si>
+  <si>
+    <t>1084690434650226688</t>
+  </si>
+  <si>
+    <t>2373363534</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 05:55:26 +0000 2019</t>
+  </si>
+  <si>
+    <t>"🐢 ඉබ්බා vs කොක්කු අලුත් එක  + මෙ දැන් උඩ යන ගමන් ඉන්නෙ .. කොල්ලො කුරුට්ටෝ හු.. කිව්වොත් කට අරින්න එපා .. මතකනෙ උම්බෙ සියාට උන දේ.. - හරි බං  😒🙏"</t>
   </si>
 </sst>
 </file>
@@ -6523,10 +7615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F470"/>
+  <dimension ref="A1:F568"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A543" workbookViewId="0">
+      <selection activeCell="F568" sqref="F568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15937,6 +17029,1966 @@
         <v>50</v>
       </c>
     </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A471" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B471" s="6" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C471" s="6" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D471" s="6" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E471" s="6" t="s">
+        <v>2015</v>
+      </c>
+      <c r="F471" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A472" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="B472" s="6" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C472" s="6" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D472" s="6" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E472" s="6" t="s">
+        <v>2018</v>
+      </c>
+      <c r="F472" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A473" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="B473" s="6" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C473" s="6" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D473" s="6" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E473" s="6" t="s">
+        <v>2022</v>
+      </c>
+      <c r="F473" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A474" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B474" s="6" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C474" s="6" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D474" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="E474" s="6" t="s">
+        <v>2026</v>
+      </c>
+      <c r="F474" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A475" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="B475" s="6" t="s">
+        <v>2027</v>
+      </c>
+      <c r="C475" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D475" s="6" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E475" s="6" t="s">
+        <v>2029</v>
+      </c>
+      <c r="F475" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A476" s="6" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B476" s="6" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C476" s="6" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D476" s="6" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E476" s="6" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F476" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A477" s="6" t="s">
+        <v>2035</v>
+      </c>
+      <c r="B477" s="6" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C477" s="6" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D477" s="6" t="s">
+        <v>2038</v>
+      </c>
+      <c r="E477" s="6" t="s">
+        <v>2039</v>
+      </c>
+      <c r="F477" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A478" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B478" s="6" t="s">
+        <v>2040</v>
+      </c>
+      <c r="C478" s="6" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D478" s="6" t="s">
+        <v>2041</v>
+      </c>
+      <c r="E478" s="6" t="s">
+        <v>2042</v>
+      </c>
+      <c r="F478" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A479" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="B479" s="6" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C479" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="D479" s="6" t="s">
+        <v>2044</v>
+      </c>
+      <c r="E479" s="6" t="s">
+        <v>2045</v>
+      </c>
+      <c r="F479" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A480" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B480" s="6" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C480" s="6" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D480" s="6" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E480" s="6" t="s">
+        <v>2049</v>
+      </c>
+      <c r="F480" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A481" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B481" s="6" t="s">
+        <v>2050</v>
+      </c>
+      <c r="C481" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="D481" s="6" t="s">
+        <v>2051</v>
+      </c>
+      <c r="E481" s="6" t="s">
+        <v>2052</v>
+      </c>
+      <c r="F481" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A482" s="6" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B482" s="6" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C482" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D482" s="6" t="s">
+        <v>2055</v>
+      </c>
+      <c r="E482" s="6" t="s">
+        <v>2056</v>
+      </c>
+      <c r="F482" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A483" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="B483" s="6" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C483" s="6" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D483" s="6" t="s">
+        <v>2058</v>
+      </c>
+      <c r="E483" s="6" t="s">
+        <v>2059</v>
+      </c>
+      <c r="F483" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A484" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="B484" s="6" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C484" s="6" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D484" s="6" t="s">
+        <v>2061</v>
+      </c>
+      <c r="E484" s="6" t="s">
+        <v>2062</v>
+      </c>
+      <c r="F484" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A485" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="B485" s="6" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C485" s="6" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D485" s="6" t="s">
+        <v>2065</v>
+      </c>
+      <c r="E485" s="6" t="s">
+        <v>2066</v>
+      </c>
+      <c r="F485" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A486" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B486" s="6" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C486" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="D486" s="6" t="s">
+        <v>2068</v>
+      </c>
+      <c r="E486" s="6" t="s">
+        <v>2069</v>
+      </c>
+      <c r="F486" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A487" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B487" s="6" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C487" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D487" s="6" t="s">
+        <v>2071</v>
+      </c>
+      <c r="E487" s="6" t="s">
+        <v>2072</v>
+      </c>
+      <c r="F487" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A488" s="6" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B488" s="6" t="s">
+        <v>2074</v>
+      </c>
+      <c r="C488" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="D488" s="6" t="s">
+        <v>2075</v>
+      </c>
+      <c r="E488" s="6" t="s">
+        <v>2076</v>
+      </c>
+      <c r="F488" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A489" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B489" s="6" t="s">
+        <v>2077</v>
+      </c>
+      <c r="C489" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D489" s="6" t="s">
+        <v>2078</v>
+      </c>
+      <c r="E489" s="6" t="s">
+        <v>2079</v>
+      </c>
+      <c r="F489" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A490" s="6" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B490" s="6" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C490" s="6" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D490" s="6" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E490" s="6" t="s">
+        <v>2084</v>
+      </c>
+      <c r="F490" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A491" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B491" s="6" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C491" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D491" s="6" t="s">
+        <v>2086</v>
+      </c>
+      <c r="E491" s="6" t="s">
+        <v>2087</v>
+      </c>
+      <c r="F491" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A492" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="B492" s="6" t="s">
+        <v>2088</v>
+      </c>
+      <c r="C492" s="6" t="s">
+        <v>2089</v>
+      </c>
+      <c r="D492" s="6" t="s">
+        <v>2090</v>
+      </c>
+      <c r="E492" s="6" t="s">
+        <v>2091</v>
+      </c>
+      <c r="F492" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A493" s="6" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B493" s="6" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C493" s="6" t="s">
+        <v>2094</v>
+      </c>
+      <c r="D493" s="6" t="s">
+        <v>2095</v>
+      </c>
+      <c r="E493" s="6" t="s">
+        <v>2096</v>
+      </c>
+      <c r="F493" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A494" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="B494" s="6" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C494" s="6" t="s">
+        <v>2098</v>
+      </c>
+      <c r="D494" s="6" t="s">
+        <v>2099</v>
+      </c>
+      <c r="E494" s="6" t="s">
+        <v>2100</v>
+      </c>
+      <c r="F494" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A495" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B495" s="6" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C495" s="6" t="s">
+        <v>2102</v>
+      </c>
+      <c r="D495" s="6" t="s">
+        <v>2103</v>
+      </c>
+      <c r="E495" s="6" t="s">
+        <v>2104</v>
+      </c>
+      <c r="F495" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A496" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="B496" s="6" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C496" s="6" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D496" s="6" t="s">
+        <v>2107</v>
+      </c>
+      <c r="E496" s="6" t="s">
+        <v>2108</v>
+      </c>
+      <c r="F496" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A497" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="B497" s="6" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C497" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="D497" s="6" t="s">
+        <v>2110</v>
+      </c>
+      <c r="E497" s="6" t="s">
+        <v>2111</v>
+      </c>
+      <c r="F497" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A498" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B498" s="6" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C498" s="6" t="s">
+        <v>2113</v>
+      </c>
+      <c r="D498" s="6" t="s">
+        <v>2114</v>
+      </c>
+      <c r="E498" s="6" t="s">
+        <v>2115</v>
+      </c>
+      <c r="F498" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A499" s="6" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B499" s="6" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C499" s="6" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D499" s="6" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E499" s="6" t="s">
+        <v>2119</v>
+      </c>
+      <c r="F499" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A500" s="6" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B500" s="6" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C500" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D500" s="6" t="s">
+        <v>2122</v>
+      </c>
+      <c r="E500" s="11" t="s">
+        <v>2123</v>
+      </c>
+      <c r="F500" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A501" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="B501" s="6" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C501" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D501" s="6" t="s">
+        <v>2125</v>
+      </c>
+      <c r="E501" s="11" t="s">
+        <v>2126</v>
+      </c>
+      <c r="F501" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A502" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B502" s="6" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C502" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D502" s="6" t="s">
+        <v>2128</v>
+      </c>
+      <c r="E502" s="6" t="s">
+        <v>2129</v>
+      </c>
+      <c r="F502" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A503" s="6" t="s">
+        <v>2130</v>
+      </c>
+      <c r="B503" s="6" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C503" s="6" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D503" s="6" t="s">
+        <v>2133</v>
+      </c>
+      <c r="E503" s="6" t="s">
+        <v>2134</v>
+      </c>
+      <c r="F503" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A504" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B504" s="6" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C504" s="6" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D504" s="6" t="s">
+        <v>2137</v>
+      </c>
+      <c r="E504" s="6" t="s">
+        <v>2138</v>
+      </c>
+      <c r="F504" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A505" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B505" s="6" t="s">
+        <v>2139</v>
+      </c>
+      <c r="C505" s="6" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D505" s="6" t="s">
+        <v>2140</v>
+      </c>
+      <c r="E505" s="6" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F505" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A506" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B506" s="6" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C506" s="6" t="s">
+        <v>2143</v>
+      </c>
+      <c r="D506" s="6" t="s">
+        <v>2144</v>
+      </c>
+      <c r="E506" s="6" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F506" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A507" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B507" s="6" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C507" s="6" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D507" s="6" t="s">
+        <v>2148</v>
+      </c>
+      <c r="E507" s="6" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F507" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A508" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B508" s="6" t="s">
+        <v>2150</v>
+      </c>
+      <c r="C508" s="6" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D508" s="6" t="s">
+        <v>2152</v>
+      </c>
+      <c r="E508" s="6" t="s">
+        <v>2153</v>
+      </c>
+      <c r="F508" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A509" s="6" t="s">
+        <v>2154</v>
+      </c>
+      <c r="B509" s="6" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C509" s="6" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D509" s="6" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E509" s="6" t="s">
+        <v>2158</v>
+      </c>
+      <c r="F509" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A510" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="B510" s="6" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C510" s="6" t="s">
+        <v>2160</v>
+      </c>
+      <c r="D510" s="6" t="s">
+        <v>2161</v>
+      </c>
+      <c r="E510" s="6" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F510" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A511" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B511" s="6" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C511" s="6" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D511" s="6" t="s">
+        <v>2164</v>
+      </c>
+      <c r="E511" s="6" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F511" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A512" s="6" t="s">
+        <v>2166</v>
+      </c>
+      <c r="B512" s="6" t="s">
+        <v>2167</v>
+      </c>
+      <c r="C512" s="6" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D512" s="6" t="s">
+        <v>2168</v>
+      </c>
+      <c r="E512" s="6" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F512" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A513" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="B513" s="6" t="s">
+        <v>2170</v>
+      </c>
+      <c r="C513" s="6" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D513" s="6" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E513" s="6" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F513" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A514" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="B514" s="6" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C514" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D514" s="6" t="s">
+        <v>2174</v>
+      </c>
+      <c r="E514" s="6" t="s">
+        <v>2175</v>
+      </c>
+      <c r="F514" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A515" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="B515" s="6" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C515" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D515" s="6" t="s">
+        <v>2177</v>
+      </c>
+      <c r="E515" s="6" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F515" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A516" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B516" s="6" t="s">
+        <v>2179</v>
+      </c>
+      <c r="C516" s="6" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D516" s="6" t="s">
+        <v>2181</v>
+      </c>
+      <c r="E516" s="6" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F516" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A517" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B517" s="6" t="s">
+        <v>2183</v>
+      </c>
+      <c r="C517" s="6" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D517" s="6" t="s">
+        <v>2185</v>
+      </c>
+      <c r="E517" s="6" t="s">
+        <v>2186</v>
+      </c>
+      <c r="F517" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A518" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="B518" s="6" t="s">
+        <v>2187</v>
+      </c>
+      <c r="C518" s="6" t="s">
+        <v>2188</v>
+      </c>
+      <c r="D518" s="6" t="s">
+        <v>2189</v>
+      </c>
+      <c r="E518" s="11" t="s">
+        <v>2190</v>
+      </c>
+      <c r="F518" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A519" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="B519" s="6" t="s">
+        <v>2191</v>
+      </c>
+      <c r="C519" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D519" s="6" t="s">
+        <v>2192</v>
+      </c>
+      <c r="E519" s="6" t="s">
+        <v>2193</v>
+      </c>
+      <c r="F519" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A520" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B520" s="6" t="s">
+        <v>2194</v>
+      </c>
+      <c r="C520" s="6" t="s">
+        <v>2195</v>
+      </c>
+      <c r="D520" s="6" t="s">
+        <v>2196</v>
+      </c>
+      <c r="E520" s="6" t="s">
+        <v>2197</v>
+      </c>
+      <c r="F520" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A521" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="B521" s="6" t="s">
+        <v>2198</v>
+      </c>
+      <c r="C521" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D521" s="6" t="s">
+        <v>2199</v>
+      </c>
+      <c r="E521" s="6" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F521" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A522" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="B522" s="6" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C522" s="6" t="s">
+        <v>2132</v>
+      </c>
+      <c r="D522" s="6" t="s">
+        <v>2202</v>
+      </c>
+      <c r="E522" s="6" t="s">
+        <v>2203</v>
+      </c>
+      <c r="F522" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A523" s="6" t="s">
+        <v>555</v>
+      </c>
+      <c r="B523" s="6" t="s">
+        <v>2204</v>
+      </c>
+      <c r="C523" s="6" t="s">
+        <v>2205</v>
+      </c>
+      <c r="D523" s="6" t="s">
+        <v>2206</v>
+      </c>
+      <c r="E523" s="6" t="s">
+        <v>2207</v>
+      </c>
+      <c r="F523" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A524" s="6" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B524" s="6" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C524" s="6" t="s">
+        <v>2210</v>
+      </c>
+      <c r="D524" s="6" t="s">
+        <v>2211</v>
+      </c>
+      <c r="E524" s="6" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F524" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A525" s="6" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B525" s="6" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C525" s="6" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D525" s="6" t="s">
+        <v>2216</v>
+      </c>
+      <c r="E525" s="6" t="s">
+        <v>2217</v>
+      </c>
+      <c r="F525" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A526" s="6" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B526" s="6" t="s">
+        <v>2219</v>
+      </c>
+      <c r="C526" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D526" s="6" t="s">
+        <v>2220</v>
+      </c>
+      <c r="E526" s="6" t="s">
+        <v>2221</v>
+      </c>
+      <c r="F526" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A527" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="B527" s="6" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C527" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D527" s="6" t="s">
+        <v>2223</v>
+      </c>
+      <c r="E527" s="6" t="s">
+        <v>2224</v>
+      </c>
+      <c r="F527" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A528" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="B528" s="6" t="s">
+        <v>2225</v>
+      </c>
+      <c r="C528" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D528" s="6" t="s">
+        <v>2226</v>
+      </c>
+      <c r="E528" s="6" t="s">
+        <v>2227</v>
+      </c>
+      <c r="F528" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A529" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="B529" s="6" t="s">
+        <v>2228</v>
+      </c>
+      <c r="C529" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D529" s="6" t="s">
+        <v>2229</v>
+      </c>
+      <c r="E529" s="6" t="s">
+        <v>2230</v>
+      </c>
+      <c r="F529" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A530" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="B530" s="6" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C530" s="6" t="s">
+        <v>2232</v>
+      </c>
+      <c r="D530" s="6" t="s">
+        <v>2233</v>
+      </c>
+      <c r="E530" s="6" t="s">
+        <v>2234</v>
+      </c>
+      <c r="F530" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A531" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="B531" s="6" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C531" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D531" s="6" t="s">
+        <v>2236</v>
+      </c>
+      <c r="E531" s="6" t="s">
+        <v>2237</v>
+      </c>
+      <c r="F531" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A532" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="B532" s="6" t="s">
+        <v>2238</v>
+      </c>
+      <c r="C532" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="D532" s="6" t="s">
+        <v>2239</v>
+      </c>
+      <c r="E532" s="6" t="s">
+        <v>2240</v>
+      </c>
+      <c r="F532" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A533" s="6" t="s">
+        <v>588</v>
+      </c>
+      <c r="B533" s="6" t="s">
+        <v>2241</v>
+      </c>
+      <c r="C533" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D533" s="6" t="s">
+        <v>2242</v>
+      </c>
+      <c r="E533" s="6" t="s">
+        <v>2243</v>
+      </c>
+      <c r="F533" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A534" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B534" s="6" t="s">
+        <v>2244</v>
+      </c>
+      <c r="C534" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D534" s="6" t="s">
+        <v>2245</v>
+      </c>
+      <c r="E534" s="6" t="s">
+        <v>2246</v>
+      </c>
+      <c r="F534" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A535" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="B535" s="6" t="s">
+        <v>2247</v>
+      </c>
+      <c r="C535" s="6" t="s">
+        <v>2195</v>
+      </c>
+      <c r="D535" s="6" t="s">
+        <v>2248</v>
+      </c>
+      <c r="E535" s="6" t="s">
+        <v>2249</v>
+      </c>
+      <c r="F535" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A536" s="6" t="s">
+        <v>2250</v>
+      </c>
+      <c r="B536" s="6" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C536" s="6" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D536" s="6" t="s">
+        <v>2252</v>
+      </c>
+      <c r="E536" s="6" t="s">
+        <v>2253</v>
+      </c>
+      <c r="F536" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A537" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="B537" s="6" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C537" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D537" s="6" t="s">
+        <v>2256</v>
+      </c>
+      <c r="E537" s="6" t="s">
+        <v>2257</v>
+      </c>
+      <c r="F537" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A538" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B538" s="6" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C538" s="6" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D538" s="6" t="s">
+        <v>2260</v>
+      </c>
+      <c r="E538" s="11" t="s">
+        <v>2261</v>
+      </c>
+      <c r="F538" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A539" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="B539" s="6" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C539" s="6" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D539" s="6" t="s">
+        <v>2263</v>
+      </c>
+      <c r="E539" s="6" t="s">
+        <v>2264</v>
+      </c>
+      <c r="F539" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A540" s="6" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B540" s="6" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C540" s="6" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D540" s="6" t="s">
+        <v>2267</v>
+      </c>
+      <c r="E540" s="6" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F540" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A541" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B541" s="6" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C541" s="6" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D541" s="6" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E541" s="6" t="s">
+        <v>2272</v>
+      </c>
+      <c r="F541" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A542" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="B542" s="6" t="s">
+        <v>2273</v>
+      </c>
+      <c r="C542" s="6" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D542" s="6" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E542" s="6" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F542" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A543" s="6" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B543" s="6" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C543" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="D543" s="6" t="s">
+        <v>2278</v>
+      </c>
+      <c r="E543" s="6" t="s">
+        <v>2279</v>
+      </c>
+      <c r="F543" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A544" s="6" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B544" s="6" t="s">
+        <v>2281</v>
+      </c>
+      <c r="C544" s="6" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D544" s="6" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E544" s="6" t="s">
+        <v>2283</v>
+      </c>
+      <c r="F544" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A545" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="B545" s="6" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C545" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D545" s="6" t="s">
+        <v>2285</v>
+      </c>
+      <c r="E545" s="6" t="s">
+        <v>2286</v>
+      </c>
+      <c r="F545" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A546" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="B546" s="6" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C546" s="6" t="s">
+        <v>2289</v>
+      </c>
+      <c r="D546" s="6" t="s">
+        <v>2290</v>
+      </c>
+      <c r="E546" s="6" t="s">
+        <v>2291</v>
+      </c>
+      <c r="F546" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A547" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B547" s="6" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C547" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D547" s="6" t="s">
+        <v>2293</v>
+      </c>
+      <c r="E547" s="6" t="s">
+        <v>2294</v>
+      </c>
+      <c r="F547" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A548" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="B548" s="6" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C548" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D548" s="6" t="s">
+        <v>2296</v>
+      </c>
+      <c r="E548" s="6" t="s">
+        <v>2297</v>
+      </c>
+      <c r="F548" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A549" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="B549" s="6" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C549" s="6" t="s">
+        <v>873</v>
+      </c>
+      <c r="D549" s="6" t="s">
+        <v>2299</v>
+      </c>
+      <c r="E549" s="6" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F549" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A550" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="B550" s="6" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C550" s="6" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D550" s="6" t="s">
+        <v>2302</v>
+      </c>
+      <c r="E550" s="6" t="s">
+        <v>2303</v>
+      </c>
+      <c r="F550" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A551" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="B551" s="6" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C551" s="6" t="s">
+        <v>2305</v>
+      </c>
+      <c r="D551" s="6" t="s">
+        <v>2306</v>
+      </c>
+      <c r="E551" s="6" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F551" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A552" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B552" s="6" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C552" s="6" t="s">
+        <v>2309</v>
+      </c>
+      <c r="D552" s="6" t="s">
+        <v>2310</v>
+      </c>
+      <c r="E552" s="6" t="s">
+        <v>2311</v>
+      </c>
+      <c r="F552" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A553" s="6" t="s">
+        <v>2312</v>
+      </c>
+      <c r="B553" s="6" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C553" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D553" s="6" t="s">
+        <v>2314</v>
+      </c>
+      <c r="E553" s="6" t="s">
+        <v>2315</v>
+      </c>
+      <c r="F553" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A554" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B554" s="6" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C554" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D554" s="6" t="s">
+        <v>2317</v>
+      </c>
+      <c r="E554" s="6" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F554" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A555" s="6" t="s">
+        <v>2319</v>
+      </c>
+      <c r="B555" s="6" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C555" s="6" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D555" s="6" t="s">
+        <v>2321</v>
+      </c>
+      <c r="E555" s="6" t="s">
+        <v>2322</v>
+      </c>
+      <c r="F555" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A556" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="B556" s="6" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C556" s="6" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D556" s="6" t="s">
+        <v>2325</v>
+      </c>
+      <c r="E556" s="6" t="s">
+        <v>2326</v>
+      </c>
+      <c r="F556" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A557" s="6" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B557" s="6" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C557" s="6" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D557" s="6" t="s">
+        <v>2329</v>
+      </c>
+      <c r="E557" s="6" t="s">
+        <v>2330</v>
+      </c>
+      <c r="F557" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A558" s="6" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B558" s="6" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C558" s="6" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D558" s="6" t="s">
+        <v>2334</v>
+      </c>
+      <c r="E558" s="6" t="s">
+        <v>2335</v>
+      </c>
+      <c r="F558" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A559" s="6" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B559" s="6" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C559" s="6" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D559" s="6" t="s">
+        <v>2339</v>
+      </c>
+      <c r="E559" s="6" t="s">
+        <v>2340</v>
+      </c>
+      <c r="F559" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A560" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="B560" s="6" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C560" s="6" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D560" s="6" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E560" s="6" t="s">
+        <v>2344</v>
+      </c>
+      <c r="F560" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A561" s="6" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B561" s="6" t="s">
+        <v>2346</v>
+      </c>
+      <c r="C561" s="6" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D561" s="6" t="s">
+        <v>2348</v>
+      </c>
+      <c r="E561" s="6" t="s">
+        <v>2349</v>
+      </c>
+      <c r="F561" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A562" s="6" t="s">
+        <v>674</v>
+      </c>
+      <c r="B562" s="6" t="s">
+        <v>2350</v>
+      </c>
+      <c r="C562" s="6" t="s">
+        <v>2351</v>
+      </c>
+      <c r="D562" s="6" t="s">
+        <v>2352</v>
+      </c>
+      <c r="E562" s="11" t="s">
+        <v>2353</v>
+      </c>
+      <c r="F562" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A563" s="6" t="s">
+        <v>679</v>
+      </c>
+      <c r="B563" s="6" t="s">
+        <v>2354</v>
+      </c>
+      <c r="C563" s="6" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D563" s="6" t="s">
+        <v>2356</v>
+      </c>
+      <c r="E563" s="6" t="s">
+        <v>2357</v>
+      </c>
+      <c r="F563" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A564" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="B564" s="6" t="s">
+        <v>2358</v>
+      </c>
+      <c r="C564" s="6" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D564" s="6" t="s">
+        <v>2359</v>
+      </c>
+      <c r="E564" s="6" t="s">
+        <v>2360</v>
+      </c>
+      <c r="F564" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A565" s="6" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B565" s="6" t="s">
+        <v>2362</v>
+      </c>
+      <c r="C565" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D565" s="6" t="s">
+        <v>2363</v>
+      </c>
+      <c r="E565" s="6" t="s">
+        <v>2364</v>
+      </c>
+      <c r="F565" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A566" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="B566" s="6" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C566" s="6" t="s">
+        <v>2366</v>
+      </c>
+      <c r="D566" s="6" t="s">
+        <v>2367</v>
+      </c>
+      <c r="E566" s="6" t="s">
+        <v>2368</v>
+      </c>
+      <c r="F566" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A567" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="B567" s="6" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C567" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D567" s="6" t="s">
+        <v>2370</v>
+      </c>
+      <c r="E567" s="6" t="s">
+        <v>2371</v>
+      </c>
+      <c r="F567" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A568" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="B568" s="6" t="s">
+        <v>2372</v>
+      </c>
+      <c r="C568" s="6" t="s">
+        <v>2373</v>
+      </c>
+      <c r="D568" s="6" t="s">
+        <v>2374</v>
+      </c>
+      <c r="E568" s="6" t="s">
+        <v>2375</v>
+      </c>
+      <c r="F568" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">

</xml_diff>

<commit_message>
add more 100 tweets
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3408" uniqueCount="2376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="2702">
   <si>
     <t>instance_id</t>
   </si>
@@ -7171,6 +7171,984 @@
   </si>
   <si>
     <t>"🐢 ඉබ්බා vs කොක්කු අලුත් එක  + මෙ දැන් උඩ යන ගමන් ඉන්නෙ .. කොල්ලො කුරුට්ටෝ හු.. කිව්වොත් කට අරින්න එපා .. මතකනෙ උම්බෙ සියාට උන දේ.. - හරි බං  😒🙏"</t>
+  </si>
+  <si>
+    <t>1085548159013507073</t>
+  </si>
+  <si>
+    <t>984824053398515712</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 14:43:44 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ හහ් හා අපි ගාවත් photos තියෙනව දාන්නද ???😂😂"</t>
+  </si>
+  <si>
+    <t>1085545993632919552</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 14:35:08 +0000 2019</t>
+  </si>
+  <si>
+    <t>"'කුළියාපිටියේ...කිරි පිටි' කා බී හැදුන වැඩුන....'හරකෙක්'  කොහොම ද....දිග😅 https://t.co/CxCDfBUmXY"</t>
+  </si>
+  <si>
+    <t>1085543031393071105</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 14:23:21 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DeV_DaZ අහිංසක මෝංගල් පාටක් තියෙනව තමානේ 😂😂"</t>
+  </si>
+  <si>
+    <t>1085519264386244609</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 12:48:55 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sanju_Live @Dilan_Perera45 හොස්පිටල් එකක් හදල ගන්නව කියන්නෙ. ගෙයක් හදල කැන්දගෙන යන්නම් කියල. මේ වැස්සිට ඒක තේරෙන්නෙ නෑ 🤪"</t>
+  </si>
+  <si>
+    <t>1085508780085850112</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 12:07:15 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@LadyBossHippo උඔ කොහේ කොහොම කාගේ වෙලා හිටියත් මගේගෙන් පස්සේ අනිත් උන්ගේ 😍😍"</t>
+  </si>
+  <si>
+    <t>1085473003465392128</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 09:45:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@KawdaBoy ඒ ලව් එක තමා මේ වෙනකල්ම ඇදිඇදී තියෙන්නේ. 😞 අනාගතේ නම් කොහොම වෙයිද මංදා"</t>
+  </si>
+  <si>
+    <t>1085465402178625538</t>
+  </si>
+  <si>
+    <t>1042790863389114368</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 09:14:53 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DJSlash9 කන්නාඩි එක්ක පොඩි ගතියකුත් තියෙනව ඉතිං"</t>
+  </si>
+  <si>
+    <t>1085447073737134081</t>
+  </si>
+  <si>
+    <t>896772955623104512</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 08:02:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>""සෙරෙප්පු දෙකක් නැතුව බිම බහින්න බැරි එකෙක් කොහොම යුද්ධ කලාද මම දන්නේ නැහැ" (VIDEO) https://t.co/x11dpWC3F7"</t>
+  </si>
+  <si>
+    <t>1085446638548611072</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 08:00:19 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ReddeCricket හෑබැයි ආදරය, දයාව , කරුණාව තියෙනව ඉතිරෙන්න. ඔයාලට වරදින්නෙ නෑ යලුවනේ."</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>1085411568467304449</t>
+  </si>
+  <si>
+    <t>947667642</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 05:40:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>"8 වසරෙදි මෙහෙම හිටියනම්, ඉපදෙද්දි කොහොම ඉන්න ඇතිද 😂😂 https://t.co/aEAw3677FE"</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>1085385693881356288</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 03:58:09 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ExcuzeMiReturn සෙල්ෆියක් ගන්නව 😁😁"</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>1085384653370998785</t>
+  </si>
+  <si>
+    <t>986583153761398784</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 03:54:01 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sansajran අපේ ගෙදර තාත්තගේ ඉස්කෝලෙයි දුවගේ ඉස්කෝලෙයි දෙකම තියෙනව. Sms දෙකට බෙදෙනවා 🤭"</t>
+  </si>
+  <si>
+    <t>4579848553</t>
+  </si>
+  <si>
+    <t>1085382197954179078</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 03:44:16 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@tharu__ ඕක මට අනන්තවත් වෙලා තියෙනව. ඕකෙන් වෙන්නෙ වැරදි වැරදි හරි මිනිස්සු ඉංග්‍රීසි කතා කරන්න බයයි. ඉතින් කොහොමද ඉංග්‍රීසි හදාගන්නෙ."</t>
+  </si>
+  <si>
+    <t>1085374044189405184</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 03:11:52 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@nthathsaranii ඒවගෙ තමා අපි එයාලට කරන ආදරේට සමාන ආදරයක් වෙන කාටවත් දෙන්නත් බෑ අපේ අතින්.කවුරු කොහොම කිව්වත් මට බෑ😒හිතට එකගව"</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>1085360230374957056</t>
+  </si>
+  <si>
+    <t>3268719913</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 02:16:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>"සව්දියෙ උන් උන්ගෙ ගෑනුන්ට ළමයින්ට සලකන්නෙ එහෙමනං වෙන රටවල් වලින් වැඩට යන අයට කොහොම සලකනවා ඇතිද."</t>
+  </si>
+  <si>
+    <t>1085356927419326465</t>
+  </si>
+  <si>
+    <t>2208722564</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 02:03:51 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ලංකාවේ බල්ලො හදන්න බැ... ඔහොම නෙමේ කොහොම video දැම්මත්... https://t.co/VRbLi5TTva"</t>
+  </si>
+  <si>
+    <t>1085222923613470721</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 17:11:22 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Annnuza ඇයි උබ ලඟ ජෙනුයින් වින්ඩෝස් එකක් තියෙනව කිව්වේ"</t>
+  </si>
+  <si>
+    <t>1085216111539429376</t>
+  </si>
+  <si>
+    <t>997485999457423362</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 16:44:17 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Wind_Desika පොඩි ගතියක් තියෙනව නේ?"</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>1085202884499623936</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 15:51:44 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කොහොම හරි ප්‍රැක්ටිස් ඉවර වෙලා #රෑනවයටසිත්ගත්ගී අහන්න.. එන්න ඔයාලත් @vishiru කැමතිම සිංදු අහන්නේ.. #RathumakaraFM @RathuMakaraFM_"</t>
+  </si>
+  <si>
+    <t>1085186420723961856</t>
+  </si>
+  <si>
+    <t>2175356713</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 14:46:19 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NishadiAnuttara ඉත්ත ඔහොමනම් ගහ කොහොම ඇතිද? 🙊🙈"</t>
+  </si>
+  <si>
+    <t>1085167823360585729</t>
+  </si>
+  <si>
+    <t>1081345331844055042</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 13:32:25 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@adaderana හොඳ වෙලාවට. එහෙම කියලත් මෙහෙම නම් එහෙම නොකිව්වා නම් කොහොම තියෙයිද?"</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>1085163641048088582</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 13:15:48 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sanju_Live ඊයෙ වැස්සනෙ කවුරුහරි වැහි නැටුම නටල තියෙනව 🙄"</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>1085156958296891392</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 12:49:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Amashani_Herath ලක්සනට තියෙනව.😋කියන්න පොටෝ ටික"</t>
+  </si>
+  <si>
+    <t>1085153885226823681</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 12:37:02 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Amashani_Herath ඒ වුනාට ඒ වගේ පොඩි මෙවුව එකක් තියෙනව..😋"</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>1085081578055716864</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:49:42 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@itzJambole මේම හරි එකක් ඒ දවස් වල කරලා තියෙනව දැං ඒමවත් බෑ 😂😂"</t>
+  </si>
+  <si>
+    <t>1085075707795890176</t>
+  </si>
+  <si>
+    <t>947587112051838976</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 07:26:23 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@stranshad දැන් පැයක් විතර කනව,කන ගමන් නිදා ගන්නව නැගිටිනව වතුර බොනවා අයේ කනවා"</t>
+  </si>
+  <si>
+    <t>1085012548695613440</t>
+  </si>
+  <si>
+    <t>1965649878</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 03:15:24 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කොහොම ද ගහෙන් ගහට ගිහින් පුවක් කඩන හෑටි🤓 යාලුවන්ටත් බලන්න Share කරමු https://t.co/ZvpC9AGtUG"</t>
+  </si>
+  <si>
+    <t>1084846810185650182</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 16:16:49 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@MaheshNegombo ඔව් අද හදිස්සියේ විනාඩි කීපෙකට බැලුවේ..! පොඩි ගතියක් තියෙනව වගේ ඉතිං..! 😆"</t>
+  </si>
+  <si>
+    <t>1084796009518002176</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 12:54:57 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@anuwa01 තොපි කොහොම හරි මාවත් කාපල්ලකො 😂"</t>
+  </si>
+  <si>
+    <t>1084787780620697601</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 12:22:15 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@RansaraniBole @Busty_Bubble හැබැයි ඒ ලමයා මෝචරියෙත් කෙල්ලො හොයල තියෙනව😂"</t>
+  </si>
+  <si>
+    <t>1084779386627252225</t>
+  </si>
+  <si>
+    <t>2602073233</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 11:48:54 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ExcuzeMiReturn එක ගිණි කූරක් ගහල අහල ගම් හතම ගිනි ගන්නව දැන්"</t>
+  </si>
+  <si>
+    <t>1084764865506484225</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 10:51:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"එකක් කඩතොළු වසා ගන්නට        ගිහිං මේ වෙන කාරියා සියක් ⁣කඩතොළු හදා ගන්නව පොළොන්නරැ ආචාරියා."</t>
+  </si>
+  <si>
+    <t>1084752229427335168</t>
+  </si>
+  <si>
+    <t>375471748</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 10:00:59 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@kazZtr_ ඔවු.. මේකත් නිකන් දැම්මෙ.. උඹල සිරා ගන්නව 🤦"</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>1084749049591263232</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 09:48:21 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@maalupaan තාම හරියට හොයාගන්න බැරුව ඉන්නෙ සීන් එක මොකක්ද කියල..කොන් වෙලා වගේ හැගීමක් තියෙනව😂"</t>
+  </si>
+  <si>
+    <t>1084741041855459328</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 09:16:32 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Ma_Du_Ka ඔව්. කොහොම උනත් මම ඒ පලාතේ ගියෙ නෑ ලැජ්ජාවටම 😆😆😆"</t>
+  </si>
+  <si>
+    <t>1084724443358756865</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 08:10:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@lishwebber lol, මමත් දැකල තියෙනව එහෙම උන්. අපේ ඔෆිස් එකෙත් ඉන්නව ඔහොම එකක් දෙකක් :D"</t>
+  </si>
+  <si>
+    <t>1084714940106125313</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:32:49 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මැච් එකට දවස් ගානක් තියල මෙහෙම නම් ලං වෙනකොට කොහොම තියෙයිද?    #TCLSL"</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>1084714213233385472</t>
+  </si>
+  <si>
+    <t>2164826550</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 07:29:56 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මේ දවස්වල ඉතාලි භාශාව ඉගෙන ගන්නව..ඒකත් ගොඩ දා ගත්තොත් මව් භාශාවත් එක්ක භාශා 4ක් පුළුවන්.. 🤩"</t>
+  </si>
+  <si>
+    <t>245</t>
+  </si>
+  <si>
+    <t>1084702132190642178</t>
+  </si>
+  <si>
+    <t>4829912481</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 06:41:55 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@issapraveen අපිත් තීන්ත ගාල තියෙනව හැබැයි ,, මේම තීන්ත නාල නෑ.... කමන්නෑ ඉතින් පලවෙනි පාරට වෙන්නැතිනෙ තින්‍ත ගාන්නෙ 😂😂"</t>
+  </si>
+  <si>
+    <t>1084664380308873216</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 04:11:55 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@nam3chang3d වේකන්සි තියෙනව..කුබුරක...පුරං වෙලා තියෙන්නෙ..😁 අයිතිකාරයට දැං වයසයි.. වැඩ කරගන්න බෑ.."</t>
+  </si>
+  <si>
+    <t>1084627164429873152</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 01:44:02 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@maalupaan වැඩක නෑ. මම අඹ, බුරියානි, පොලොස්, ... මෙකී නොකී දේවල් දීල තියෙනව. කිසිම අගය කිරීමක් නෑ."</t>
+  </si>
+  <si>
+    <t>1084499715171860480</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 17:17:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@tikirimaarie @Chamalka_N @Soulchild_Rishi අපේ මුවාත තියෙනව මල්ලෙ අමුතුවෙන් තියන්න ඕන නෑ 😂"</t>
+  </si>
+  <si>
+    <t>1084498328770002945</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 17:12:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"රැවුලත් තියෙනව..😁 කොන්දකුත් තියෙනව..😁 හැබැයි කොන්ද තියෙන්නෙ පිට නෙමෙයි..මගෙම ඇගෙ..😁😁 https://t.co/CPYllckE56"</t>
+  </si>
+  <si>
+    <t>1084491069704683520</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 16:43:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@GloryMinion @nthathsaranii කොච්චරවත් හිතල තියෙනව. ඒත් ආයෙ අමතක වෙනව."</t>
+  </si>
+  <si>
+    <t>1084486486181974016</t>
+  </si>
+  <si>
+    <t>933893323240214529</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 16:25:01 +0000 2019</t>
+  </si>
+  <si>
+    <t>"වටේම කෙල්ලො එක්ක යාලු වෙන්න වුවමනාව තිබ්බා. කොහොම වුනත්... https://t.co/PJqnq90x3f"</t>
+  </si>
+  <si>
+    <t>1084480129521180673</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 15:59:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Dhanush21417946 @Gimalka ඉතින් මං සාරි ඇදීම ගැන මොනාත් කියලා නෑනෙ වැරැද්දක් මට ඒක කොහොම ඇන්දත් එකයි බ්‍රෝ 😂"</t>
+  </si>
+  <si>
+    <t>1084471641541754880</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 15:26:02 +0000 2019</t>
+  </si>
+  <si>
+    <t>"Team 8 යි පුලුවන් 10ක් තියෙනව. ඔන්න ඔතනයි පුතේ තරඟෙ තියෙන්නෙ. #TCLSL"</t>
+  </si>
+  <si>
+    <t>1084449981141057536</t>
+  </si>
+  <si>
+    <t>2369956382</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:59:58 +0000 2019</t>
+  </si>
+  <si>
+    <t>"දැන් කාලේ එන සිංදු වල Album Art වලට Visual concepts කොහොම ඔලුවට එනවද මංදා. 🖤🖤🖤"</t>
+  </si>
+  <si>
+    <t>1084443207780438016</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:33:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@NishadiAnuttara @Wind_Desika @NileeGamage @daughterislife ඕක මම ඒ කාලෙම රිපෝට් කරපු එකක්....ඔය වගෙ එලවුන්ට් දෙක තුනක්ම තියෙනව"</t>
+  </si>
+  <si>
+    <t>1084442291278819331</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:29:24 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@mushi_lk ඔව් හොඳ පළපුරුද්දක් තියෙනව... Ground  එකේ කොනකට වෙලා හිටං ඉදල පුරුදුයි 😬 ... @thiiish මෙයා සාක්කී 😂"</t>
+  </si>
+  <si>
+    <t>1084435222433738753</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:01:19 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@gayandinusha ආ හිතුණොත් කන්න ගන්නව 😌"</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>1084420451831402497</t>
+  </si>
+  <si>
+    <t>812297402656899077</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 12:02:37 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඔය කොහොම ගහනවා කීවත් @ReddeCricket කට්ටිය බැස්ස ගමන් ගහන ගැහිල්ල බලපල්ලකෝ. ඇඩෙයි ඈ 😁  ගහන්නෙ ක්‍රිකට් හොදේ 😇"</t>
+  </si>
+  <si>
+    <t>1084418326334488576</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 11:54:11 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@itzJambole @rasikalink වෙන Profile Picture එකකුයි වෙන නමකුයි දාන ඉද්දි කොහොම අඳුර ගන්නද"</t>
+  </si>
+  <si>
+    <t>1084416287382491136</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 11:46:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Annnuza අනේ පලයන් ඩෝ යන්ඩ🤣🤣ගොඩක් ක්‍රම තියෙනව😂"</t>
+  </si>
+  <si>
+    <t>1084357780369096705</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 07:53:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@lasankaOnline උඹට කැම්පස් එකෙන් email එකක් දීලා තියෙනව නේද? 😏"</t>
+  </si>
+  <si>
+    <t>1084345191547297792</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 07:03:34 +0000 2019</t>
+  </si>
+  <si>
+    <t>"සතිය මැද නිවාඩුවක්  තියෙනව කියල දැනුනම හිතට දැනෙන සතුට  සල්ලි වලට ගන්ඩ බෑ මහත්තයෝ #holidays  #WeekendUpdate"</t>
+  </si>
+  <si>
+    <t>1084321330806353920</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 05:28:45 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මේ දාස් වල ටීම් එකෙන් ටීම් එකට මඩ ගහ ගන්නව😂😂 සික් යකෝ ඔක්කොම ශ්‍රිලංකන් ටීම් නේද වෙන රටවලින් ආවොත් කෝම තියේද යුද පිටියක් වෙලා තියෙයි"</t>
+  </si>
+  <si>
+    <t>1084299906444083200</t>
+  </si>
+  <si>
+    <t>720141928</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 04:03:37 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@KanaShot කොහොම තිබ්බ team එකක්ද ඕයී මේක? @ExcuzeMiReturn  😭"</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>1084292905622155265</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 03:35:48 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මගෙයි ජූඩගෙයි කඩල කරත්තෙත් එදාට තියෙනව.. උණු බල්ලොත් දෙන්න හිතාන ඉන්නේ 😁  #TCLSL #BusinessIdeas"</t>
+  </si>
+  <si>
+    <t>266</t>
+  </si>
+  <si>
+    <t>1084152901520510976</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 18:19:28 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@DJSlash9 පැන්ඩෙක් වෙලා ඒ ටික කොහොම දැනගත්තද මන්දානේහ් 😂😂"</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>1084126644837670912</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 16:35:08 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@_ArEreP_NeEvArT ඔව් නේ.. හොදට ෆිල්ම් එකක් එහෙම බලල නිදාගන්න දවසක් තියෙනව 😂"</t>
+  </si>
+  <si>
+    <t>268</t>
+  </si>
+  <si>
+    <t>1084110544469217282</t>
+  </si>
+  <si>
+    <t>349095615</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 15:31:10 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අපේ උන් හයේ ඒවා ගහන්න බුදු ගේමක් දෙන වෙලාවක ගින්නක් නැතුව හයේ ඒවා ගහන්නෙ මෙහෙමයි.  කොහොම ගහනවද මන්දා :/ https://t.co/QQ1lGuOIZr"</t>
+  </si>
+  <si>
+    <t>1084109819055726592</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 15:28:17 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Sankha_Mudhitha තව 4ක් තියෙනව 😂"</t>
+  </si>
+  <si>
+    <t>1084101590447878144</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 14:55:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@rainbowdreamzz වළලුකර ලඟත් ඇට දෙකක් තියෙනව බං.. උබ දන්නවද ඒක.. මාත් අද දන්නෙ යාළුවෙක් කීව නිසා 😋"</t>
+  </si>
+  <si>
+    <t>1084085356805255168</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 13:51:05 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කට්ටියම කියන්නෙ නම් "අපි මැච් එක ගහන්නෙ ආතල් එකට" කියලා ඒ උනාට යටි හිතින් කොහොම හරි දිනන එක තමා පරම පරමාර්තය.....! 😂  #TCLSL"</t>
+  </si>
+  <si>
+    <t>1084062495516418049</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 12:20:14 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Rasthiyaduwa @bumrahge ඇත්ත අයියේ ඕක මාත් අහල තියෙනව.... මිනිහ අවුට් උනාම යන්නැතුව ආපහු ගහනවලු 😂😂"</t>
+  </si>
+  <si>
+    <t>1084047779343798273</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 11:21:45 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මං කැමති කලුයි සුදුයි පූසන්ට. ඉන්න පූසො තුන් දෙනාම කලුයි සුදුයි නෙමේ. ඒ නිසා කලුයි සුදුයි බල්ලෙක් ගන්නව."</t>
+  </si>
+  <si>
+    <t>274</t>
+  </si>
+  <si>
+    <t>1084039340345372677</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 10:48:13 +0000 2019</t>
+  </si>
+  <si>
+    <t>"දැන් ඔය කොහොම මාකටින් කරත් vote වැඩිපුර තිබුනත් එදාට මැච් ටික ගහලම එපැයි දිනන්න 😂  #TCLSL"</t>
+  </si>
+  <si>
+    <t>1085414300209086464</t>
+  </si>
+  <si>
+    <t>Wed Jan 16 05:51:49 +0000 2019</t>
+  </si>
+  <si>
+    <t>"සමහර උන්ගෙ සෝශල් මීඩියා හැසිරීම දැක්කාම හිතෙනවා උන්ට ඉන්න සමාජෙන් කොහොම කොහොම ගුටි සෙට්වෙලා ඇද්ද කියලා...😬  ඒත් පස්සෙ මතක්වෙනවා ඒ වගේ උන් ආශ්‍රය කරන්නෙත් එහෙම පිරිසක්ම නිසා දෙකක් ඇනලා හදාගන්න උන් නෑ කියලා  පව් මොනා වුනත්...හැදෙන්නෙ නෑ ගුටියක් කනකන් 😂✋🏽  #දැකලා_හිතුණා"</t>
+  </si>
+  <si>
+    <t>1085257764513796096</t>
+  </si>
+  <si>
+    <t>Tue Jan 15 19:29:48 +0000 2019</t>
+  </si>
+  <si>
+    <t>"දිලීප් සාරංගගෙ Mashup මිනිස්සු දැනගත්තෙ හතරවෙනි කවර් එකෙන් ඉදල. අවුරුදු ගානක් ගිහිල්ලත් එපා නොවි අහන සින්දු දෙකක් තියෙනව එකක් ඕක අනික ඉරාජ්ගෙ ආශාවරි .. ඇයි කියන්න මන් දන්නෙත් නැ ඒ සෝන්ග්ස් දෙක ෆට්ට. අනිත් ඒව එක දිගට අහනකොට ටික කාලයක් යද්දි එපා වෙනව.🤷😬🤚"</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>1084851308987731969</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 16:34:42 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඔබ මල නම්  මම ගස නම් මම කම්පා නොවී කොහොම ඉන්නද? ඔබ වෙනුවෙන්,  මම මල වෙන්නම්. මම මියෙන්නම්. ඒ ගැන කම්පාවක් මට නැති තරම්. https://t.co/oDd6711JtQ"</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t>1084790869113200641</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 12:34:32 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අපි යශෝදරාලා හෙව්වට  දැන් ඉන්නේ සනී ලියෝන්ලා,  ඒකයි අපිත් සිද්ධාර්ථ නොවී  ජොනී සින්ස්ලා උනේ  බුකියේ තිබිලා ගත්තේ මේක. මට හිතෙන විදිහට අපිට කලින් පරම්පරා වල මිනිස්සුත් මෙහෙම හිතලා හිටියනං මේ රට මේ වෙනකොට කොහොම තියේවිද? 😶"</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>1084737648076288001</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 09:03:03 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@Ma_Du_Ka එහෙම බැහැ. එතන නෝටිස් දාල තියෙනවා ගෙනියන්න කලින් බලලා ඒවගේ දේවල් තියෙනව නම් පෙන්නලා ගෙනියන්න කියලා. ඉරිලා වගේ නම් එයාලට කිව්වම එයාලා පොතේ නෝට් එකක් දානව. අනික පොඩි උන් බයයිනේ 😂"</t>
+  </si>
+  <si>
+    <t>281</t>
+  </si>
+  <si>
+    <t>1084684031629897728</t>
+  </si>
+  <si>
+    <t>Mon Jan 14 05:30:00 +0000 2019</t>
+  </si>
+  <si>
+    <t>"‘‘උඹේ ඩෙස් එක හිස්ව තියෙනව දකින්නෙ කොහොමද බං..?‘‘ පන්ති යන බව පවසා මිතුරන් සමඟ සතුටු වෙන්න ගිය සිසුවා මහවැලි ගඟට බිලි වෙයි…! https://t.co/sv1lgr3WJu"</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>1084529053158105089</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 19:14:10 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@nthathsaranii කෑලි කියන්නෙ layers කපන එකනෙ..ඒව නම් මාත් කරල තියෙනව..එත් අනිට්බ් chemical නාවන වැඩයි කොන්ඩෙ පුච්චන වැඩයි නැති කොන්ඩ හරි අඩුයි..ඔයාට ලස්සන කොන්ඩයක් තියෙනව..💎"</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>1084510289486262277</t>
+  </si>
+  <si>
+    <t>326979191</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 17:59:36 +0000 2019</t>
+  </si>
+  <si>
+    <t>"සිරස කියන්නෙ තමන්ට විරුද්ධ මිනිහට එලව එලව පහරදීම. සිරස ගිනිගත්ත වෙලාවෙ රාජපක්ෂලට ගැහුව. දැන් රාජපක්ෂ එක්ක එකතුවෙලා රනිල්ට ගහනව.  අපි ඔක්කොම දන්නව කිලී සහ රනිල් අතර ලොකු ප්‍රශ්නයක් තියෙනව කියල.  එහෙම කියල මාද්‍ය කියනදේ මිනිසුන්ට එපා කරන්න හොඳ නැහැ. #LKA #BlackMedia #SirasaTV https://t.co/NElBC9VA82"</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>1084454447076569091</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 14:17:43 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අක්කලාගේ දිහයින් එද්දී පොඩි කෙල්ල නිදි. පොඩ්ඩක් වෙලා බලන් ඉඳලා හිමිට කිස් එකක් දීලා ආවා. කොල්ලා මා.... කියාගෙන දුවන් ඇවිත් ඇඟට පැනලා මට කිස් එකක් දීපි. කොහොම මුන් දෙන්නව දාලා එන්නද. ආයේ ඉතිං අවුරුදු දෙහෙකින් වගේනේ දකින්න වෙන්නේ. 😭😭😭"</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>1084446669943402497</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:46:48 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ලීක් කරන ඒවත් තියෙනව සමහරු බ්ලැක්මේල් කරන්න ලීක් කරනවා තවත් ඒවා ලීක් වෙන්නෙ ෆෝන්ෂොප් වලින් තවත් ඒවා ඒ කොල්ලො එක්ක යාලුවෙලා ඉන්න වෙන කෙල්ලොම ලීක් කරනව 😶😶😶 https://t.co/1r4qhVzKaL"</t>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>1084445981607743488</t>
+  </si>
+  <si>
+    <t>736883083</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:44:04 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කොහොම උනත්  මන් තේරුම් ගත්තා හදවතට අංශක ගානක් ඉස්සරහින් මොලේ තියාගන්න ඕනි කියන එක. එතකොට හැමදේම දරා ගන්නත්,ඒවත් එක්කම බාහිරින් ඇති හිස් අවකාශය එක්ක අලුත් මුහුනතක් ගොඩනගා ගන්නත් කාලය විනාශ කරනවා වගේම උදව්වකුත් කරනවා කියලා මන් තේරුම් ගත්තා ...."</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>1084445763319390208</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:43:12 +0000 2019</t>
+  </si>
+  <si>
+    <t>"ඒත් මන් තේරුම් අරන්, කාලයත් එක්ක විසඳුමක් හෙව්වා.කොටින්ම කිව්වොත් මට එහෙම කරන්න උනෙත් දෛවයේ බලපෑම නිසාමයි. කොහොම උනත් අද මට සතුටුයි. මොකද පුංචි දුකක් තියනවා,ඉස්සරහට කොහොමද මන් දරාගන්නේ කියලා ...."</t>
+  </si>
+  <si>
+    <t>291</t>
+  </si>
+  <si>
+    <t>1084445610965590017</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:42:36 +0000 2019</t>
+  </si>
+  <si>
+    <t>"කොහොම උනත් ඒ දේවල් දෛවයටත් පිටින් මට කරගන්න ඕනි වෙන්න ඇති,ගොඩාක් දුරට ඔව්. ඉතින් ඒ දේවල් දෛවයේ නෙමේ මගේ ආත්මේම ලැබෙන්න අවශ්‍යයි කියන නියමයක් නෑ . ඒ නිසා ඒ දේවල් මොන ඒව උනත්, ගොඩාක් හිත රිදුනු තැන් තිබුනා..."</t>
+  </si>
+  <si>
+    <t>292</t>
+  </si>
+  <si>
+    <t>1084442596666007552</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:30:37 +0000 2019</t>
+  </si>
+  <si>
+    <t>"උස්සන්ගොඩ වෙරළෙ සුද්දො 2000ක් කෑම්ප් එකක් ගහලලු. එකෙක් මම දැක්ක කමෙන්ට් එකක් දාල තියෙනව. "අපි ගැහුවනම් තමයි උඹල කෑ ගහන්නෙ සුද්දො ගැහුවොත් මොකුත් නෑ" කියල. සුද්දා 2000ක් නෙවෙයි 10000 ක් ගැහුවත් උන් යන්නෙ දැක්ක කෙනෙක්ට Camp එකක් තිබ්බද නැද්ද කියල හොයාගන්න බැරිවෙන්න. ඒකට අපේ උන් 😂"</t>
+  </si>
+  <si>
+    <t>293</t>
+  </si>
+  <si>
+    <t>1084440742011973632</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 13:23:15 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@SLFreedomParty @PodujanaParty පොහොට්ටු දීගයට මං විරුද්දයි.. ශ‍්‍රීලනිප සංවිධායකයන් රැසක් මා සමගයි..- CBK චන්ද්‍රිකා ජනපති @MaithripalaS ට තදින් ලියා දන්වයි.. දැන් ඔය 10 වෙන්න ඇති ඉන්න බහුතරය. ඔය බහුතරේට කොහොම @PresRajapaksa අමතකවුනේ. ඔහුටත් මෙයින් කොපියක් යා යුතුයි නේද ?@Neetwit https://t.co/DKq5BcTrT5"</t>
+  </si>
+  <si>
+    <t>1084419251937660928</t>
+  </si>
+  <si>
+    <t>47276839</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 11:57:51 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@ExcuzeMiReturn @rathgamaya මූ වැඩියෙන්ම ෆේමස් උනේ කොහොම දන්නවද? අර මොබිටෙල් ස්ක්‍රීන් එකේ ටොයිලට් තියෙන තැන අහලා.  ඕල්ද බෙස්ට් රත්තෝ..  තව ඇක්සියෝ එකක් ගන්න ලැබේවා.."</t>
+  </si>
+  <si>
+    <t>1084415511843094528</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 11:43:00 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අපිත් එක්ක එලෝ මෙලෝ නැතුව සමහරුන්ට බැනපු කස්ටිය, ඒ කටවල් වලින්ම බැන්න උදවියගේ ගුන වයනව කියහංකො.  ලෝකෙ නම් කොහොම වෙනස් වෙනවද මංද. මිනිස්සු එහෙ බලලා මෙහෙ බලන්න කලින් වෙනස් වෙනවා මේම මේම.  රසවත්ම ටික අපි ගැන තැන් තැන් වල කියනේව ටික.😂😂😂"</t>
+  </si>
+  <si>
+    <t>1084367087462739969</t>
+  </si>
+  <si>
+    <t>4019364913</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 08:30:34 +0000 2019</t>
+  </si>
+  <si>
+    <t>"https://t.co/hMj21EdlZ1 කොහොම හරි කමක් නෑ ගලහ රෝහල විවෘත වෙනවා නම් හොඳයි. ගම් 15 කට වැඩි ප්‍රමාණයක ජනතාව මෙම රෝහලෙන් ප්‍රතිකාර ලබා ගන්නවා. #lka #Srilanka"</t>
+  </si>
+  <si>
+    <t>1084309171355283456</t>
+  </si>
+  <si>
+    <t>Sun Jan 13 04:40:26 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මේකෙත් ඉන්නව නේ කාටහරි ගින්නක් අවුලන්න තියෙනව නම් ඊට වඩා දෙයක් නැති මිනිස්සු?? රීට්වීට් කරලා ක්වෝට් කරල හරි සහයෝගයක් දෙනව ඒ වගේ ඒවට නම්.අප්පිරියයි🤢"</t>
+  </si>
+  <si>
+    <t>1084149092895391744</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 18:04:20 +0000 2019</t>
+  </si>
+  <si>
+    <t>"@lasankaOnline @CrizBale ලසියා උඹ ඒක කොහොම දරාගන්නවද කියන්න මම නම් දන්නැ..😅 ඒත් මෙ කෙල්ලෙක් ඉන්න නාකි කුපාඩියා කරන එව්වා මට ඉවසන් බලන් ඉන්න බෑ බන්...😭💔"</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>1084023369639448576</t>
+  </si>
+  <si>
+    <t>3654264274</t>
+  </si>
+  <si>
+    <t>Sat Jan 12 09:44:46 +0000 2019</t>
+  </si>
+  <si>
+    <t>"අරුණ පත්තරේ, හිත කැමති පොත විශේෂාංගයේ සුමිත්‍රා රාහුබද්ධ එයා කැමති පොත ගැන කියලා තියෙන්නේ, "සෙදෝනා" ඊවා රණවීර කතෘ. අහලා තියෙනවාද ? මේ පොත දැන් මුද්‍රණය කරන්නෙත් නෑ කියලා තියෙනවා, සුමිත්‍රා පොත ගැන කියලා තියෙන විදියට පොත කොහොම හරි හොයාගෙන කියවන්ඩ හිතුනා."</t>
   </si>
 </sst>
 </file>
@@ -7615,10 +8593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F568"/>
+  <dimension ref="A1:F658"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A543" workbookViewId="0">
-      <selection activeCell="F568" sqref="F568"/>
+    <sheetView tabSelected="1" topLeftCell="A633" workbookViewId="0">
+      <selection activeCell="F645" sqref="F645:F658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18989,6 +19967,1806 @@
         <v>50</v>
       </c>
     </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A569" s="6" t="s">
+        <v>703</v>
+      </c>
+      <c r="B569" s="6" t="s">
+        <v>2376</v>
+      </c>
+      <c r="C569" s="6" t="s">
+        <v>2377</v>
+      </c>
+      <c r="D569" s="6" t="s">
+        <v>2378</v>
+      </c>
+      <c r="E569" s="6" t="s">
+        <v>2379</v>
+      </c>
+      <c r="F569" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A570" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="B570" s="6" t="s">
+        <v>2380</v>
+      </c>
+      <c r="C570" s="6" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D570" s="6" t="s">
+        <v>2381</v>
+      </c>
+      <c r="E570" s="6" t="s">
+        <v>2382</v>
+      </c>
+      <c r="F570" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A571" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="B571" s="6" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C571" s="6" t="s">
+        <v>2377</v>
+      </c>
+      <c r="D571" s="6" t="s">
+        <v>2384</v>
+      </c>
+      <c r="E571" s="6" t="s">
+        <v>2385</v>
+      </c>
+      <c r="F571" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A572" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="B572" s="6" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C572" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D572" s="6" t="s">
+        <v>2387</v>
+      </c>
+      <c r="E572" s="6" t="s">
+        <v>2388</v>
+      </c>
+      <c r="F572" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A573" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="B573" s="6" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C573" s="6" t="s">
+        <v>2195</v>
+      </c>
+      <c r="D573" s="6" t="s">
+        <v>2390</v>
+      </c>
+      <c r="E573" s="6" t="s">
+        <v>2391</v>
+      </c>
+      <c r="F573" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A574" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="B574" s="6" t="s">
+        <v>2392</v>
+      </c>
+      <c r="C574" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D574" s="6" t="s">
+        <v>2393</v>
+      </c>
+      <c r="E574" s="6" t="s">
+        <v>2394</v>
+      </c>
+      <c r="F574" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A575" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="B575" s="6" t="s">
+        <v>2395</v>
+      </c>
+      <c r="C575" s="6" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D575" s="6" t="s">
+        <v>2397</v>
+      </c>
+      <c r="E575" s="6" t="s">
+        <v>2398</v>
+      </c>
+      <c r="F575" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A576" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="B576" s="6" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C576" s="6" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D576" s="6" t="s">
+        <v>2401</v>
+      </c>
+      <c r="E576" s="6" t="s">
+        <v>2402</v>
+      </c>
+      <c r="F576" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A577" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="B577" s="6" t="s">
+        <v>2403</v>
+      </c>
+      <c r="C577" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D577" s="6" t="s">
+        <v>2404</v>
+      </c>
+      <c r="E577" s="6" t="s">
+        <v>2405</v>
+      </c>
+      <c r="F577" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A578" s="6" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B578" s="6" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C578" s="6" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D578" s="6" t="s">
+        <v>2409</v>
+      </c>
+      <c r="E578" s="6" t="s">
+        <v>2410</v>
+      </c>
+      <c r="F578" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A579" s="6" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B579" s="6" t="s">
+        <v>2412</v>
+      </c>
+      <c r="C579" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D579" s="6" t="s">
+        <v>2413</v>
+      </c>
+      <c r="E579" s="6" t="s">
+        <v>2414</v>
+      </c>
+      <c r="F579" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A580" s="6" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B580" s="6" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C580" s="6" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D580" s="6" t="s">
+        <v>2418</v>
+      </c>
+      <c r="E580" s="6" t="s">
+        <v>2419</v>
+      </c>
+      <c r="F580" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A581" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="B581" s="6" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C581" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D581" s="6" t="s">
+        <v>2422</v>
+      </c>
+      <c r="E581" s="6" t="s">
+        <v>2423</v>
+      </c>
+      <c r="F581" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A582" s="6" t="s">
+        <v>770</v>
+      </c>
+      <c r="B582" s="6" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C582" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D582" s="6" t="s">
+        <v>2425</v>
+      </c>
+      <c r="E582" s="6" t="s">
+        <v>2426</v>
+      </c>
+      <c r="F582" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A583" s="6" t="s">
+        <v>2427</v>
+      </c>
+      <c r="B583" s="6" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C583" s="6" t="s">
+        <v>2429</v>
+      </c>
+      <c r="D583" s="6" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E583" s="6" t="s">
+        <v>2431</v>
+      </c>
+      <c r="F583" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A584" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="B584" s="6" t="s">
+        <v>2432</v>
+      </c>
+      <c r="C584" s="6" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D584" s="6" t="s">
+        <v>2434</v>
+      </c>
+      <c r="E584" s="6" t="s">
+        <v>2435</v>
+      </c>
+      <c r="F584" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A585" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="B585" s="6" t="s">
+        <v>2436</v>
+      </c>
+      <c r="C585" s="6" t="s">
+        <v>2205</v>
+      </c>
+      <c r="D585" s="6" t="s">
+        <v>2437</v>
+      </c>
+      <c r="E585" s="6" t="s">
+        <v>2438</v>
+      </c>
+      <c r="F585" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A586" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="B586" s="6" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C586" s="6" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D586" s="6" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E586" s="6" t="s">
+        <v>2442</v>
+      </c>
+      <c r="F586" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A587" s="6" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B587" s="6" t="s">
+        <v>2444</v>
+      </c>
+      <c r="C587" s="6" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D587" s="6" t="s">
+        <v>2445</v>
+      </c>
+      <c r="E587" s="6" t="s">
+        <v>2446</v>
+      </c>
+      <c r="F587" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A588" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="B588" s="6" t="s">
+        <v>2447</v>
+      </c>
+      <c r="C588" s="6" t="s">
+        <v>2448</v>
+      </c>
+      <c r="D588" s="6" t="s">
+        <v>2449</v>
+      </c>
+      <c r="E588" s="6" t="s">
+        <v>2450</v>
+      </c>
+      <c r="F588" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A589" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="B589" s="6" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C589" s="6" t="s">
+        <v>2452</v>
+      </c>
+      <c r="D589" s="6" t="s">
+        <v>2453</v>
+      </c>
+      <c r="E589" s="6" t="s">
+        <v>2454</v>
+      </c>
+      <c r="F589" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A590" s="6" t="s">
+        <v>2455</v>
+      </c>
+      <c r="B590" s="6" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C590" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="D590" s="6" t="s">
+        <v>2457</v>
+      </c>
+      <c r="E590" s="6" t="s">
+        <v>2458</v>
+      </c>
+      <c r="F590" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A591" s="6" t="s">
+        <v>2459</v>
+      </c>
+      <c r="B591" s="6" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C591" s="6" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D591" s="6" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E591" s="6" t="s">
+        <v>2084</v>
+      </c>
+      <c r="F591" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A592" s="6" t="s">
+        <v>2460</v>
+      </c>
+      <c r="B592" s="6" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C592" s="6" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D592" s="6" t="s">
+        <v>2462</v>
+      </c>
+      <c r="E592" s="6" t="s">
+        <v>2463</v>
+      </c>
+      <c r="F592" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A593" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="B593" s="6" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C593" s="6" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D593" s="6" t="s">
+        <v>2465</v>
+      </c>
+      <c r="E593" s="6" t="s">
+        <v>2466</v>
+      </c>
+      <c r="F593" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A594" s="6" t="s">
+        <v>2467</v>
+      </c>
+      <c r="B594" s="6" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C594" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="D594" s="6" t="s">
+        <v>2469</v>
+      </c>
+      <c r="E594" s="6" t="s">
+        <v>2470</v>
+      </c>
+      <c r="F594" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A595" s="6" t="s">
+        <v>803</v>
+      </c>
+      <c r="B595" s="6" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C595" s="6" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D595" s="6" t="s">
+        <v>2473</v>
+      </c>
+      <c r="E595" s="6" t="s">
+        <v>2474</v>
+      </c>
+      <c r="F595" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A596" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="B596" s="6" t="s">
+        <v>2475</v>
+      </c>
+      <c r="C596" s="6" t="s">
+        <v>2476</v>
+      </c>
+      <c r="D596" s="6" t="s">
+        <v>2477</v>
+      </c>
+      <c r="E596" s="6" t="s">
+        <v>2478</v>
+      </c>
+      <c r="F596" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A597" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="B597" s="6" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C597" s="6" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D597" s="6" t="s">
+        <v>2480</v>
+      </c>
+      <c r="E597" s="6" t="s">
+        <v>2481</v>
+      </c>
+      <c r="F597" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A598" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="B598" s="6" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C598" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D598" s="6" t="s">
+        <v>2483</v>
+      </c>
+      <c r="E598" s="6" t="s">
+        <v>2484</v>
+      </c>
+      <c r="F598" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A599" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="B599" s="6" t="s">
+        <v>2485</v>
+      </c>
+      <c r="C599" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D599" s="6" t="s">
+        <v>2486</v>
+      </c>
+      <c r="E599" s="6" t="s">
+        <v>2487</v>
+      </c>
+      <c r="F599" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A600" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="B600" s="6" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C600" s="6" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D600" s="6" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E600" s="6" t="s">
+        <v>2491</v>
+      </c>
+      <c r="F600" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A601" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="B601" s="6" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C601" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="D601" s="6" t="s">
+        <v>2493</v>
+      </c>
+      <c r="E601" s="6" t="s">
+        <v>2494</v>
+      </c>
+      <c r="F601" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A602" s="6" t="s">
+        <v>837</v>
+      </c>
+      <c r="B602" s="6" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C602" s="6" t="s">
+        <v>2496</v>
+      </c>
+      <c r="D602" s="6" t="s">
+        <v>2497</v>
+      </c>
+      <c r="E602" s="6" t="s">
+        <v>2498</v>
+      </c>
+      <c r="F602" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A603" s="6" t="s">
+        <v>2499</v>
+      </c>
+      <c r="B603" s="6" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C603" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D603" s="6" t="s">
+        <v>2501</v>
+      </c>
+      <c r="E603" s="6" t="s">
+        <v>2502</v>
+      </c>
+      <c r="F603" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A604" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="B604" s="6" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C604" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D604" s="6" t="s">
+        <v>2504</v>
+      </c>
+      <c r="E604" s="6" t="s">
+        <v>2505</v>
+      </c>
+      <c r="F604" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A605" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="B605" s="6" t="s">
+        <v>2506</v>
+      </c>
+      <c r="C605" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D605" s="6" t="s">
+        <v>2507</v>
+      </c>
+      <c r="E605" s="6" t="s">
+        <v>2508</v>
+      </c>
+      <c r="F605" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A606" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="B606" s="6" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C606" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D606" s="6" t="s">
+        <v>2510</v>
+      </c>
+      <c r="E606" s="6" t="s">
+        <v>2511</v>
+      </c>
+      <c r="F606" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A607" s="6" t="s">
+        <v>2512</v>
+      </c>
+      <c r="B607" s="6" t="s">
+        <v>2513</v>
+      </c>
+      <c r="C607" s="6" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D607" s="6" t="s">
+        <v>2515</v>
+      </c>
+      <c r="E607" s="6" t="s">
+        <v>2516</v>
+      </c>
+      <c r="F607" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A608" s="6" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B608" s="6" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C608" s="6" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D608" s="6" t="s">
+        <v>2520</v>
+      </c>
+      <c r="E608" s="6" t="s">
+        <v>2521</v>
+      </c>
+      <c r="F608" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A609" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="B609" s="6" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C609" s="6" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D609" s="6" t="s">
+        <v>2523</v>
+      </c>
+      <c r="E609" s="6" t="s">
+        <v>2524</v>
+      </c>
+      <c r="F609" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A610" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="B610" s="6" t="s">
+        <v>2525</v>
+      </c>
+      <c r="C610" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="D610" s="6" t="s">
+        <v>2526</v>
+      </c>
+      <c r="E610" s="6" t="s">
+        <v>2527</v>
+      </c>
+      <c r="F610" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A611" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="B611" s="6" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C611" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D611" s="6" t="s">
+        <v>2529</v>
+      </c>
+      <c r="E611" s="6" t="s">
+        <v>2530</v>
+      </c>
+      <c r="F611" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A612" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="B612" s="6" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C612" s="6" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D612" s="6" t="s">
+        <v>2532</v>
+      </c>
+      <c r="E612" s="6" t="s">
+        <v>2533</v>
+      </c>
+      <c r="F612" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A613" s="6" t="s">
+        <v>876</v>
+      </c>
+      <c r="B613" s="6" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C613" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D613" s="6" t="s">
+        <v>2535</v>
+      </c>
+      <c r="E613" s="6" t="s">
+        <v>2536</v>
+      </c>
+      <c r="F613" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A614" s="6" t="s">
+        <v>881</v>
+      </c>
+      <c r="B614" s="6" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C614" s="6" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D614" s="6" t="s">
+        <v>2539</v>
+      </c>
+      <c r="E614" s="6" t="s">
+        <v>2540</v>
+      </c>
+      <c r="F614" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A615" s="6" t="s">
+        <v>886</v>
+      </c>
+      <c r="B615" s="6" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C615" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="D615" s="6" t="s">
+        <v>2542</v>
+      </c>
+      <c r="E615" s="6" t="s">
+        <v>2543</v>
+      </c>
+      <c r="F615" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A616" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="B616" s="6" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C616" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D616" s="6" t="s">
+        <v>2545</v>
+      </c>
+      <c r="E616" s="6" t="s">
+        <v>2546</v>
+      </c>
+      <c r="F616" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A617" s="6" t="s">
+        <v>895</v>
+      </c>
+      <c r="B617" s="6" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C617" s="6" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D617" s="6" t="s">
+        <v>2549</v>
+      </c>
+      <c r="E617" s="6" t="s">
+        <v>2550</v>
+      </c>
+      <c r="F617" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A618" s="6" t="s">
+        <v>900</v>
+      </c>
+      <c r="B618" s="6" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C618" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="D618" s="6" t="s">
+        <v>2552</v>
+      </c>
+      <c r="E618" s="6" t="s">
+        <v>2553</v>
+      </c>
+      <c r="F618" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A619" s="6" t="s">
+        <v>905</v>
+      </c>
+      <c r="B619" s="6" t="s">
+        <v>2554</v>
+      </c>
+      <c r="C619" s="6" t="s">
+        <v>2377</v>
+      </c>
+      <c r="D619" s="6" t="s">
+        <v>2555</v>
+      </c>
+      <c r="E619" s="6" t="s">
+        <v>2556</v>
+      </c>
+      <c r="F619" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A620" s="6" t="s">
+        <v>910</v>
+      </c>
+      <c r="B620" s="6" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C620" s="6" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D620" s="6" t="s">
+        <v>2558</v>
+      </c>
+      <c r="E620" s="6" t="s">
+        <v>2559</v>
+      </c>
+      <c r="F620" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A621" s="6" t="s">
+        <v>2560</v>
+      </c>
+      <c r="B621" s="6" t="s">
+        <v>2561</v>
+      </c>
+      <c r="C621" s="6" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D621" s="6" t="s">
+        <v>2563</v>
+      </c>
+      <c r="E621" s="6" t="s">
+        <v>2564</v>
+      </c>
+      <c r="F621" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A622" s="6" t="s">
+        <v>915</v>
+      </c>
+      <c r="B622" s="6" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C622" s="6" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D622" s="6" t="s">
+        <v>2566</v>
+      </c>
+      <c r="E622" s="6" t="s">
+        <v>2567</v>
+      </c>
+      <c r="F622" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A623" s="6" t="s">
+        <v>919</v>
+      </c>
+      <c r="B623" s="6" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C623" s="6" t="s">
+        <v>2205</v>
+      </c>
+      <c r="D623" s="6" t="s">
+        <v>2569</v>
+      </c>
+      <c r="E623" s="6" t="s">
+        <v>2570</v>
+      </c>
+      <c r="F623" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A624" s="6" t="s">
+        <v>923</v>
+      </c>
+      <c r="B624" s="6" t="s">
+        <v>2571</v>
+      </c>
+      <c r="C624" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="D624" s="6" t="s">
+        <v>2572</v>
+      </c>
+      <c r="E624" s="6" t="s">
+        <v>2573</v>
+      </c>
+      <c r="F624" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A625" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="B625" s="6" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C625" s="6" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D625" s="6" t="s">
+        <v>2575</v>
+      </c>
+      <c r="E625" s="6" t="s">
+        <v>2576</v>
+      </c>
+      <c r="F625" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A626" s="6" t="s">
+        <v>932</v>
+      </c>
+      <c r="B626" s="6" t="s">
+        <v>2577</v>
+      </c>
+      <c r="C626" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="D626" s="6" t="s">
+        <v>2578</v>
+      </c>
+      <c r="E626" s="6" t="s">
+        <v>2579</v>
+      </c>
+      <c r="F626" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A627" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="B627" s="6" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C627" s="6" t="s">
+        <v>2581</v>
+      </c>
+      <c r="D627" s="6" t="s">
+        <v>2582</v>
+      </c>
+      <c r="E627" s="6" t="s">
+        <v>2583</v>
+      </c>
+      <c r="F627" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A628" s="6" t="s">
+        <v>2584</v>
+      </c>
+      <c r="B628" s="6" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C628" s="6" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D628" s="6" t="s">
+        <v>2586</v>
+      </c>
+      <c r="E628" s="6" t="s">
+        <v>2587</v>
+      </c>
+      <c r="F628" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A629" s="6" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B629" s="6" t="s">
+        <v>2589</v>
+      </c>
+      <c r="C629" s="6" t="s">
+        <v>2417</v>
+      </c>
+      <c r="D629" s="6" t="s">
+        <v>2590</v>
+      </c>
+      <c r="E629" s="6" t="s">
+        <v>2591</v>
+      </c>
+      <c r="F629" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="630" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A630" s="6" t="s">
+        <v>2592</v>
+      </c>
+      <c r="B630" s="6" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C630" s="6" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D630" s="6" t="s">
+        <v>2594</v>
+      </c>
+      <c r="E630" s="6" t="s">
+        <v>2595</v>
+      </c>
+      <c r="F630" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A631" s="6" t="s">
+        <v>2596</v>
+      </c>
+      <c r="B631" s="6" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C631" s="6" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D631" s="6" t="s">
+        <v>2599</v>
+      </c>
+      <c r="E631" s="6" t="s">
+        <v>2600</v>
+      </c>
+      <c r="F631" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A632" s="6" t="s">
+        <v>942</v>
+      </c>
+      <c r="B632" s="6" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C632" s="6" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D632" s="6" t="s">
+        <v>2602</v>
+      </c>
+      <c r="E632" s="6" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F632" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A633" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="B633" s="6" t="s">
+        <v>2604</v>
+      </c>
+      <c r="C633" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D633" s="6" t="s">
+        <v>2605</v>
+      </c>
+      <c r="E633" s="6" t="s">
+        <v>2606</v>
+      </c>
+      <c r="F633" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A634" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="B634" s="6" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C634" s="6" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D634" s="6" t="s">
+        <v>2608</v>
+      </c>
+      <c r="E634" s="6" t="s">
+        <v>2609</v>
+      </c>
+      <c r="F634" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A635" s="6" t="s">
+        <v>956</v>
+      </c>
+      <c r="B635" s="6" t="s">
+        <v>2610</v>
+      </c>
+      <c r="C635" s="6" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D635" s="6" t="s">
+        <v>2611</v>
+      </c>
+      <c r="E635" s="6" t="s">
+        <v>2612</v>
+      </c>
+      <c r="F635" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A636" s="6" t="s">
+        <v>961</v>
+      </c>
+      <c r="B636" s="6" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C636" s="6" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D636" s="6" t="s">
+        <v>2614</v>
+      </c>
+      <c r="E636" s="6" t="s">
+        <v>2615</v>
+      </c>
+      <c r="F636" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A637" s="6" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B637" s="6" t="s">
+        <v>2617</v>
+      </c>
+      <c r="C637" s="6" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D637" s="6" t="s">
+        <v>2618</v>
+      </c>
+      <c r="E637" s="6" t="s">
+        <v>2619</v>
+      </c>
+      <c r="F637" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A638" s="6" t="s">
+        <v>966</v>
+      </c>
+      <c r="B638" s="6" t="s">
+        <v>2620</v>
+      </c>
+      <c r="C638" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="D638" s="6" t="s">
+        <v>2621</v>
+      </c>
+      <c r="E638" s="6" t="s">
+        <v>2622</v>
+      </c>
+      <c r="F638" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A639" s="6" t="s">
+        <v>971</v>
+      </c>
+      <c r="B639" s="6" t="s">
+        <v>2623</v>
+      </c>
+      <c r="C639" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D639" s="6" t="s">
+        <v>2624</v>
+      </c>
+      <c r="E639" s="6" t="s">
+        <v>2625</v>
+      </c>
+      <c r="F639" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A640" s="6" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B640" s="6" t="s">
+        <v>2627</v>
+      </c>
+      <c r="C640" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D640" s="6" t="s">
+        <v>2628</v>
+      </c>
+      <c r="E640" s="6" t="s">
+        <v>2629</v>
+      </c>
+      <c r="F640" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A641" s="6" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B641" s="6" t="s">
+        <v>2631</v>
+      </c>
+      <c r="C641" s="6" t="s">
+        <v>963</v>
+      </c>
+      <c r="D641" s="6" t="s">
+        <v>2632</v>
+      </c>
+      <c r="E641" s="6" t="s">
+        <v>2633</v>
+      </c>
+      <c r="F641" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A642" s="6" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B642" s="6" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C642" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="D642" s="6" t="s">
+        <v>2636</v>
+      </c>
+      <c r="E642" s="6" t="s">
+        <v>2637</v>
+      </c>
+      <c r="F642" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A643" s="6" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B643" s="6" t="s">
+        <v>2639</v>
+      </c>
+      <c r="C643" s="6" t="s">
+        <v>2420</v>
+      </c>
+      <c r="D643" s="6" t="s">
+        <v>2640</v>
+      </c>
+      <c r="E643" s="6" t="s">
+        <v>2641</v>
+      </c>
+      <c r="F643" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A644" s="6" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B644" s="6" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C644" s="6" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D644" s="6" t="s">
+        <v>2644</v>
+      </c>
+      <c r="E644" s="6" t="s">
+        <v>2645</v>
+      </c>
+      <c r="F644" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A645" s="6" t="s">
+        <v>2646</v>
+      </c>
+      <c r="B645" s="6" t="s">
+        <v>2647</v>
+      </c>
+      <c r="C645" s="6" t="s">
+        <v>2648</v>
+      </c>
+      <c r="D645" s="6" t="s">
+        <v>2649</v>
+      </c>
+      <c r="E645" s="6" t="s">
+        <v>2650</v>
+      </c>
+      <c r="F645" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A646" s="6" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B646" s="6" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C646" s="6" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D646" s="6" t="s">
+        <v>2653</v>
+      </c>
+      <c r="E646" s="6" t="s">
+        <v>2654</v>
+      </c>
+      <c r="F646" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A647" s="6" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B647" s="6" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C647" s="6" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D647" s="6" t="s">
+        <v>2657</v>
+      </c>
+      <c r="E647" s="6" t="s">
+        <v>2658</v>
+      </c>
+      <c r="F647" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A648" s="6" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B648" s="6" t="s">
+        <v>2660</v>
+      </c>
+      <c r="C648" s="6" t="s">
+        <v>2661</v>
+      </c>
+      <c r="D648" s="6" t="s">
+        <v>2662</v>
+      </c>
+      <c r="E648" s="6" t="s">
+        <v>2663</v>
+      </c>
+      <c r="F648" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A649" s="6" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B649" s="6" t="s">
+        <v>2665</v>
+      </c>
+      <c r="C649" s="6" t="s">
+        <v>2661</v>
+      </c>
+      <c r="D649" s="6" t="s">
+        <v>2666</v>
+      </c>
+      <c r="E649" s="6" t="s">
+        <v>2667</v>
+      </c>
+      <c r="F649" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A650" s="6" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B650" s="6" t="s">
+        <v>2669</v>
+      </c>
+      <c r="C650" s="6" t="s">
+        <v>2661</v>
+      </c>
+      <c r="D650" s="6" t="s">
+        <v>2670</v>
+      </c>
+      <c r="E650" s="6" t="s">
+        <v>2671</v>
+      </c>
+      <c r="F650" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A651" s="6" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B651" s="6" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C651" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D651" s="6" t="s">
+        <v>2674</v>
+      </c>
+      <c r="E651" s="6" t="s">
+        <v>2675</v>
+      </c>
+      <c r="F651" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A652" s="6" t="s">
+        <v>2676</v>
+      </c>
+      <c r="B652" s="6" t="s">
+        <v>2677</v>
+      </c>
+      <c r="C652" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D652" s="6" t="s">
+        <v>2678</v>
+      </c>
+      <c r="E652" s="6" t="s">
+        <v>2679</v>
+      </c>
+      <c r="F652" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A653" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="B653" s="6" t="s">
+        <v>2680</v>
+      </c>
+      <c r="C653" s="6" t="s">
+        <v>2681</v>
+      </c>
+      <c r="D653" s="6" t="s">
+        <v>2682</v>
+      </c>
+      <c r="E653" s="6" t="s">
+        <v>2683</v>
+      </c>
+      <c r="F653" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A654" s="6" t="s">
+        <v>988</v>
+      </c>
+      <c r="B654" s="6" t="s">
+        <v>2684</v>
+      </c>
+      <c r="C654" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D654" s="6" t="s">
+        <v>2685</v>
+      </c>
+      <c r="E654" s="6" t="s">
+        <v>2686</v>
+      </c>
+      <c r="F654" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="655" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A655" s="6" t="s">
+        <v>989</v>
+      </c>
+      <c r="B655" s="6" t="s">
+        <v>2687</v>
+      </c>
+      <c r="C655" s="6" t="s">
+        <v>2688</v>
+      </c>
+      <c r="D655" s="6" t="s">
+        <v>2689</v>
+      </c>
+      <c r="E655" s="6" t="s">
+        <v>2690</v>
+      </c>
+      <c r="F655" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="656" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A656" s="6" t="s">
+        <v>994</v>
+      </c>
+      <c r="B656" s="6" t="s">
+        <v>2691</v>
+      </c>
+      <c r="C656" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D656" s="6" t="s">
+        <v>2692</v>
+      </c>
+      <c r="E656" s="6" t="s">
+        <v>2693</v>
+      </c>
+      <c r="F656" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="657" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A657" s="6" t="s">
+        <v>998</v>
+      </c>
+      <c r="B657" s="6" t="s">
+        <v>2694</v>
+      </c>
+      <c r="C657" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D657" s="6" t="s">
+        <v>2695</v>
+      </c>
+      <c r="E657" s="6" t="s">
+        <v>2696</v>
+      </c>
+      <c r="F657" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="658" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A658" s="6" t="s">
+        <v>2697</v>
+      </c>
+      <c r="B658" s="6" t="s">
+        <v>2698</v>
+      </c>
+      <c r="C658" s="6" t="s">
+        <v>2699</v>
+      </c>
+      <c r="D658" s="6" t="s">
+        <v>2700</v>
+      </c>
+      <c r="E658" s="6" t="s">
+        <v>2701</v>
+      </c>
+      <c r="F658" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -18998,7 +21776,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211 A371:E470" numberStoredAsText="1"/>
+    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211 A371:E470 A569:E576 A579:E580 A578:D578 A582:E641 A581:E581 A577:E577 A642:E643 A644:E645 A646:E658" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
select best model with iterating epoch and save it on disk
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6006" uniqueCount="4124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6007" uniqueCount="4124">
   <si>
     <t>instance_id</t>
   </si>
@@ -31747,12 +31747,15 @@
       <c r="D787" s="6" t="s">
         <v>3220</v>
       </c>
-      <c r="E787" s="6" t="s">
+      <c r="E787" s="11" t="s">
         <v>3221</v>
+      </c>
+      <c r="F787" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="G787" t="str">
         <f t="shared" si="12"/>
-        <v>Neutral</v>
+        <v>Racist</v>
       </c>
     </row>
     <row r="788" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add more racist tweets
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Level 4\Software Engineering Research Project - SENG 44696\GitRepo\sinhalese_language_racism_detection\data-set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC1BAB0-7297-44AB-8B36-22F5D85ABCC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE8BD9F-2ADA-48E9-9B53-156D7AAE0887}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7771" uniqueCount="5071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8191" uniqueCount="5318">
   <si>
     <t>instance_id</t>
   </si>
@@ -15257,6 +15257,747 @@
   </si>
   <si>
     <t>"රැල්ලට පුක පෙන්නපු කොල්ලො ටික හොයාගෙන නඩු දාලා ඇතුලට යවන්ඩ සතියක්වත් ගියෙ නෑ.. ඒ උනාට පැත්ත මාරු කර කර විල්පත්තුවේ කැලෑ කපන රිශාඩ් බදූර්දීන් අල්ලන්ඩ පොලිස් ඉවවත් නීතියේ දෙවගනගෙ ඇස් දෙකවත් පේන්නෙ නැහැ..  #රටේනීතියගැනආඩම්බරයි"</t>
+  </si>
+  <si>
+    <t>1014894303523426304</t>
+  </si>
+  <si>
+    <t>Thu Jul 05 15:30:32 +0000 2018</t>
+  </si>
+  <si>
+    <t>"@Indrajithonline නෙද්දකිං හම්බය😂"</t>
+  </si>
+  <si>
+    <t>813812078406307840</t>
+  </si>
+  <si>
+    <t>Tue Dec 27 18:21:34 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@WenuraGamage අයෙත් අහලා යාපනෙ තම්බි ලා කියන්නේ තන්නීර් කියලලු 😂"</t>
+  </si>
+  <si>
+    <t>811942120277741568</t>
+  </si>
+  <si>
+    <t>177930225</t>
+  </si>
+  <si>
+    <t>Thu Dec 22 14:31:01 +0000 2016</t>
+  </si>
+  <si>
+    <t>"RT තම්බි මරන්ඩ යනවනන් මටත් කෝල් එකක් දියන්"</t>
+  </si>
+  <si>
+    <t>810119174152454145</t>
+  </si>
+  <si>
+    <t>Sat Dec 17 13:47:17 +0000 2016</t>
+  </si>
+  <si>
+    <t>"RT මට කාවවත් 'හම්බ' උනෙත් නෑ... මම මීට පස්සේ මොකාවත් 'හම්බ' වෙන්නෙත් නෑ... ජිවිතේට 'හම්බ' කරන්නෙත් නෑ... මට ඔය 'හම්බයෝ' පේන්න බෑ &amp;gt;:("</t>
+  </si>
+  <si>
+    <t>810087877874892800</t>
+  </si>
+  <si>
+    <t>797374741140996100</t>
+  </si>
+  <si>
+    <t>Sat Dec 17 11:42:55 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@NeThU1191  ඒ කිය්න්නෙ දැන් චුට්ටකට කලින් අපේ පාරෙන් තම්බි සැට් එක දක්කන් ගිය හරක් සෙට් එකේ ඔයත් හිටියද"</t>
+  </si>
+  <si>
+    <t>807858922589683712</t>
+  </si>
+  <si>
+    <t>2787583639</t>
+  </si>
+  <si>
+    <t>Sun Dec 11 08:05:51 +0000 2016</t>
+  </si>
+  <si>
+    <t>"ප්‍රශ්ණයක් වුණත් කිව්වේ නැත්නම් නැටවෙන්න අහන්නෙම නෑමයි නේ බං මේ රටේ හැත්ත"</t>
+  </si>
+  <si>
+    <t>807378587170914304</t>
+  </si>
+  <si>
+    <t>2431399224</t>
+  </si>
+  <si>
+    <t>Sat Dec 10 00:17:10 +0000 2016</t>
+  </si>
+  <si>
+    <t>"හම්බයෝ ලංකාවේ නැගෙනහිර පළාතේ වෙනම රාජ්ජයක් පිහිටුවාගෙන කරන්න යන දේ https://t.co/VBc0LjKdFY via @YouTube"</t>
+  </si>
+  <si>
+    <t>807114366944415744</t>
+  </si>
+  <si>
+    <t>768317565412093952</t>
+  </si>
+  <si>
+    <t>Fri Dec 09 06:47:15 +0000 2016</t>
+  </si>
+  <si>
+    <t>"උරෙක් නිසා කාටුනයක් හලාල් වෙලා…. https://t.co/CverUxW0KJ"</t>
+  </si>
+  <si>
+    <t>807085138190467072</t>
+  </si>
+  <si>
+    <t>Fri Dec 09 04:51:06 +0000 2016</t>
+  </si>
+  <si>
+    <t>"ඌරා නිසා මුස්ලිම් අයට Peppa Pig එපාලු..! හලාල් කාටූන් එයි..! (VIDEO)  https://t.co/0BwgLH9twR https://t.co/NrEb2hxrTO"</t>
+  </si>
+  <si>
+    <t>806819072931303424</t>
+  </si>
+  <si>
+    <t>Thu Dec 08 11:13:51 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@IsuruSam තමන්ගෙ සතුටක හොඳක ගුණ නොහොයන හැත්ත වලියට නම් පොර කාගෙන. මං පඩේකට මායිම් කරන්නෙ නෑ"</t>
+  </si>
+  <si>
+    <t>806516139056476160</t>
+  </si>
+  <si>
+    <t>2990685931</t>
+  </si>
+  <si>
+    <t>Wed Dec 07 15:10:06 +0000 2016</t>
+  </si>
+  <si>
+    <t>"දන්න කියන සේරෝම ඇක්සසයිස් කොරල යන්තං සන්තං කිලෝ හතරක් අඩු කර ගත්තා. යකෝ කරුමේ කියන්නේ මෙලෝ මිනිහෙක් ඒක විස්වාස කරන්නෑ නේ ඕයි කුහක හැත්ත...!"</t>
+  </si>
+  <si>
+    <t>806512822599307264</t>
+  </si>
+  <si>
+    <t>4296682354</t>
+  </si>
+  <si>
+    <t>Wed Dec 07 14:56:55 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@IAyeshwanthe  තෝ කට වහපං හම්බය."</t>
+  </si>
+  <si>
+    <t>806116087712583680</t>
+  </si>
+  <si>
+    <t>2939388553</t>
+  </si>
+  <si>
+    <t>Tue Dec 06 12:40:26 +0000 2016</t>
+  </si>
+  <si>
+    <t>"බේබදු හැත්ත 😳😳😳 අදත් 😕😖 — feeling hurt"</t>
+  </si>
+  <si>
+    <t>802199277145563136</t>
+  </si>
+  <si>
+    <t>805933899314589696</t>
+  </si>
+  <si>
+    <t>Tue Dec 06 00:36:29 +0000 2016</t>
+  </si>
+  <si>
+    <t>"හම්බයෝ ලංකාවේ නැගෙනහිර පළාතේ වෙනම රාජ්ජයක්"</t>
+  </si>
+  <si>
+    <t>805933897901101056</t>
+  </si>
+  <si>
+    <t>"I added a video to a @YouTube playlist https://t.co/oc0xxYU9A6 හම්බයෝ ලංකාවේ නැගෙනහිර"</t>
+  </si>
+  <si>
+    <t>805922499582013440</t>
+  </si>
+  <si>
+    <t>755381592</t>
+  </si>
+  <si>
+    <t>Mon Dec 05 23:51:11 +0000 2016</t>
+  </si>
+  <si>
+    <t>"හම්බයෝ ලංකාවේ නැගෙනහිර පළාතට කරන්න යන දේ 3:) :'( https://t.co/4r3OXNsYlE"</t>
+  </si>
+  <si>
+    <t>805494933402439680</t>
+  </si>
+  <si>
+    <t>3401962264</t>
+  </si>
+  <si>
+    <t>Sun Dec 04 19:32:12 +0000 2016</t>
+  </si>
+  <si>
+    <t>"ළදරුවන්ට හුකන්න ඉල්ලන තම්බි පරයන් ගැන YAMU කට්ටියේ අදහස් https://t.co/WXv27j3T94"</t>
+  </si>
+  <si>
+    <t>805206952590577669</t>
+  </si>
+  <si>
+    <t>763040930962153472</t>
+  </si>
+  <si>
+    <t>Sun Dec 04 00:27:52 +0000 2016</t>
+  </si>
+  <si>
+    <t>"මෙන්න මෙකට උත්තර දිපල්ලා බලන්න තම්බි... https://t.co/Y55os7p4hD"</t>
+  </si>
+  <si>
+    <t>805061543691833344</t>
+  </si>
+  <si>
+    <t>357995892</t>
+  </si>
+  <si>
+    <t>Sat Dec 03 14:50:03 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@Ashenr2 lets be the change. මේ නාකි හැත්ත මැරිලා ගියාම බලමුකෝ 😹😹😹"</t>
+  </si>
+  <si>
+    <t>805001045923471360</t>
+  </si>
+  <si>
+    <t>1579738386</t>
+  </si>
+  <si>
+    <t>Sat Dec 03 10:49:40 +0000 2016</t>
+  </si>
+  <si>
+    <t>"තෙරුම් ගනින් අපේ උන්මයි අපේ ජාතියට ආගමට කෙලින්නේ පර හැත්ත... https://t.co/fQZyPH0IFG"</t>
+  </si>
+  <si>
+    <t>804894089019871232</t>
+  </si>
+  <si>
+    <t>2765974958</t>
+  </si>
+  <si>
+    <t>Sat Dec 03 03:44:39 +0000 2016</t>
+  </si>
+  <si>
+    <t>"මෙහෙවු රටේ තමයි පර ජාතික හැත්ත දැන් උඩු බුරන්නෙ https://t.co/Xhh14J0BpN"</t>
+  </si>
+  <si>
+    <t>804584633815986176</t>
+  </si>
+  <si>
+    <t>2741905841</t>
+  </si>
+  <si>
+    <t>Fri Dec 02 07:14:59 +0000 2016</t>
+  </si>
+  <si>
+    <t>"Private බස් වර්ජනය කරානම් හරි.. මෝඩ හැත්ත..."</t>
+  </si>
+  <si>
+    <t>804355221140992001</t>
+  </si>
+  <si>
+    <t>2387310594</t>
+  </si>
+  <si>
+    <t>Thu Dec 01 16:03:23 +0000 2016</t>
+  </si>
+  <si>
+    <t>"තම්බි හැත්ත මක බෑවිලා පල..සිංහලයන්ට කලගුණ මතක නැතිකම තමා ලොකුම අඩුව. — feeling මකබෑවිලා පල"</t>
+  </si>
+  <si>
+    <t>804217228581158914</t>
+  </si>
+  <si>
+    <t>2477102623</t>
+  </si>
+  <si>
+    <t>Thu Dec 01 06:55:03 +0000 2016</t>
+  </si>
+  <si>
+    <t>"පාර්ලිමේන්තුවෙ ඉන්න හැත්ත බුරුත්ත තමන්ගේ ගාන වැඩි කරගත්තා  හැන්ද තියෙන එකා තමන්ට ලොකු හැන්දෙනුත් අනිත් එවුන්ට කන් හැන්දෙනුත් බෙදනවා කියන්නේ"</t>
+  </si>
+  <si>
+    <t>804210303088984064</t>
+  </si>
+  <si>
+    <t>Thu Dec 01 06:27:32 +0000 2016</t>
+  </si>
+  <si>
+    <t>"@ib_banz එකත් එකක් 😂  බස් එකෙ ඉන්න උන් කෑගහන්න ගනි තොපි විලිලැජ්ජාවක් නැති පර හැත්ත අරකයි මෙකයි කියලා 😂😂😂😂😂"</t>
+  </si>
+  <si>
+    <t>682647745321017344</t>
+  </si>
+  <si>
+    <t>2569552316</t>
+  </si>
+  <si>
+    <t>Thu Dec 31 19:41:20 +0000 2015</t>
+  </si>
+  <si>
+    <t>"එක්සත් අරාබි එමිර් රාජ්‍යයේ ඩුබායි නුවර උස් ගොඩනැගිල්ලක මහා ගින්නක් ඇතිවි ඇති බව වාර්තාවේ.මේ වන විට 14 දෙනෙකු සුළු තුවාල ලබා ඇත.#lka"</t>
+  </si>
+  <si>
+    <t>682636430661795841</t>
+  </si>
+  <si>
+    <t>Thu Dec 31 18:56:22 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @ranjanieguruge: @MaithripalaS යුධ හමුදාව 50% කින් අඩු කිරීමට ඇමෙරිකාවට යමපාලනය පොරොන්දු වෙයි.  සිංහල රණවිරුවෝ දංගෙඩියට - කොටි රජගෙට htt…"</t>
+  </si>
+  <si>
+    <t>682461619343986688</t>
+  </si>
+  <si>
+    <t>2773119895</t>
+  </si>
+  <si>
+    <t>Thu Dec 31 07:21:44 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කොටි සතුව තිබූ අවි තොග ගැන විශේෂ අධිකරණයට තොරතුරු කියන්න පිරිසක්‌ සූදානම් -  https://t.co/BjSjzNRNhf"</t>
+  </si>
+  <si>
+    <t>682440099196473349</t>
+  </si>
+  <si>
+    <t>859641008</t>
+  </si>
+  <si>
+    <t>Thu Dec 31 05:56:13 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කෝ මේ අනන් මනං කියවපු හැත්ත 😒😒 මම කිව්වනේ අද දිනනවා කියලා 💪💪💪💪"</t>
+  </si>
+  <si>
+    <t>682427221886255104</t>
+  </si>
+  <si>
+    <t>4660634476</t>
+  </si>
+  <si>
+    <t>Thu Dec 31 05:05:03 +0000 2015</t>
+  </si>
+  <si>
+    <t>"nago nagoo.....හිතට වදින අරාබි ගායනයක් බලන්න...: https://t.co/GfN81GB330"</t>
+  </si>
+  <si>
+    <t>682347290439323648</t>
+  </si>
+  <si>
+    <t>1338509876</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 23:47:26 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කොටි සතුව තිබූ අවි තොග ගැන විශේෂ අධිකරණයට තොරතුරු කියන්න පිරිසක්‌ සූදානම්.. සම්පූර්ණ විස්තරය මෙතනින් කියවන්න &amp;gt;&amp;gt;... https://t.co/JFblWe8JcC"</t>
+  </si>
+  <si>
+    <t>682202164077445120</t>
+  </si>
+  <si>
+    <t>1655800231</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 14:10:45 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @greatgalle: බහරේන් රාජ්‍යයට අයත් F 16 ප්‍රහාරක ජෙට් යානයක් සෞදි අරාබි යේමන දේශ සිමාවට කඩාවැටි ඇති බව වාර්තාවේ.#lka #SriLanka"</t>
+  </si>
+  <si>
+    <t>682165065760428032</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 11:43:20 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කෝ මේ නුවර හැත්ත 😂😂😂"</t>
+  </si>
+  <si>
+    <t>682118957667454976</t>
+  </si>
+  <si>
+    <t>2782237856</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 08:40:07 +0000 2015</t>
+  </si>
+  <si>
+    <t>"පුරාණ රජමහා විහාරය ඉදිරිපස අරාබි පාසලක් හදයි. | සිංහල බෞද්ධයා https://t.co/1kQlJ3GgvX"</t>
+  </si>
+  <si>
+    <t>682051784680931328</t>
+  </si>
+  <si>
+    <t>4553302515</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 04:13:12 +0000 2015</t>
+  </si>
+  <si>
+    <t>"භූත ආත්මයක් නිසා කොටි 3ක් නැති කරගත් බිරිඳ  Read More&amp;gt;&amp;gt;&amp;gt; https://t.co/1HwbMr7WqT"</t>
+  </si>
+  <si>
+    <t>681997473708036097</t>
+  </si>
+  <si>
+    <t>107109153</t>
+  </si>
+  <si>
+    <t>Wed Dec 30 00:37:23 +0000 2015</t>
+  </si>
+  <si>
+    <t>"@imran226 අනේ ගොබ්බයො අහපන් කතාව මුල ඉදන් අග වෙනකන්, මහ ලොකු ඇත්ත කිව්ව එකා දිවුරන්න එපැයි අල්ලාගෙ පොතේ අත තියලා. ඕවා කියහන් අරාබි මොඩයන්ට."</t>
+  </si>
+  <si>
+    <t>681896214837723136</t>
+  </si>
+  <si>
+    <t>968590231</t>
+  </si>
+  <si>
+    <t>Tue Dec 29 17:55:01 +0000 2015</t>
+  </si>
+  <si>
+    <t>"ජනවාරි අට වෙනිද මුන්ගේ අලි/කොටි කුමන්තුනයට රැවටිලා මහින්දට රිදවන්න ගිහින් මෝඩ සිංහලයෝ පැරදුනා,..ඒකේ පුථිඵල දැන්... https://t.co/NsgNDt6kvS"</t>
+  </si>
+  <si>
+    <t>681830771968077825</t>
+  </si>
+  <si>
+    <t>2356608355</t>
+  </si>
+  <si>
+    <t>Tue Dec 29 13:34:58 +0000 2015</t>
+  </si>
+  <si>
+    <t>"මේ #ෆ්බි එකේ ඉන්න අසහන හැත්ත පාඩුවේ ඉඩපල්ලා හු**ටෝ,,  මගේ චුටි නංගි මෝන පෝටෝ දාලා තිබ්බත් #තෝපිට මෝකද අසහන හැත්ත,... https://t.co/pKFQgmYayb"</t>
+  </si>
+  <si>
+    <t>4195213480</t>
+  </si>
+  <si>
+    <t>2494979057</t>
+  </si>
+  <si>
+    <t>681541404527620096</t>
+  </si>
+  <si>
+    <t>432236442</t>
+  </si>
+  <si>
+    <t>Mon Dec 28 18:25:07 +0000 2015</t>
+  </si>
+  <si>
+    <t>"රිෂාඩ් ගස්වැද්දා කියන විදිහට ඒ හිවලා තමයි කොටි එල්වලා තියෙන්නේ ... මන්නාරමේ... අනේ හිවලෝ තර්කානුකූලව තමුන් පරාදයි.. තවත් කියවිලි ඕනී නැහැ.."</t>
+  </si>
+  <si>
+    <t>681494501597122560</t>
+  </si>
+  <si>
+    <t>2545283606</t>
+  </si>
+  <si>
+    <t>Mon Dec 28 15:18:45 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @sraddhabuddhi: වසර 15 කට පසු කොටි නඩුවක් විභාගයට https://t.co/7LXTrpNLC4 via @lankadeepa"</t>
+  </si>
+  <si>
+    <t>681425676969181184</t>
+  </si>
+  <si>
+    <t>3054580129</t>
+  </si>
+  <si>
+    <t>Mon Dec 28 10:45:16 +0000 2015</t>
+  </si>
+  <si>
+    <t>"වසර 15 කට පසු කොටි නඩුවක් විභාගයට:  පලාලි සිට රත්මලාන දක්වා පියාසර කරමින් තිබු ඇන්ටනෝව් 32 යානයකට ... https://t.co/rMqzjzervC #lka #news"</t>
+  </si>
+  <si>
+    <t>774055057</t>
+  </si>
+  <si>
+    <t>681395144717893632</t>
+  </si>
+  <si>
+    <t>Mon Dec 28 08:43:56 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @sraddhabuddhi: කොටි නායකයාගේ පුවරු තමිල්නාඩුවේ චෙන්නායි නුවර https://t.co/7Q4vneDJ7S"</t>
+  </si>
+  <si>
+    <t>681371661807976448</t>
+  </si>
+  <si>
+    <t>605766432</t>
+  </si>
+  <si>
+    <t>Mon Dec 28 07:10:38 +0000 2015</t>
+  </si>
+  <si>
+    <t>"'නිකරුණේ රඳවාගෙන සිටින කොටි සැකකරුවන් වහාම නිදහස් කළ යුතුයි' - කාදිනල් තුමා - Colombo Today https://t.co/jXX9M6SC8K"</t>
+  </si>
+  <si>
+    <t>681119037405835264</t>
+  </si>
+  <si>
+    <t>314032855</t>
+  </si>
+  <si>
+    <t>Sun Dec 27 14:26:47 +0000 2015</t>
+  </si>
+  <si>
+    <t>"@KaluMallii කොටි බ්‍රා නැද්ද?😺"</t>
+  </si>
+  <si>
+    <t>681069464071176192</t>
+  </si>
+  <si>
+    <t>43835089</t>
+  </si>
+  <si>
+    <t>Sun Dec 27 11:09:48 +0000 2015</t>
+  </si>
+  <si>
+    <t>"අන්තර්ජාතික කොටි ඩයස්පෝරාව සතු ඩොලර් මිලියණ ගණනක ධනස්කන්ධයක් පිළිබඳව පුවත් වාර්ථා පලවුනි. යහපාලන ආණ්ඩුව ඕනෑම... https://t.co/blAHKFifA9"</t>
+  </si>
+  <si>
+    <t>680976101385048068</t>
+  </si>
+  <si>
+    <t>Sun Dec 27 04:58:49 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @nirowa74: මේ තව අලුත් කොටි පැටව්  අල්ලලා පෙන්වනවාද ??? https://t.co/RRrzdkl0He"</t>
+  </si>
+  <si>
+    <t>680976079763451905</t>
+  </si>
+  <si>
+    <t>Sun Dec 27 04:58:43 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @nirowa74: දැක්කේ නෑ කිව්ව නිසා දැම්මේ. දැන් ඉතින් කොටි අල්ලලා පෙන්වන්න !!! https://t.co/p5dR5Qa6CV"</t>
+  </si>
+  <si>
+    <t>680949689840197633</t>
+  </si>
+  <si>
+    <t>Sun Dec 27 03:13:52 +0000 2015</t>
+  </si>
+  <si>
+    <t>680817815943798785</t>
+  </si>
+  <si>
+    <t>2610566038</t>
+  </si>
+  <si>
+    <t>Sat Dec 26 18:29:50 +0000 2015</t>
+  </si>
+  <si>
+    <t>"අපි කොන්ඩෙ වැව්වහම තමා කටත් අමරුව උන්ගෙ ලමයි කොන්ඩෙ වැව්වටට කන විද්දට කොන්ඩෙ ඩයිකරට කරාබු දම්මට කිසී ප්‍රශ්නයක් නෑ නෙදකින් ගම් වල ඉන්න හැත්ත"</t>
+  </si>
+  <si>
+    <t>680767553669476352</t>
+  </si>
+  <si>
+    <t>2274598537</t>
+  </si>
+  <si>
+    <t>Sat Dec 26 15:10:07 +0000 2015</t>
+  </si>
+  <si>
+    <t>"සිංහ ලේ නෙවෙයි ගොං බෙටි කියලා ගහගනියව් මෝඩ හැත්ත."</t>
+  </si>
+  <si>
+    <t>680750527936860160</t>
+  </si>
+  <si>
+    <t>Sat Dec 26 14:02:28 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @sraddhabuddhi: කොටි වැනසූ රණවිරුවන් ගස් යවන  යුද අපරාධ විමර්ශන විශේෂ පනත එයි https://t.co/SOJtf6M8XM"</t>
+  </si>
+  <si>
+    <t>680692203400884224</t>
+  </si>
+  <si>
+    <t>2836936358</t>
+  </si>
+  <si>
+    <t>Sat Dec 26 10:10:42 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @Neetwit: බිලියනයක වත්කම් රාජ් රාජරත්නම්ට යළි දෙනවාට කොටි බෝම්බ මැරුම් කෑ අයගේ ඥාතීන්ගේ විරෝධය https://t.co/fKqzoflP5M #sriLanka #lka #G…"</t>
+  </si>
+  <si>
+    <t>680349152207835136</t>
+  </si>
+  <si>
+    <t>Fri Dec 25 11:27:32 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @Neetwit: මෛත්‍රී-රනිල් ආණ්ඩුව දෙමළ චන්ද අරන් දුන්න කොටි ඩයස්පෝරාව සතුටු කලා අපේ හමුදාවෙ අභිමානය බල්ලට! https://t.co/D0szymWyKO #sriLank…"</t>
+  </si>
+  <si>
+    <t>"RT @ApiWenuwen: අරාබි වසන්තය පාරා වළල්ලක්‌ වූ අයුරු https://t.co/uGEkW8WaaL @sampath201028 @sraddhabuddhi https://t.co/kKXvuhnsDK"</t>
+  </si>
+  <si>
+    <t>679966448182259712</t>
+  </si>
+  <si>
+    <t>Thu Dec 24 10:06:49 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @ranjanieguruge: වීරෝධාර රණවිරුවාණෙනි! ඔබ ට මෙසේ වන්නේ  දෙමළ කොටි බලයට අවනත ආණ්ඩුවක් නිසාය.  එය වෙස් මූනක් පමණයි. තෙරුවන් සරණයි. https:/…"</t>
+  </si>
+  <si>
+    <t>679897908502605824</t>
+  </si>
+  <si>
+    <t>Thu Dec 24 05:34:27 +0000 2015</t>
+  </si>
+  <si>
+    <t>"හිටපු කොටි සාමාජිකයෝ නත්තල් සමරති"</t>
+  </si>
+  <si>
+    <t>679897907558879233</t>
+  </si>
+  <si>
+    <t>"හිටපු කොටි සාමාජිකයෝ නත්තල් සමරති:  පැරණි කොටි සාමාජිකයන් පුනරුත්ථාපනය කරන වව්නියා පුනරුත්ථාපන කඳවුරේ දි නත්තල් සැමරීම බදාදා රාත්‍රී..."</t>
+  </si>
+  <si>
+    <t>679805234881925120</t>
+  </si>
+  <si>
+    <t>Wed Dec 23 23:26:12 +0000 2015</t>
+  </si>
+  <si>
+    <t>679697058199158784</t>
+  </si>
+  <si>
+    <t>Wed Dec 23 16:16:21 +0000 2015</t>
+  </si>
+  <si>
+    <t>"ශ්‍රී ලාංකික කාන්තාවකට ගල් ගසා මරා දැමීම සඳහා නියම කෙරුණ අධිකරණ නියෝගය සෞදි අරාබි බලධාරීන් විසින් ඉවත් කර ගෙන ඇති බව ශ්‍රී ලංකා රජය පවසයි."</t>
+  </si>
+  <si>
+    <t>679592748559806464</t>
+  </si>
+  <si>
+    <t>Wed Dec 23 09:21:52 +0000 2015</t>
+  </si>
+  <si>
+    <t>"@IAmMrHumorist ඈහ්?වෙන කවුද කොටි පැන්නුවෙ? 😳"</t>
+  </si>
+  <si>
+    <t>679592201383489536</t>
+  </si>
+  <si>
+    <t>Wed Dec 23 09:19:41 +0000 2015</t>
+  </si>
+  <si>
+    <t>"@IAmMrHumorist @dilchaaa_ මහින්ද මාමි කොටි පැන්නුවා 😇"</t>
+  </si>
+  <si>
+    <t>679556472716537856</t>
+  </si>
+  <si>
+    <t>1142062112</t>
+  </si>
+  <si>
+    <t>Wed Dec 23 06:57:43 +0000 2015</t>
+  </si>
+  <si>
+    <t>"😇😈󾌾   Truth First - Lanka su Twitter: "සුප්පා යහපාලනයමතකද කොලබට කිරි ගමට කැකිරි කිව්ව හැත්ත සෞඛ්‍ය අමාත්‍යංශය... https://t.co/v1yX94D1n8"</t>
+  </si>
+  <si>
+    <t>679349919367471108</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 17:16:57 +0000 2015</t>
+  </si>
+  <si>
+    <t>679144661873786880</t>
+  </si>
+  <si>
+    <t>Tue Dec 22 03:41:19 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කොටි යළි අරක් ගනී ! හමුදා නායකයන් දංගෙඩියට දක්කන්න මෙහෙයුම් ! - https://t.co/4EMcAu9dop via @Shareaholic"</t>
+  </si>
+  <si>
+    <t>678887871168704513</t>
+  </si>
+  <si>
+    <t>Mon Dec 21 10:40:56 +0000 2015</t>
+  </si>
+  <si>
+    <t>"දෙමළ - සිංහල සැකකරුවෝ 27ක් යළි රිමාන්ඩ්:  ත්‍රස්තවාදය වැළැක්වීමේ පනත යටතේ රඳවාගෙන සිටි දෙමළ හා සිංහල කොටි සැකකරුවෝ 27 දෙනෙක් කොළඹ අත..."</t>
+  </si>
+  <si>
+    <t>678877952533209088</t>
+  </si>
+  <si>
+    <t>Mon Dec 21 10:01:31 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @sraddhabuddhi: සාමය උදාකළ මහින්දට කොටි පැරදවීමට හැකි වූයේත්  ඔය "අන්තවාදීන්"ට  සවන් දීම නිසා බව අමතක නොකරමු! https://t.co/KSW7D6kc8h vi…"</t>
+  </si>
+  <si>
+    <t>678861010976055296</t>
+  </si>
+  <si>
+    <t>Mon Dec 21 08:54:12 +0000 2015</t>
+  </si>
+  <si>
+    <t>678796230126866433</t>
+  </si>
+  <si>
+    <t>Mon Dec 21 04:36:47 +0000 2015</t>
+  </si>
+  <si>
+    <t>"කාට හරි මගේ බඩ කෑගහන සද්දෙ ඇහුනොත් ෂුවර් එකටම හිතයි කොටි නැගිටලා කියලා"</t>
+  </si>
+  <si>
+    <t>678400462069096448</t>
+  </si>
+  <si>
+    <t>Sun Dec 20 02:24:08 +0000 2015</t>
+  </si>
+  <si>
+    <t>"මෙම පනත අහෝසි කිරීමත් සමඟ ත්‍රස්‌ත මර්දන පනත යටතේ රඳවාගෙන ඇති හිටපු කොටි ක්‍රියාකාරීන් ද නිදහස්‌ වනු ඇත. @surendirans @GTFonline"</t>
+  </si>
+  <si>
+    <t>678276511414116352</t>
+  </si>
+  <si>
+    <t>Sat Dec 19 18:11:36 +0000 2015</t>
+  </si>
+  <si>
+    <t>"RT @ranjanieguruge: @MaithripalaS ඔබට ස්තුති කොටි එලියේ රනවිරුවෝ පෝරකයට??? https://t.co/140Mg6MD6t"</t>
+  </si>
+  <si>
+    <t>1090038963409244162</t>
+  </si>
+  <si>
+    <t>Tue Jan 29 00:08:35 +0000 2019</t>
+  </si>
+  <si>
+    <t>"මේ තම්බි මනුස්සයා ඉඹින්නේ ජාතික කොඩියේ 'කොළ පාට (තම්බි මිනිස්සුන්ට අයිති පාට)' තියෙන තීරුව නේද? 🤔 https://t.co/uX0afCSlpI"</t>
   </si>
 </sst>
 </file>
@@ -15706,10 +16447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1295"/>
+  <dimension ref="A1:G1365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1284" workbookViewId="0">
-      <selection activeCell="E1295" sqref="E1295"/>
+    <sheetView tabSelected="1" topLeftCell="A1353" workbookViewId="0">
+      <selection activeCell="E1365" sqref="E1365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45627,6 +46368,1406 @@
         <v>217</v>
       </c>
     </row>
+    <row r="1296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1296" s="16" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B1296" s="16" t="s">
+        <v>5071</v>
+      </c>
+      <c r="C1296" s="16" t="s">
+        <v>3159</v>
+      </c>
+      <c r="D1296" s="16" t="s">
+        <v>5072</v>
+      </c>
+      <c r="E1296" s="16" t="s">
+        <v>5073</v>
+      </c>
+      <c r="F1296" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1297" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1297" s="16" t="s">
+        <v>5074</v>
+      </c>
+      <c r="C1297" s="16" t="s">
+        <v>5009</v>
+      </c>
+      <c r="D1297" s="16" t="s">
+        <v>5075</v>
+      </c>
+      <c r="E1297" s="16" t="s">
+        <v>5076</v>
+      </c>
+      <c r="F1297" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1298" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="B1298" s="16" t="s">
+        <v>5077</v>
+      </c>
+      <c r="C1298" s="16" t="s">
+        <v>5078</v>
+      </c>
+      <c r="D1298" s="16" t="s">
+        <v>5079</v>
+      </c>
+      <c r="E1298" s="16" t="s">
+        <v>5080</v>
+      </c>
+      <c r="F1298" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1299" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1299" s="16" t="s">
+        <v>5081</v>
+      </c>
+      <c r="C1299" s="16" t="s">
+        <v>5078</v>
+      </c>
+      <c r="D1299" s="16" t="s">
+        <v>5082</v>
+      </c>
+      <c r="E1299" s="16" t="s">
+        <v>5083</v>
+      </c>
+      <c r="F1299" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1300" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="B1300" s="16" t="s">
+        <v>5084</v>
+      </c>
+      <c r="C1300" s="16" t="s">
+        <v>5085</v>
+      </c>
+      <c r="D1300" s="16" t="s">
+        <v>5086</v>
+      </c>
+      <c r="E1300" s="16" t="s">
+        <v>5087</v>
+      </c>
+      <c r="F1300" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1301" s="16" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B1301" s="16" t="s">
+        <v>5088</v>
+      </c>
+      <c r="C1301" s="16" t="s">
+        <v>5089</v>
+      </c>
+      <c r="D1301" s="16" t="s">
+        <v>5090</v>
+      </c>
+      <c r="E1301" s="16" t="s">
+        <v>5091</v>
+      </c>
+      <c r="F1301" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1302" s="16" t="s">
+        <v>2035</v>
+      </c>
+      <c r="B1302" s="16" t="s">
+        <v>5092</v>
+      </c>
+      <c r="C1302" s="16" t="s">
+        <v>5093</v>
+      </c>
+      <c r="D1302" s="16" t="s">
+        <v>5094</v>
+      </c>
+      <c r="E1302" s="16" t="s">
+        <v>5095</v>
+      </c>
+      <c r="F1302" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1303" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1303" s="16" t="s">
+        <v>5096</v>
+      </c>
+      <c r="C1303" s="16" t="s">
+        <v>5097</v>
+      </c>
+      <c r="D1303" s="16" t="s">
+        <v>5098</v>
+      </c>
+      <c r="E1303" s="16" t="s">
+        <v>5099</v>
+      </c>
+      <c r="F1303" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1304" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1304" s="16" t="s">
+        <v>5100</v>
+      </c>
+      <c r="C1304" s="16" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D1304" s="16" t="s">
+        <v>5101</v>
+      </c>
+      <c r="E1304" s="16" t="s">
+        <v>5102</v>
+      </c>
+      <c r="F1304" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1305" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1305" s="16" t="s">
+        <v>5103</v>
+      </c>
+      <c r="C1305" s="16" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D1305" s="16" t="s">
+        <v>5104</v>
+      </c>
+      <c r="E1305" s="16" t="s">
+        <v>5105</v>
+      </c>
+      <c r="F1305" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1306" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1306" s="16" t="s">
+        <v>5106</v>
+      </c>
+      <c r="C1306" s="16" t="s">
+        <v>5107</v>
+      </c>
+      <c r="D1306" s="16" t="s">
+        <v>5108</v>
+      </c>
+      <c r="E1306" s="16" t="s">
+        <v>5109</v>
+      </c>
+      <c r="F1306" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1307" s="16" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B1307" s="16" t="s">
+        <v>5110</v>
+      </c>
+      <c r="C1307" s="16" t="s">
+        <v>5111</v>
+      </c>
+      <c r="D1307" s="16" t="s">
+        <v>5112</v>
+      </c>
+      <c r="E1307" s="16" t="s">
+        <v>5113</v>
+      </c>
+      <c r="F1307" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1308" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B1308" s="16" t="s">
+        <v>5114</v>
+      </c>
+      <c r="C1308" s="16" t="s">
+        <v>5115</v>
+      </c>
+      <c r="D1308" s="16" t="s">
+        <v>5116</v>
+      </c>
+      <c r="E1308" s="16" t="s">
+        <v>5117</v>
+      </c>
+      <c r="F1308" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1309" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1309" s="16" t="s">
+        <v>5119</v>
+      </c>
+      <c r="C1309" s="16" t="s">
+        <v>5118</v>
+      </c>
+      <c r="D1309" s="16" t="s">
+        <v>5120</v>
+      </c>
+      <c r="E1309" s="16" t="s">
+        <v>5121</v>
+      </c>
+      <c r="F1309" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1310" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1310" s="16" t="s">
+        <v>5122</v>
+      </c>
+      <c r="C1310" s="16" t="s">
+        <v>5118</v>
+      </c>
+      <c r="D1310" s="16" t="s">
+        <v>5120</v>
+      </c>
+      <c r="E1310" s="16" t="s">
+        <v>5123</v>
+      </c>
+      <c r="F1310" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1311" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1311" s="16" t="s">
+        <v>5124</v>
+      </c>
+      <c r="C1311" s="16" t="s">
+        <v>5125</v>
+      </c>
+      <c r="D1311" s="16" t="s">
+        <v>5126</v>
+      </c>
+      <c r="E1311" s="16" t="s">
+        <v>5127</v>
+      </c>
+      <c r="F1311" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1312" s="16" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B1312" s="16" t="s">
+        <v>5128</v>
+      </c>
+      <c r="C1312" s="16" t="s">
+        <v>5129</v>
+      </c>
+      <c r="D1312" s="16" t="s">
+        <v>5130</v>
+      </c>
+      <c r="E1312" s="16" t="s">
+        <v>5131</v>
+      </c>
+      <c r="F1312" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1313" s="16" t="s">
+        <v>423</v>
+      </c>
+      <c r="B1313" s="16" t="s">
+        <v>5132</v>
+      </c>
+      <c r="C1313" s="16" t="s">
+        <v>5133</v>
+      </c>
+      <c r="D1313" s="16" t="s">
+        <v>5134</v>
+      </c>
+      <c r="E1313" s="16" t="s">
+        <v>5135</v>
+      </c>
+      <c r="F1313" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1314" s="16" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B1314" s="16" t="s">
+        <v>5136</v>
+      </c>
+      <c r="C1314" s="16" t="s">
+        <v>5137</v>
+      </c>
+      <c r="D1314" s="16" t="s">
+        <v>5138</v>
+      </c>
+      <c r="E1314" s="16" t="s">
+        <v>5139</v>
+      </c>
+      <c r="F1314" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1315" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="B1315" s="16" t="s">
+        <v>5140</v>
+      </c>
+      <c r="C1315" s="16" t="s">
+        <v>5141</v>
+      </c>
+      <c r="D1315" s="16" t="s">
+        <v>5142</v>
+      </c>
+      <c r="E1315" s="11" t="s">
+        <v>5143</v>
+      </c>
+      <c r="F1315" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1316" s="16" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1316" s="16" t="s">
+        <v>5144</v>
+      </c>
+      <c r="C1316" s="16" t="s">
+        <v>5145</v>
+      </c>
+      <c r="D1316" s="16" t="s">
+        <v>5146</v>
+      </c>
+      <c r="E1316" s="11" t="s">
+        <v>5147</v>
+      </c>
+      <c r="F1316" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1317" s="16" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B1317" s="16" t="s">
+        <v>5148</v>
+      </c>
+      <c r="C1317" s="16" t="s">
+        <v>5149</v>
+      </c>
+      <c r="D1317" s="16" t="s">
+        <v>5150</v>
+      </c>
+      <c r="E1317" s="16" t="s">
+        <v>5151</v>
+      </c>
+      <c r="F1317" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1318" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="B1318" s="16" t="s">
+        <v>5152</v>
+      </c>
+      <c r="C1318" s="16" t="s">
+        <v>5153</v>
+      </c>
+      <c r="D1318" s="16" t="s">
+        <v>5154</v>
+      </c>
+      <c r="E1318" s="16" t="s">
+        <v>5155</v>
+      </c>
+      <c r="F1318" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1319" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="B1319" s="16" t="s">
+        <v>5156</v>
+      </c>
+      <c r="C1319" s="16" t="s">
+        <v>5157</v>
+      </c>
+      <c r="D1319" s="16" t="s">
+        <v>5158</v>
+      </c>
+      <c r="E1319" s="16" t="s">
+        <v>5159</v>
+      </c>
+      <c r="F1319" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1320" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="B1320" s="16" t="s">
+        <v>5160</v>
+      </c>
+      <c r="C1320" s="16" t="s">
+        <v>5009</v>
+      </c>
+      <c r="D1320" s="16" t="s">
+        <v>5161</v>
+      </c>
+      <c r="E1320" s="16" t="s">
+        <v>5162</v>
+      </c>
+      <c r="F1320" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1321" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1321" s="16" t="s">
+        <v>5163</v>
+      </c>
+      <c r="C1321" s="16" t="s">
+        <v>5164</v>
+      </c>
+      <c r="D1321" s="16" t="s">
+        <v>5165</v>
+      </c>
+      <c r="E1321" s="16" t="s">
+        <v>5166</v>
+      </c>
+      <c r="F1321" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1322" s="16" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B1322" s="16" t="s">
+        <v>5167</v>
+      </c>
+      <c r="C1322" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1322" s="16" t="s">
+        <v>5168</v>
+      </c>
+      <c r="E1322" s="11" t="s">
+        <v>5169</v>
+      </c>
+      <c r="F1322" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1323" s="16" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B1323" s="16" t="s">
+        <v>5170</v>
+      </c>
+      <c r="C1323" s="16" t="s">
+        <v>5171</v>
+      </c>
+      <c r="D1323" s="16" t="s">
+        <v>5172</v>
+      </c>
+      <c r="E1323" s="16" t="s">
+        <v>5173</v>
+      </c>
+      <c r="F1323" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1324" s="16" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B1324" s="16" t="s">
+        <v>5174</v>
+      </c>
+      <c r="C1324" s="16" t="s">
+        <v>5175</v>
+      </c>
+      <c r="D1324" s="16" t="s">
+        <v>5176</v>
+      </c>
+      <c r="E1324" s="16" t="s">
+        <v>5177</v>
+      </c>
+      <c r="F1324" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1325" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1325" s="16" t="s">
+        <v>5178</v>
+      </c>
+      <c r="C1325" s="16" t="s">
+        <v>5179</v>
+      </c>
+      <c r="D1325" s="16" t="s">
+        <v>5180</v>
+      </c>
+      <c r="E1325" s="16" t="s">
+        <v>5181</v>
+      </c>
+      <c r="F1325" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1326" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1326" s="16" t="s">
+        <v>5182</v>
+      </c>
+      <c r="C1326" s="16" t="s">
+        <v>5183</v>
+      </c>
+      <c r="D1326" s="16" t="s">
+        <v>5184</v>
+      </c>
+      <c r="E1326" s="16" t="s">
+        <v>5185</v>
+      </c>
+      <c r="F1326" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1327" s="16" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1327" s="16" t="s">
+        <v>5186</v>
+      </c>
+      <c r="C1327" s="16" t="s">
+        <v>5187</v>
+      </c>
+      <c r="D1327" s="16" t="s">
+        <v>5188</v>
+      </c>
+      <c r="E1327" s="16" t="s">
+        <v>5189</v>
+      </c>
+      <c r="F1327" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1328" s="16" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B1328" s="16" t="s">
+        <v>5190</v>
+      </c>
+      <c r="C1328" s="16" t="s">
+        <v>5175</v>
+      </c>
+      <c r="D1328" s="16" t="s">
+        <v>5191</v>
+      </c>
+      <c r="E1328" s="16" t="s">
+        <v>5192</v>
+      </c>
+      <c r="F1328" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1329" s="16" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B1329" s="16" t="s">
+        <v>5193</v>
+      </c>
+      <c r="C1329" s="16" t="s">
+        <v>5194</v>
+      </c>
+      <c r="D1329" s="16" t="s">
+        <v>5195</v>
+      </c>
+      <c r="E1329" s="16" t="s">
+        <v>5196</v>
+      </c>
+      <c r="F1329" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1330" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1330" s="16" t="s">
+        <v>5197</v>
+      </c>
+      <c r="C1330" s="16" t="s">
+        <v>5198</v>
+      </c>
+      <c r="D1330" s="16" t="s">
+        <v>5199</v>
+      </c>
+      <c r="E1330" s="16" t="s">
+        <v>5200</v>
+      </c>
+      <c r="F1330" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1331" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1331" s="16" t="s">
+        <v>5201</v>
+      </c>
+      <c r="C1331" s="16" t="s">
+        <v>5202</v>
+      </c>
+      <c r="D1331" s="16" t="s">
+        <v>5203</v>
+      </c>
+      <c r="E1331" s="16" t="s">
+        <v>5204</v>
+      </c>
+      <c r="F1331" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1332" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1332" s="16" t="s">
+        <v>5205</v>
+      </c>
+      <c r="C1332" s="16" t="s">
+        <v>5206</v>
+      </c>
+      <c r="D1332" s="16" t="s">
+        <v>5207</v>
+      </c>
+      <c r="E1332" s="11" t="s">
+        <v>5208</v>
+      </c>
+      <c r="F1332" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1333" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1333" s="16" t="s">
+        <v>5209</v>
+      </c>
+      <c r="C1333" s="16" t="s">
+        <v>5210</v>
+      </c>
+      <c r="D1333" s="16" t="s">
+        <v>5211</v>
+      </c>
+      <c r="E1333" s="16" t="s">
+        <v>5212</v>
+      </c>
+      <c r="F1333" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1334" s="16" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B1334" s="16" t="s">
+        <v>5215</v>
+      </c>
+      <c r="C1334" s="16" t="s">
+        <v>5216</v>
+      </c>
+      <c r="D1334" s="16" t="s">
+        <v>5217</v>
+      </c>
+      <c r="E1334" s="16" t="s">
+        <v>5218</v>
+      </c>
+      <c r="F1334" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1335" s="16" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B1335" s="16" t="s">
+        <v>5219</v>
+      </c>
+      <c r="C1335" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1335" s="16" t="s">
+        <v>5221</v>
+      </c>
+      <c r="E1335" s="16" t="s">
+        <v>5222</v>
+      </c>
+      <c r="F1335" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1336" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1336" s="16" t="s">
+        <v>5223</v>
+      </c>
+      <c r="C1336" s="16" t="s">
+        <v>5224</v>
+      </c>
+      <c r="D1336" s="16" t="s">
+        <v>5225</v>
+      </c>
+      <c r="E1336" s="16" t="s">
+        <v>5226</v>
+      </c>
+      <c r="F1336" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1337" s="16" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B1337" s="16" t="s">
+        <v>5228</v>
+      </c>
+      <c r="C1337" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1337" s="16" t="s">
+        <v>5229</v>
+      </c>
+      <c r="E1337" s="16" t="s">
+        <v>5230</v>
+      </c>
+      <c r="F1337" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1338" s="16" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B1338" s="16" t="s">
+        <v>5231</v>
+      </c>
+      <c r="C1338" s="16" t="s">
+        <v>5232</v>
+      </c>
+      <c r="D1338" s="16" t="s">
+        <v>5233</v>
+      </c>
+      <c r="E1338" s="16" t="s">
+        <v>5234</v>
+      </c>
+      <c r="F1338" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1339" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1339" s="16" t="s">
+        <v>5235</v>
+      </c>
+      <c r="C1339" s="16" t="s">
+        <v>5236</v>
+      </c>
+      <c r="D1339" s="16" t="s">
+        <v>5237</v>
+      </c>
+      <c r="E1339" s="16" t="s">
+        <v>5238</v>
+      </c>
+      <c r="F1339" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1340" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1340" s="16" t="s">
+        <v>5239</v>
+      </c>
+      <c r="C1340" s="16" t="s">
+        <v>5240</v>
+      </c>
+      <c r="D1340" s="16" t="s">
+        <v>5241</v>
+      </c>
+      <c r="E1340" s="16" t="s">
+        <v>5242</v>
+      </c>
+      <c r="F1340" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1341" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1341" s="16" t="s">
+        <v>5243</v>
+      </c>
+      <c r="C1341" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1341" s="16" t="s">
+        <v>5244</v>
+      </c>
+      <c r="E1341" s="16" t="s">
+        <v>5245</v>
+      </c>
+      <c r="F1341" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1342" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1342" s="16" t="s">
+        <v>5246</v>
+      </c>
+      <c r="C1342" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1342" s="16" t="s">
+        <v>5247</v>
+      </c>
+      <c r="E1342" s="16" t="s">
+        <v>5248</v>
+      </c>
+      <c r="F1342" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1343" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1343" s="16" t="s">
+        <v>5249</v>
+      </c>
+      <c r="C1343" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1343" s="16" t="s">
+        <v>5250</v>
+      </c>
+      <c r="E1343" s="16" t="s">
+        <v>5248</v>
+      </c>
+      <c r="F1343" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1344" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1344" s="16" t="s">
+        <v>5251</v>
+      </c>
+      <c r="C1344" s="16" t="s">
+        <v>5252</v>
+      </c>
+      <c r="D1344" s="16" t="s">
+        <v>5253</v>
+      </c>
+      <c r="E1344" s="16" t="s">
+        <v>5254</v>
+      </c>
+      <c r="F1344" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1345" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1345" s="16" t="s">
+        <v>5255</v>
+      </c>
+      <c r="C1345" s="16" t="s">
+        <v>5256</v>
+      </c>
+      <c r="D1345" s="16" t="s">
+        <v>5257</v>
+      </c>
+      <c r="E1345" s="16" t="s">
+        <v>5258</v>
+      </c>
+      <c r="F1345" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1346" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1346" s="16" t="s">
+        <v>5259</v>
+      </c>
+      <c r="C1346" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1346" s="16" t="s">
+        <v>5260</v>
+      </c>
+      <c r="E1346" s="16" t="s">
+        <v>5261</v>
+      </c>
+      <c r="F1346" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1347" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1347" s="16" t="s">
+        <v>5262</v>
+      </c>
+      <c r="C1347" s="16" t="s">
+        <v>5263</v>
+      </c>
+      <c r="D1347" s="16" t="s">
+        <v>5264</v>
+      </c>
+      <c r="E1347" s="16" t="s">
+        <v>5265</v>
+      </c>
+      <c r="F1347" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1348" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1348" s="16" t="s">
+        <v>5266</v>
+      </c>
+      <c r="C1348" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1348" s="16" t="s">
+        <v>5267</v>
+      </c>
+      <c r="E1348" s="11" t="s">
+        <v>5268</v>
+      </c>
+      <c r="F1348" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1349" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1349" s="16" t="s">
+        <v>5270</v>
+      </c>
+      <c r="C1349" s="16" t="s">
+        <v>5213</v>
+      </c>
+      <c r="D1349" s="16" t="s">
+        <v>5271</v>
+      </c>
+      <c r="E1349" s="16" t="s">
+        <v>5272</v>
+      </c>
+      <c r="F1349" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1350" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1350" s="16" t="s">
+        <v>5273</v>
+      </c>
+      <c r="C1350" s="16" t="s">
+        <v>5227</v>
+      </c>
+      <c r="D1350" s="16" t="s">
+        <v>5274</v>
+      </c>
+      <c r="E1350" s="16" t="s">
+        <v>5275</v>
+      </c>
+      <c r="F1350" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1351" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1351" s="16" t="s">
+        <v>5276</v>
+      </c>
+      <c r="C1351" s="16" t="s">
+        <v>5227</v>
+      </c>
+      <c r="D1351" s="16" t="s">
+        <v>5274</v>
+      </c>
+      <c r="E1351" s="16" t="s">
+        <v>5277</v>
+      </c>
+      <c r="F1351" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1352" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1352" s="16" t="s">
+        <v>5278</v>
+      </c>
+      <c r="C1352" s="16" t="s">
+        <v>5214</v>
+      </c>
+      <c r="D1352" s="16" t="s">
+        <v>5279</v>
+      </c>
+      <c r="E1352" s="16" t="s">
+        <v>5272</v>
+      </c>
+      <c r="F1352" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1353" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1353" s="16" t="s">
+        <v>5280</v>
+      </c>
+      <c r="C1353" s="16" t="s">
+        <v>724</v>
+      </c>
+      <c r="D1353" s="16" t="s">
+        <v>5281</v>
+      </c>
+      <c r="E1353" s="16" t="s">
+        <v>5282</v>
+      </c>
+      <c r="F1353" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1354" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1354" s="16" t="s">
+        <v>5283</v>
+      </c>
+      <c r="C1354" s="16" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1354" s="16" t="s">
+        <v>5284</v>
+      </c>
+      <c r="E1354" s="16" t="s">
+        <v>5285</v>
+      </c>
+      <c r="F1354" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1355" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1355" s="16" t="s">
+        <v>5286</v>
+      </c>
+      <c r="C1355" s="16" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D1355" s="16" t="s">
+        <v>5287</v>
+      </c>
+      <c r="E1355" s="16" t="s">
+        <v>5288</v>
+      </c>
+      <c r="F1355" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1356" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1356" s="16" t="s">
+        <v>5289</v>
+      </c>
+      <c r="C1356" s="16" t="s">
+        <v>5290</v>
+      </c>
+      <c r="D1356" s="16" t="s">
+        <v>5291</v>
+      </c>
+      <c r="E1356" s="16" t="s">
+        <v>5292</v>
+      </c>
+      <c r="F1356" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1357" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1357" s="16" t="s">
+        <v>5293</v>
+      </c>
+      <c r="C1357" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1357" s="16" t="s">
+        <v>5294</v>
+      </c>
+      <c r="E1357" s="16" t="s">
+        <v>5269</v>
+      </c>
+      <c r="F1357" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1358" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1358" s="16" t="s">
+        <v>5295</v>
+      </c>
+      <c r="C1358" s="16" t="s">
+        <v>2850</v>
+      </c>
+      <c r="D1358" s="16" t="s">
+        <v>5296</v>
+      </c>
+      <c r="E1358" s="16" t="s">
+        <v>5297</v>
+      </c>
+      <c r="F1358" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1359" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1359" s="16" t="s">
+        <v>5298</v>
+      </c>
+      <c r="C1359" s="16" t="s">
+        <v>5227</v>
+      </c>
+      <c r="D1359" s="16" t="s">
+        <v>5299</v>
+      </c>
+      <c r="E1359" s="11" t="s">
+        <v>5300</v>
+      </c>
+      <c r="F1359" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1360" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="B1360" s="16" t="s">
+        <v>5301</v>
+      </c>
+      <c r="C1360" s="16" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D1360" s="16" t="s">
+        <v>5302</v>
+      </c>
+      <c r="E1360" s="16" t="s">
+        <v>5303</v>
+      </c>
+      <c r="F1360" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1361" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1361" s="16" t="s">
+        <v>5304</v>
+      </c>
+      <c r="C1361" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1361" s="16" t="s">
+        <v>5305</v>
+      </c>
+      <c r="E1361" s="16" t="s">
+        <v>5303</v>
+      </c>
+      <c r="F1361" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1362" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1362" s="16" t="s">
+        <v>5306</v>
+      </c>
+      <c r="C1362" s="16" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D1362" s="16" t="s">
+        <v>5307</v>
+      </c>
+      <c r="E1362" s="16" t="s">
+        <v>5308</v>
+      </c>
+      <c r="F1362" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1363" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1363" s="16" t="s">
+        <v>5309</v>
+      </c>
+      <c r="C1363" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1363" s="16" t="s">
+        <v>5310</v>
+      </c>
+      <c r="E1363" s="16" t="s">
+        <v>5311</v>
+      </c>
+      <c r="F1363" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1364" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B1364" s="16" t="s">
+        <v>5312</v>
+      </c>
+      <c r="C1364" s="16" t="s">
+        <v>5220</v>
+      </c>
+      <c r="D1364" s="16" t="s">
+        <v>5313</v>
+      </c>
+      <c r="E1364" s="16" t="s">
+        <v>5314</v>
+      </c>
+      <c r="F1364" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1365" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1365" s="16" t="s">
+        <v>5315</v>
+      </c>
+      <c r="C1365" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="D1365" s="16" t="s">
+        <v>5316</v>
+      </c>
+      <c r="E1365" s="16" t="s">
+        <v>5317</v>
+      </c>
+      <c r="F1365" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -45636,7 +47777,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211 A371:E470 A569:E576 A579:E580 A578:D578 A582:E641 A581:E581 A577:E577 A642:E643 A644:E645 A646:E658 A659:E693 A694:E746 A747:E756 A757:E757 A758:E766 A768:E786 A767:E767 A787:E788 A789:E789 A790:E790 A791:E792 A793:E795 A796:E799 A800:E843 A844:E854 A855:E866 A867:E868 A869:E895 A897:E900 A896:D896 A901:E935 A936:E942 A943:E945 A946:E954 A955:E974 A976:E977 A975:D975 A978:E980 A981:E986 A987:E996 A997:E1000 A1001:E1001 A1002:E1052 A1054:E1071 A1053:D1053 A1072:E1092 A1093:E1094 A1095:E1108 A1109:E1109 A1110:E1112 A1113:E1125 A1126:E1128 A1129:E1130 A1131:E1132 A1133:E1136 A1137:E1141 A1142:E1144 A1145:E1146 A1147:E1155 A1156:E1168 A1169:E1171 A1172:E1193 A1194:E1196 A1197:E1198 A1199:E1200 A1201:E1206 A1207:E1209 A1210:E1212 A1213:E1214 A1215:E1216 A1217:E1220 A1221:E1230 A1231:E1234 A1235:E1235 A1236:E1236 A1237:E1239 A1240:E1242 A1243:E1243 A1244:E1245 A1246:E1250 A1251:E1269 A1270:E1276 A1277:E1277 A1278:E1278 A1279:E1280 A1281:E1281 A1282:E1282 A1283:E1283 A1284:E1285 A1286:E1292 A1293:E1294 A1295:E1295" numberStoredAsText="1"/>
+    <ignoredError sqref="A47:C57 A58:C58 A59:C64 A65:C75 A76:C80 A81:C84 A85:C89 A90:C90 A91:C92 A93:C97 A98:C99 A100:C104 A105:C106 A107:C117 A118:C124 A125:C126 A127:C129 A130:C131 A132:C132 A133:C138 A139:C139 A140:C140 A141:C141 A142:C144 A145:C157 A158:C158 A159:C159 A160:C162 A163:C165 A166:C167 A168:C168 A169:C176 A177:C179 A180:C191 A192:C197 A198:C202 A203:C204 A205:C205 A206:C206 A207:C211 A371:E470 A569:E576 A579:E580 A578:D578 A582:E641 A581:E581 A577:E577 A642:E643 A644:E645 A646:E658 A659:E693 A694:E746 A747:E756 A757:E757 A758:E766 A768:E786 A767:E767 A787:E788 A789:E789 A790:E790 A791:E792 A793:E795 A796:E799 A800:E843 A844:E854 A855:E866 A867:E868 A869:E895 A897:E900 A896:D896 A901:E935 A936:E942 A943:E945 A946:E954 A955:E974 A976:E977 A975:D975 A978:E980 A981:E986 A987:E996 A997:E1000 A1001:E1001 A1002:E1052 A1054:E1071 A1053:D1053 A1072:E1092 A1093:E1094 A1095:E1108 A1109:E1109 A1110:E1112 A1113:E1125 A1126:E1128 A1129:E1130 A1131:E1132 A1133:E1136 A1137:E1141 A1142:E1144 A1145:E1146 A1147:E1155 A1156:E1168 A1169:E1171 A1172:E1193 A1194:E1196 A1197:E1198 A1199:E1200 A1201:E1206 A1207:E1209 A1210:E1212 A1213:E1214 A1215:E1216 A1217:E1220 A1221:E1230 A1231:E1234 A1235:E1235 A1236:E1236 A1237:E1239 A1240:E1242 A1243:E1243 A1244:E1245 A1246:E1250 A1251:E1269 A1270:E1276 A1277:E1277 A1278:E1278 A1279:E1280 A1281:E1281 A1282:E1282 A1283:E1283 A1284:E1285 A1286:E1292 A1293:E1294 A1295:E1295 A1297:E1301 A1296:D1296 A1302:E1308 A1309:E1320 A1321:E1327 A1328:E1333 A1334:E1335 A1336:E1336 A1337:E1343 A1344:E1346 A1347:E1347 A1348:E1348 A1349:E1349 A1350:E1351 A1352:E1352 A1353:E1356 A1357:E1357 A1358:E1358 A1359:E1359 A1360:E1362 A1363:E1364 A1365:E1365" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add jupyter notebook files for running google colab
</commit_message>
<xml_diff>
--- a/data-set/final-data-set.xlsx
+++ b/data-set/final-data-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Level 4\Software Engineering Research Project - SENG 44696\GitRepo\sinhalese_language_racism_detection\data-set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4D73C7-7702-413E-B61E-3A846E9D526A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5874A522-FA79-419A-BC5E-3F7015226817}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16911,9 +16911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1422" workbookViewId="0">
-      <selection activeCell="E1388" sqref="E1388"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>